<commit_message>
comparer checks threshold values now
</commit_message>
<xml_diff>
--- a/ROI_leagues.xlsx
+++ b/ROI_leagues.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA32"/>
+  <dimension ref="A1:AB32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,6 +570,11 @@
           <t>HT1.5UP</t>
         </is>
       </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Games</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -578,76 +583,79 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-72.95588235294117</v>
+        <v>-15.38</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>29.91666666666666</v>
+        <v>71.58</v>
       </c>
       <c r="D2" t="n">
-        <v>-165.3846153846154</v>
+        <v>-75</v>
       </c>
       <c r="E2" t="n">
-        <v>-34.93055555555556</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-23</v>
+        <v>-7.93</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>-40.35294117647059</v>
+        <v>-10.33</v>
       </c>
       <c r="H2" t="n">
-        <v>-48.92105263157895</v>
+        <v>-10.06</v>
       </c>
       <c r="I2" t="n">
-        <v>-56.23529411764706</v>
+        <v>-3.29</v>
       </c>
       <c r="J2" t="n">
-        <v>-123.0769230769231</v>
+        <v>-46.15</v>
       </c>
       <c r="K2" t="n">
-        <v>-33.10000000000001</v>
+        <v>-2.41</v>
       </c>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="n">
-        <v>-10.43010752688172</v>
+      <c r="M2" s="2" t="n">
+        <v>1.81</v>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
-        <v>-8.956989247311812</v>
+        <v>-2.32</v>
       </c>
       <c r="P2" t="n">
-        <v>-127.0769230769231</v>
+        <v>-53.71</v>
       </c>
       <c r="Q2" t="n">
-        <v>-65.90000000000001</v>
+        <v>-19.41</v>
       </c>
       <c r="R2" t="n">
-        <v>-121.7857142857143</v>
-      </c>
-      <c r="S2" t="n">
-        <v>-10.71428571428573</v>
+        <v>-43.21</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>26.46</v>
       </c>
       <c r="T2" t="n">
-        <v>-200</v>
-      </c>
-      <c r="U2" t="n">
-        <v>-16.01639344262296</v>
+        <v>-100</v>
+      </c>
+      <c r="U2" s="2" t="n">
+        <v>0.33</v>
       </c>
       <c r="V2" t="inlineStr"/>
-      <c r="W2" t="n">
-        <v>-13.15625</v>
+      <c r="W2" s="2" t="n">
+        <v>5.59</v>
       </c>
       <c r="X2" t="n">
-        <v>-45.81578947368422</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>-8.823529411764707</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>-12.5</v>
+        <v>-5.62</v>
+      </c>
+      <c r="Y2" s="2" t="n">
+        <v>32.35</v>
+      </c>
+      <c r="Z2" s="2" t="n">
+        <v>37.5</v>
       </c>
       <c r="AA2" t="n">
-        <v>-39.8901098901099</v>
+        <v>-11.88</v>
+      </c>
+      <c r="AB2" s="2" t="n">
+        <v>95</v>
       </c>
     </row>
     <row r="3">
@@ -657,80 +665,83 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-108.7307692307692</v>
+        <v>-42.39</v>
       </c>
       <c r="C3" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="D3" t="n">
-        <v>-63.57142857142858</v>
+        <v>-6.43</v>
       </c>
       <c r="E3" t="n">
-        <v>-41.45</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-4.857142857142867</v>
+        <v>-14.5</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>9.43</v>
       </c>
       <c r="G3" t="n">
-        <v>-130.6666666666667</v>
+        <v>-64</v>
       </c>
       <c r="H3" t="n">
-        <v>-34.33333333333334</v>
+        <v>-7.89</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>300</v>
       </c>
-      <c r="J3" t="n">
-        <v>-40.6</v>
+      <c r="J3" s="2" t="n">
+        <v>5</v>
       </c>
       <c r="K3" t="n">
-        <v>-77.70588235294117</v>
+        <v>-18.88</v>
       </c>
       <c r="L3" t="n">
-        <v>-112.2222222222222</v>
-      </c>
-      <c r="M3" t="n">
-        <v>-17.10714285714285</v>
+        <v>-16</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>9.34</v>
       </c>
       <c r="N3" t="n">
-        <v>-200</v>
-      </c>
-      <c r="O3" t="n">
-        <v>-7.342857142857144</v>
+        <v>-100</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>1.65</v>
       </c>
       <c r="P3" t="n">
-        <v>-79.68181818181819</v>
+        <v>-24.42</v>
       </c>
       <c r="Q3" t="n">
-        <v>-97.00000000000001</v>
+        <v>-30.33</v>
       </c>
       <c r="R3" t="n">
-        <v>-142.6</v>
-      </c>
-      <c r="S3" t="n">
-        <v>-27.4782608695652</v>
+        <v>-52.92</v>
+      </c>
+      <c r="S3" s="2" t="n">
+        <v>20.35</v>
       </c>
       <c r="T3" s="2" t="n">
-        <v>39.99999999999999</v>
-      </c>
-      <c r="U3" t="n">
-        <v>-12.95238095238095</v>
+        <v>90</v>
+      </c>
+      <c r="U3" s="2" t="n">
+        <v>6.61</v>
       </c>
       <c r="V3" t="inlineStr"/>
-      <c r="W3" t="n">
-        <v>-17.24999999999999</v>
+      <c r="W3" s="2" t="n">
+        <v>7.75</v>
       </c>
       <c r="X3" t="n">
-        <v>-45.37037037037037</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>-38.49999999999999</v>
+        <v>-13.62</v>
+      </c>
+      <c r="Y3" s="2" t="n">
+        <v>21.5</v>
       </c>
       <c r="Z3" t="n">
-        <v>-88.41666666666667</v>
+        <v>-27.77</v>
       </c>
       <c r="AA3" s="2" t="n">
-        <v>7.040000000000006</v>
+        <v>18.31</v>
+      </c>
+      <c r="AB3" s="2" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="4">
@@ -740,82 +751,85 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-58.15151515151516</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-65.71428571428571</v>
+        <v>-9.17</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>5.71</v>
       </c>
       <c r="D4" t="n">
-        <v>-120.3125</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-14.35483870967743</v>
+        <v>-45.31</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>5.59</v>
       </c>
       <c r="F4" t="n">
-        <v>-34.90909090909091</v>
+        <v>-7.64</v>
       </c>
       <c r="G4" t="n">
-        <v>-68.92857142857142</v>
-      </c>
-      <c r="H4" t="n">
-        <v>-15.6530612244898</v>
+        <v>-26.07</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>1.67</v>
       </c>
       <c r="I4" t="n">
-        <v>-139.2857142857143</v>
+        <v>-53.57</v>
       </c>
       <c r="J4" t="n">
-        <v>-61.10714285714286</v>
+        <v>-12.71</v>
       </c>
       <c r="K4" t="n">
-        <v>-64.39285714285715</v>
+        <v>-10.82</v>
       </c>
       <c r="L4" t="n">
-        <v>-130.1538461538462</v>
-      </c>
-      <c r="M4" t="n">
-        <v>-10.97674418604651</v>
+        <v>-40.5</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>11.47</v>
       </c>
       <c r="N4" t="n">
-        <v>-200</v>
-      </c>
-      <c r="O4" t="n">
-        <v>-8.037037037037043</v>
+        <v>-100</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>1.77</v>
       </c>
       <c r="P4" t="n">
-        <v>-89.125</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>-40.28124999999999</v>
-      </c>
-      <c r="R4" t="n">
-        <v>-27.05882352941178</v>
+        <v>-33.56</v>
+      </c>
+      <c r="Q4" s="2" t="n">
+        <v>6.21</v>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>11</v>
       </c>
       <c r="S4" t="n">
-        <v>-73.66666666666667</v>
-      </c>
-      <c r="T4" t="n">
-        <v>-53.77777777777778</v>
+        <v>-11.76</v>
+      </c>
+      <c r="T4" s="2" t="n">
+        <v>7.33</v>
       </c>
       <c r="U4" t="n">
-        <v>-15.08</v>
+        <v>-2</v>
       </c>
       <c r="V4" t="n">
-        <v>-150</v>
+        <v>-70</v>
       </c>
       <c r="W4" t="n">
-        <v>-30.96153846153845</v>
+        <v>-4.04</v>
       </c>
       <c r="X4" t="n">
-        <v>-35.2</v>
+        <v>-6.85</v>
       </c>
       <c r="Y4" t="n">
-        <v>-94.27272727272728</v>
+        <v>-21.55</v>
       </c>
       <c r="Z4" t="n">
-        <v>-184</v>
+        <v>-79.05</v>
       </c>
       <c r="AA4" t="n">
-        <v>-42.69444444444444</v>
+        <v>-3.61</v>
+      </c>
+      <c r="AB4" s="2" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="5">
@@ -825,74 +839,77 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-60.50000000000001</v>
+        <v>-14.23</v>
       </c>
       <c r="C5" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="D5" t="n">
-        <v>-85.45454545454547</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-13.66666666666667</v>
+        <v>-22.92</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.84</v>
       </c>
       <c r="F5" t="n">
-        <v>-28.26315789473683</v>
-      </c>
-      <c r="G5" t="n">
-        <v>-31.64285714285714</v>
+        <v>-1.95</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>2.19</v>
       </c>
       <c r="H5" t="n">
-        <v>-45.9264705882353</v>
+        <v>-9.74</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>150</v>
       </c>
       <c r="J5" t="n">
-        <v>-80.05555555555556</v>
+        <v>-23.21</v>
       </c>
       <c r="K5" t="n">
-        <v>-61.19607843137255</v>
+        <v>-12.37</v>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
-        <v>-30.08695652173913</v>
+        <v>-5.15</v>
       </c>
       <c r="N5" t="inlineStr"/>
-      <c r="O5" t="n">
-        <v>-6.695652173913029</v>
-      </c>
-      <c r="P5" t="n">
-        <v>-44.56521739130434</v>
+      <c r="O5" s="2" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>3.26</v>
       </c>
       <c r="Q5" t="n">
-        <v>-58.32608695652174</v>
-      </c>
-      <c r="R5" t="n">
-        <v>-52.2</v>
-      </c>
-      <c r="S5" t="n">
-        <v>-11.72881355932203</v>
+        <v>-14.42</v>
+      </c>
+      <c r="R5" s="2" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="S5" s="2" t="n">
+        <v>22.35</v>
       </c>
       <c r="T5" t="inlineStr"/>
-      <c r="U5" t="n">
-        <v>-7.884615384615373</v>
+      <c r="U5" s="2" t="n">
+        <v>0.05</v>
       </c>
       <c r="V5" t="inlineStr"/>
       <c r="W5" s="2" t="n">
-        <v>4.176470588235299</v>
+        <v>15.28</v>
       </c>
       <c r="X5" t="n">
-        <v>-45.12307692307693</v>
+        <v>-7.3</v>
       </c>
       <c r="Y5" s="2" t="n">
-        <v>56.49999999999999</v>
+        <v>81.5</v>
       </c>
       <c r="Z5" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="AA5" t="n">
-        <v>-41.39393939393939</v>
+        <v>-8.789999999999999</v>
+      </c>
+      <c r="AB5" s="2" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="6">
@@ -902,80 +919,83 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-54.86666666666665</v>
+        <v>-1.53</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="D6" t="n">
-        <v>-149.1176470588235</v>
+        <v>-68.61</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>9.583333333333321</v>
+        <v>17.92</v>
       </c>
       <c r="F6" t="n">
-        <v>-64.5</v>
+        <v>-24.5</v>
       </c>
       <c r="G6" t="n">
-        <v>-45.33333333333333</v>
-      </c>
-      <c r="H6" t="n">
-        <v>-6.294117647058825</v>
+        <v>-18.77</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>2.46</v>
       </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="n">
-        <v>-43.44</v>
+        <v>-7.15</v>
       </c>
       <c r="K6" t="n">
-        <v>-68.55555555555556</v>
-      </c>
-      <c r="L6" t="n">
-        <v>-55.11111111111111</v>
+        <v>-13</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>0.44</v>
       </c>
       <c r="M6" t="n">
-        <v>-74.44</v>
-      </c>
-      <c r="N6" t="n">
-        <v>-33.33333333333333</v>
+        <v>-24.04</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>33.33</v>
       </c>
       <c r="O6" t="n">
-        <v>-32.29032258064517</v>
-      </c>
-      <c r="P6" t="n">
-        <v>-5.333333333333323</v>
+        <v>-9</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>14.88</v>
       </c>
       <c r="Q6" t="n">
-        <v>-75.09999999999999</v>
+        <v>-15.1</v>
       </c>
       <c r="R6" s="2" t="n">
-        <v>48.84615384615383</v>
+        <v>73.93000000000001</v>
       </c>
       <c r="S6" t="n">
-        <v>-59.28571428571428</v>
+        <v>-2.14</v>
       </c>
       <c r="T6" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="U6" s="2" t="n">
-        <v>11.57894736842105</v>
+        <v>22.11</v>
       </c>
       <c r="V6" t="n">
-        <v>-32.33333333333333</v>
+        <v>-24.25</v>
       </c>
       <c r="W6" t="n">
-        <v>-25.75</v>
-      </c>
-      <c r="X6" t="n">
-        <v>-5.625000000000002</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>-13.1875</v>
+        <v>-0.75</v>
+      </c>
+      <c r="X6" s="2" t="n">
+        <v>6.67</v>
+      </c>
+      <c r="Y6" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z6" s="2" t="n">
+        <v>22.88</v>
       </c>
       <c r="AA6" t="n">
-        <v>-48.94444444444444</v>
+        <v>-10.06</v>
+      </c>
+      <c r="AB6" s="2" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="7">
@@ -985,82 +1005,85 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-23.47058823529413</v>
+        <v>-5.21</v>
       </c>
       <c r="C7" t="n">
-        <v>-106</v>
+        <v>-26</v>
       </c>
       <c r="D7" t="n">
-        <v>-131</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-5.39130434782608</v>
+        <v>-34.95</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>3.6</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>25.33333333333333</v>
+        <v>25.33</v>
       </c>
       <c r="G7" t="n">
-        <v>-67.31578947368422</v>
+        <v>-11.91</v>
       </c>
       <c r="H7" t="n">
-        <v>-31.29545454545455</v>
+        <v>-8.43</v>
       </c>
       <c r="I7" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="J7" t="n">
-        <v>-61.54166666666666</v>
+        <v>-12.14</v>
       </c>
       <c r="K7" t="n">
-        <v>-76.33333333333334</v>
+        <v>-18.32</v>
       </c>
       <c r="L7" t="n">
-        <v>-200</v>
-      </c>
-      <c r="M7" t="n">
-        <v>-29.8095238095238</v>
+        <v>-100</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>0.11</v>
       </c>
       <c r="N7" t="n">
-        <v>-200</v>
-      </c>
-      <c r="O7" t="n">
-        <v>-18.61363636363637</v>
-      </c>
-      <c r="P7" t="n">
-        <v>-24.55999999999999</v>
+        <v>-100</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>3.55</v>
       </c>
       <c r="Q7" t="n">
-        <v>-72.45</v>
+        <v>-16.62</v>
       </c>
       <c r="R7" t="n">
-        <v>-126.1428571428572</v>
-      </c>
-      <c r="S7" t="n">
-        <v>-25.93333333333334</v>
+        <v>-54.3</v>
+      </c>
+      <c r="S7" s="2" t="n">
+        <v>13.19</v>
       </c>
       <c r="T7" s="2" t="n">
-        <v>45.11111111111109</v>
+        <v>72.45</v>
       </c>
       <c r="U7" t="n">
-        <v>-33.125</v>
-      </c>
-      <c r="V7" t="n">
-        <v>-11.74999999999999</v>
+        <v>-15.19</v>
+      </c>
+      <c r="V7" s="2" t="n">
+        <v>18.6</v>
       </c>
       <c r="W7" t="n">
-        <v>-45.76470588235293</v>
+        <v>-6.89</v>
       </c>
       <c r="X7" t="n">
-        <v>-34.19512195121952</v>
+        <v>-7.33</v>
       </c>
       <c r="Y7" t="n">
-        <v>-100</v>
+        <v>-40</v>
       </c>
       <c r="Z7" t="n">
-        <v>-69.58333333333333</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>-23.81818181818183</v>
+        <v>-10.14</v>
+      </c>
+      <c r="AA7" s="2" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="AB7" s="2" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="8">
@@ -1070,80 +1093,83 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-51.6</v>
+        <v>-8.789999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>-91.875</v>
+        <v>-2.65</v>
       </c>
       <c r="D8" t="n">
-        <v>-141.36</v>
-      </c>
-      <c r="E8" t="n">
-        <v>-11.77358490566038</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-7.833333333333329</v>
+        <v>-52.54</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>5.84</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>8.83</v>
       </c>
       <c r="G8" t="n">
-        <v>-63.62962962962963</v>
+        <v>-10.68</v>
       </c>
       <c r="H8" t="n">
-        <v>-49.72602739726028</v>
-      </c>
-      <c r="I8" t="n">
-        <v>-10.53846153846155</v>
+        <v>-12.5</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>44.2</v>
       </c>
       <c r="J8" t="n">
-        <v>-75.76666666666667</v>
-      </c>
-      <c r="K8" t="n">
-        <v>-33.23214285714287</v>
+        <v>-18.94</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>4.23</v>
       </c>
       <c r="L8" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="M8" t="n">
-        <v>-23.02702702702702</v>
+        <v>-2.86</v>
       </c>
       <c r="N8" t="n">
-        <v>-200</v>
-      </c>
-      <c r="O8" t="n">
-        <v>-7.600000000000026</v>
+        <v>-100</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>1.29</v>
       </c>
       <c r="P8" t="n">
-        <v>-71.96428571428571</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>-34.67241379310346</v>
-      </c>
-      <c r="R8" t="n">
-        <v>-29.71428571428572</v>
+        <v>-12.6</v>
+      </c>
+      <c r="Q8" s="2" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="R8" s="2" t="n">
+        <v>19.59</v>
       </c>
       <c r="S8" t="n">
-        <v>-75.54166666666666</v>
+        <v>-20.67</v>
       </c>
       <c r="T8" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="U8" t="n">
-        <v>-33.08928571428572</v>
+        <v>-10.27</v>
       </c>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="n">
-        <v>-75.53333333333333</v>
+        <v>-23.24</v>
       </c>
       <c r="X8" t="n">
-        <v>-48.5945945945946</v>
+        <v>-8.9</v>
       </c>
       <c r="Y8" t="n">
-        <v>-49</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>-70.77777777777779</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>-19.76623376623376</v>
+        <v>-6.29</v>
+      </c>
+      <c r="Z8" s="2" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="AA8" s="2" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="AB8" s="2" t="n">
+        <v>93</v>
       </c>
     </row>
     <row r="9">
@@ -1152,83 +1178,86 @@
           <t>England3</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>-6.192307692307677</v>
+      <c r="B9" s="2" t="n">
+        <v>22.78</v>
       </c>
       <c r="C9" t="n">
-        <v>-104.4444444444445</v>
+        <v>-2</v>
       </c>
       <c r="D9" t="n">
-        <v>-84.46875</v>
+        <v>-21.37</v>
       </c>
       <c r="E9" t="n">
-        <v>-37.99999999999999</v>
-      </c>
-      <c r="F9" t="n">
-        <v>-24.56666666666668</v>
+        <v>-10.89</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>1.64</v>
       </c>
       <c r="G9" t="n">
-        <v>-42.51724137931034</v>
+        <v>-12.16</v>
       </c>
       <c r="H9" t="n">
-        <v>-21.48750000000001</v>
+        <v>-3.47</v>
       </c>
       <c r="I9" t="n">
-        <v>-79.76923076923079</v>
-      </c>
-      <c r="J9" t="n">
-        <v>-32.45454545454546</v>
-      </c>
-      <c r="K9" t="n">
-        <v>-25.71428571428572</v>
+        <v>-4.93</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>11.75</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>13.93</v>
       </c>
       <c r="L9" t="n">
-        <v>-84.46666666666667</v>
+        <v>-27.47</v>
       </c>
       <c r="M9" t="n">
-        <v>-35.47435897435899</v>
+        <v>-5.77</v>
       </c>
       <c r="N9" t="n">
-        <v>-140.625</v>
+        <v>-58.33</v>
       </c>
       <c r="O9" t="n">
-        <v>-27.36470588235295</v>
+        <v>-9.039999999999999</v>
       </c>
       <c r="P9" t="n">
-        <v>-48.2391304347826</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>-50.40425531914894</v>
+        <v>-0.45</v>
+      </c>
+      <c r="Q9" s="2" t="n">
+        <v>3.54</v>
       </c>
       <c r="R9" t="n">
-        <v>-51.66666666666666</v>
+        <v>-6.55</v>
       </c>
       <c r="S9" t="n">
-        <v>-104.4565217391304</v>
-      </c>
-      <c r="T9" t="n">
-        <v>-46.78260869565218</v>
+        <v>-32.08</v>
+      </c>
+      <c r="T9" s="2" t="n">
+        <v>9.33</v>
       </c>
       <c r="U9" t="n">
-        <v>-37.92857142857144</v>
-      </c>
-      <c r="V9" t="n">
-        <v>-31.16666666666665</v>
+        <v>-11.04</v>
+      </c>
+      <c r="V9" s="2" t="n">
+        <v>9</v>
       </c>
       <c r="W9" t="n">
-        <v>-35.02222222222223</v>
-      </c>
-      <c r="X9" t="n">
-        <v>-23.03896103896105</v>
+        <v>-8.51</v>
+      </c>
+      <c r="X9" s="2" t="n">
+        <v>1.2</v>
       </c>
       <c r="Y9" t="n">
-        <v>-109.3125</v>
-      </c>
-      <c r="Z9" t="n">
-        <v>-48.59999999999999</v>
+        <v>-32.84</v>
+      </c>
+      <c r="Z9" s="2" t="n">
+        <v>7.59</v>
       </c>
       <c r="AA9" t="n">
-        <v>-31.75000000000001</v>
+        <v>-5.49</v>
+      </c>
+      <c r="AB9" s="2" t="n">
+        <v>103</v>
       </c>
     </row>
     <row r="10">
@@ -1238,82 +1267,85 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-109.5238095238095</v>
+        <v>-40.1</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>85</v>
+        <v>118.33</v>
       </c>
       <c r="D10" t="n">
-        <v>-69.48717948717949</v>
+        <v>-7.75</v>
       </c>
       <c r="E10" t="n">
-        <v>-66.36363636363637</v>
+        <v>-22.5</v>
       </c>
       <c r="F10" t="n">
-        <v>-47.01851851851853</v>
+        <v>-11.3</v>
       </c>
       <c r="G10" t="n">
-        <v>-45.75</v>
+        <v>-4.89</v>
       </c>
       <c r="H10" t="n">
-        <v>-42.43478260869566</v>
+        <v>-18.46</v>
       </c>
       <c r="I10" t="n">
-        <v>-77.8</v>
+        <v>-10.44</v>
       </c>
       <c r="J10" t="n">
-        <v>-66.11764705882352</v>
-      </c>
-      <c r="K10" t="n">
-        <v>-38.94</v>
-      </c>
-      <c r="L10" t="n">
-        <v>-57.08333333333333</v>
-      </c>
-      <c r="M10" t="n">
-        <v>-12.25000000000001</v>
+        <v>-22.32</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>4.09</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>9.58</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>8.109999999999999</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="O10" t="n">
-        <v>-0.8148148148148281</v>
+        <v>116.67</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>4.66</v>
       </c>
       <c r="P10" t="n">
-        <v>-81.5</v>
+        <v>-30.58</v>
       </c>
       <c r="Q10" t="n">
-        <v>-74.78571428571429</v>
+        <v>-15.2</v>
       </c>
       <c r="R10" t="n">
-        <v>-90.51351351351352</v>
+        <v>-30.46</v>
       </c>
       <c r="S10" t="n">
-        <v>-83</v>
+        <v>-9.869999999999999</v>
       </c>
       <c r="T10" t="n">
-        <v>-131.6666666666667</v>
+        <v>-52.31</v>
       </c>
       <c r="U10" t="n">
-        <v>-56.83018867924527</v>
+        <v>-18.81</v>
       </c>
       <c r="V10" t="n">
-        <v>-90.28571428571429</v>
+        <v>-33.14</v>
       </c>
       <c r="W10" t="n">
-        <v>-66</v>
+        <v>-19.05</v>
       </c>
       <c r="X10" t="n">
-        <v>-38.93055555555556</v>
+        <v>-14.59</v>
       </c>
       <c r="Y10" t="n">
-        <v>-108.25</v>
+        <v>-33.25</v>
       </c>
       <c r="Z10" t="n">
-        <v>-87.5</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>-30.52941176470589</v>
+        <v>-23.53</v>
+      </c>
+      <c r="AA10" s="2" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="AB10" s="2" t="n">
+        <v>92</v>
       </c>
     </row>
     <row r="11">
@@ -1323,82 +1355,85 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-67.73469387755101</v>
+        <v>-17.53</v>
       </c>
       <c r="C11" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="D11" t="n">
-        <v>-76.58333333333334</v>
+        <v>-19.35</v>
       </c>
       <c r="E11" t="n">
-        <v>-20.56756756756756</v>
+        <v>-2.41</v>
       </c>
       <c r="F11" t="n">
-        <v>-32.96153846153847</v>
+        <v>-3.54</v>
       </c>
       <c r="G11" t="n">
-        <v>-51.4</v>
-      </c>
-      <c r="H11" t="n">
-        <v>-23.22222222222222</v>
+        <v>-19.11</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0.1</v>
       </c>
       <c r="I11" t="n">
-        <v>-139.2857142857143</v>
-      </c>
-      <c r="J11" t="n">
-        <v>-41.82222222222222</v>
+        <v>-59.38</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>4.26</v>
       </c>
       <c r="K11" t="n">
-        <v>-85.95348837209302</v>
+        <v>-27.62</v>
       </c>
       <c r="L11" t="n">
-        <v>-128.7</v>
+        <v>-48.7</v>
       </c>
       <c r="M11" t="n">
-        <v>-45.7051282051282</v>
+        <v>-13.83</v>
       </c>
       <c r="N11" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="O11" t="n">
-        <v>-17.73563218390805</v>
+        <v>-3.68</v>
       </c>
       <c r="P11" t="n">
-        <v>-43.39024390243902</v>
+        <v>-1.74</v>
       </c>
       <c r="Q11" t="n">
-        <v>-92.19148936170212</v>
+        <v>-30.24</v>
       </c>
       <c r="R11" t="n">
-        <v>-82.42424242424242</v>
+        <v>-3.57</v>
       </c>
       <c r="S11" t="n">
-        <v>-77.55882352941175</v>
-      </c>
-      <c r="T11" t="n">
-        <v>-56.19047619047619</v>
+        <v>-22.62</v>
+      </c>
+      <c r="T11" s="2" t="n">
+        <v>20.43</v>
       </c>
       <c r="U11" t="n">
-        <v>-38.34615384615384</v>
+        <v>-10.86</v>
       </c>
       <c r="V11" t="n">
-        <v>-114.6666666666667</v>
+        <v>-33</v>
       </c>
       <c r="W11" t="n">
-        <v>-63.46666666666666</v>
-      </c>
-      <c r="X11" t="n">
-        <v>-28.81818181818182</v>
+        <v>-18.88</v>
+      </c>
+      <c r="X11" s="2" t="n">
+        <v>2.02</v>
       </c>
       <c r="Y11" t="n">
-        <v>-130.6363636363636</v>
+        <v>-53.08</v>
       </c>
       <c r="Z11" t="n">
-        <v>-153.5714285714286</v>
+        <v>-39</v>
       </c>
       <c r="AA11" t="n">
-        <v>-43.71604938271606</v>
+        <v>-9.75</v>
+      </c>
+      <c r="AB11" s="2" t="n">
+        <v>97</v>
       </c>
     </row>
     <row r="12">
@@ -1408,80 +1443,83 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-63.95454545454545</v>
+        <v>-12.58</v>
       </c>
       <c r="C12" t="n">
-        <v>-114</v>
+        <v>-34</v>
       </c>
       <c r="D12" t="n">
-        <v>-57.47058823529412</v>
+        <v>-4.53</v>
       </c>
       <c r="E12" t="n">
-        <v>-28.80952380952381</v>
+        <v>-8.35</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>27.66666666666667</v>
+        <v>2.4</v>
       </c>
       <c r="G12" t="n">
-        <v>-60.15000000000001</v>
+        <v>-20.15</v>
       </c>
       <c r="H12" t="n">
-        <v>-19.02439024390245</v>
+        <v>-0.4</v>
       </c>
       <c r="I12" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="J12" t="n">
-        <v>-52.95833333333333</v>
+        <v>-14.27</v>
       </c>
       <c r="K12" t="n">
-        <v>-65.64999999999999</v>
+        <v>-18.77</v>
       </c>
       <c r="L12" t="n">
-        <v>-96.8125</v>
+        <v>-28.06</v>
       </c>
       <c r="M12" t="n">
-        <v>-38.82142857142858</v>
+        <v>-9.06</v>
       </c>
       <c r="N12" t="n">
-        <v>-123.8571428571429</v>
-      </c>
-      <c r="O12" t="n">
-        <v>-2.621621621621618</v>
+        <v>-38.14</v>
+      </c>
+      <c r="O12" s="2" t="n">
+        <v>3.88</v>
       </c>
       <c r="P12" t="n">
-        <v>-89.04166666666666</v>
+        <v>-30.27</v>
       </c>
       <c r="Q12" t="n">
-        <v>-96.85000000000001</v>
+        <v>-38.05</v>
       </c>
       <c r="R12" t="n">
-        <v>-79.76470588235294</v>
+        <v>-8.67</v>
       </c>
       <c r="S12" t="n">
-        <v>-136</v>
+        <v>-47.94</v>
       </c>
       <c r="T12" t="n">
-        <v>-109.5833333333333</v>
+        <v>-39.62</v>
       </c>
       <c r="U12" t="n">
-        <v>-57.96428571428572</v>
+        <v>-22.03</v>
       </c>
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="n">
-        <v>-74.3125</v>
-      </c>
-      <c r="X12" t="n">
-        <v>-16.14285714285715</v>
+        <v>-26.41</v>
+      </c>
+      <c r="X12" s="2" t="n">
+        <v>1.78</v>
       </c>
       <c r="Y12" t="n">
-        <v>-200</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>-56.52941176470588</v>
+        <v>-100</v>
+      </c>
+      <c r="Z12" s="2" t="n">
+        <v>2.29</v>
       </c>
       <c r="AA12" t="n">
-        <v>-43.81481481481482</v>
+        <v>-4.39</v>
+      </c>
+      <c r="AB12" s="2" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="13">
@@ -1490,83 +1528,86 @@
           <t>France2</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>-23.14634146341464</v>
+      <c r="B13" s="2" t="n">
+        <v>19.23</v>
       </c>
       <c r="C13" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="D13" t="n">
-        <v>-136.6071428571429</v>
+        <v>-57.19</v>
       </c>
       <c r="E13" t="n">
-        <v>-21.05263157894738</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>-24.07142857142857</v>
+        <v>-7.31</v>
       </c>
       <c r="G13" t="n">
-        <v>-154.7</v>
+        <v>-65.91</v>
       </c>
       <c r="H13" t="n">
-        <v>-36.23333333333335</v>
-      </c>
-      <c r="I13" t="n">
-        <v>-85.18181818181819</v>
+        <v>-6.61</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>5.25</v>
       </c>
       <c r="J13" t="n">
-        <v>-73.45161290322581</v>
+        <v>-14.3</v>
       </c>
       <c r="K13" t="n">
-        <v>-79.14999999999999</v>
-      </c>
-      <c r="L13" t="n">
-        <v>-32.85714285714285</v>
+        <v>-21.16</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>31.43</v>
       </c>
       <c r="M13" t="n">
-        <v>-25.94736842105265</v>
+        <v>-1.94</v>
       </c>
       <c r="N13" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="O13" t="n">
-        <v>-13.38805970149254</v>
+        <v>-3.32</v>
       </c>
       <c r="P13" t="n">
-        <v>-106.5238095238095</v>
+        <v>-42.59</v>
       </c>
       <c r="Q13" t="n">
-        <v>-53.74</v>
-      </c>
-      <c r="R13" t="n">
-        <v>-33.17391304347826</v>
+        <v>-2.8</v>
+      </c>
+      <c r="R13" s="2" t="n">
+        <v>14.7</v>
       </c>
       <c r="S13" t="n">
-        <v>-97.00000000000001</v>
+        <v>-24.92</v>
       </c>
       <c r="T13" t="n">
-        <v>-155.0833333333333</v>
-      </c>
-      <c r="U13" t="n">
-        <v>-18.3448275862069</v>
+        <v>-59.5</v>
+      </c>
+      <c r="U13" s="2" t="n">
+        <v>4.5</v>
       </c>
       <c r="V13" t="n">
-        <v>-49.91999999999999</v>
+        <v>-3.12</v>
       </c>
       <c r="W13" t="n">
-        <v>-61.1764705882353</v>
-      </c>
-      <c r="X13" t="n">
-        <v>-27.82758620689657</v>
+        <v>-13.15</v>
+      </c>
+      <c r="X13" s="2" t="n">
+        <v>1.09</v>
       </c>
       <c r="Y13" t="n">
-        <v>-116.3076923076923</v>
+        <v>-24.93</v>
       </c>
       <c r="Z13" t="n">
-        <v>-77.64705882352941</v>
+        <v>-7.06</v>
       </c>
       <c r="AA13" t="n">
-        <v>-39.07407407407408</v>
+        <v>-9.41</v>
+      </c>
+      <c r="AB13" s="2" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="14">
@@ -1576,80 +1617,83 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-76</v>
+        <v>-13.57</v>
       </c>
       <c r="C14" t="n">
-        <v>-128.75</v>
+        <v>-49.62</v>
       </c>
       <c r="D14" t="n">
-        <v>-60</v>
-      </c>
-      <c r="E14" t="n">
-        <v>-12.31818181818182</v>
+        <v>-17.65</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>2.31</v>
       </c>
       <c r="F14" t="n">
-        <v>-87.25</v>
+        <v>-37.25</v>
       </c>
       <c r="G14" t="n">
-        <v>-39.85</v>
+        <v>-21.61</v>
       </c>
       <c r="H14" t="n">
-        <v>-35.23255813953487</v>
+        <v>-13.02</v>
       </c>
       <c r="I14" t="n">
-        <v>-75</v>
+        <v>-8.33</v>
       </c>
       <c r="J14" t="n">
-        <v>-40.41176470588233</v>
-      </c>
-      <c r="K14" t="n">
-        <v>-11.99999999999999</v>
+        <v>-6.46</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>23.5</v>
       </c>
       <c r="L14" t="n">
-        <v>-52.16666666666667</v>
+        <v>-16.14</v>
       </c>
       <c r="M14" t="n">
-        <v>-36.92857142857143</v>
+        <v>-9.66</v>
       </c>
       <c r="N14" t="n">
-        <v>-160</v>
+        <v>-75.56</v>
       </c>
       <c r="O14" t="n">
-        <v>-29.81578947368422</v>
-      </c>
-      <c r="P14" t="n">
-        <v>-12.45454545454545</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>-9.923076923076916</v>
+        <v>-7.59</v>
+      </c>
+      <c r="P14" s="2" t="n">
+        <v>7.68</v>
+      </c>
+      <c r="Q14" s="2" t="n">
+        <v>27.88</v>
       </c>
       <c r="R14" t="n">
-        <v>-111.1666666666667</v>
+        <v>-44.7</v>
       </c>
       <c r="S14" t="n">
-        <v>-78.03225806451613</v>
-      </c>
-      <c r="T14" t="n">
-        <v>-42.00000000000001</v>
+        <v>-15.12</v>
+      </c>
+      <c r="T14" s="2" t="n">
+        <v>2.44</v>
       </c>
       <c r="U14" t="n">
-        <v>-26.8076923076923</v>
+        <v>-2.03</v>
       </c>
       <c r="V14" t="inlineStr"/>
-      <c r="W14" t="n">
-        <v>-12.85</v>
+      <c r="W14" s="2" t="n">
+        <v>4.7</v>
       </c>
       <c r="X14" t="n">
-        <v>-35.66666666666667</v>
+        <v>-11.8</v>
       </c>
       <c r="Y14" t="n">
-        <v>-133.4615384615385</v>
+        <v>-48.85</v>
       </c>
       <c r="Z14" t="n">
-        <v>-98.66666666666667</v>
+        <v>-32.15</v>
       </c>
       <c r="AA14" t="n">
-        <v>-73.86363636363636</v>
+        <v>-23.35</v>
+      </c>
+      <c r="AB14" s="2" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="15">
@@ -1659,82 +1703,85 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-93.29729729729731</v>
+        <v>-34.79</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="D15" t="n">
-        <v>-92.04545454545455</v>
+        <v>-12.29</v>
       </c>
       <c r="E15" t="n">
-        <v>-30.5625</v>
+        <v>-7.06</v>
       </c>
       <c r="F15" t="n">
-        <v>-56.36363636363636</v>
+        <v>-9.789999999999999</v>
       </c>
       <c r="G15" t="n">
-        <v>-77.25</v>
+        <v>-24.9</v>
       </c>
       <c r="H15" t="n">
-        <v>-26.13114754098361</v>
+        <v>-5.6</v>
       </c>
       <c r="I15" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="J15" t="n">
-        <v>-46.21951219512194</v>
+        <v>-4.96</v>
       </c>
       <c r="K15" t="n">
-        <v>-87.22727272727273</v>
-      </c>
-      <c r="L15" t="n">
-        <v>-59.33333333333333</v>
+        <v>-24.36</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>9.220000000000001</v>
       </c>
       <c r="M15" t="n">
-        <v>-57.71428571428572</v>
+        <v>-14.53</v>
       </c>
       <c r="N15" t="n">
-        <v>-81.25</v>
+        <v>-6.25</v>
       </c>
       <c r="O15" t="n">
-        <v>-16.16949152542373</v>
-      </c>
-      <c r="P15" t="n">
-        <v>-29.52631578947368</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>-33.44</v>
+        <v>-0.89</v>
+      </c>
+      <c r="P15" s="2" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="Q15" s="2" t="n">
+        <v>10.15</v>
       </c>
       <c r="R15" t="n">
-        <v>-64.41666666666667</v>
-      </c>
-      <c r="S15" t="n">
-        <v>-43.82142857142857</v>
+        <v>-5.23</v>
+      </c>
+      <c r="S15" s="2" t="n">
+        <v>21.39</v>
       </c>
       <c r="T15" t="n">
-        <v>-121.5454545454546</v>
+        <v>-49</v>
       </c>
       <c r="U15" t="n">
-        <v>-25.15625</v>
-      </c>
-      <c r="V15" t="n">
-        <v>-11.74999999999999</v>
+        <v>-1.26</v>
+      </c>
+      <c r="V15" s="2" t="n">
+        <v>21.2</v>
       </c>
       <c r="W15" t="n">
-        <v>-49.22222222222221</v>
+        <v>-6.77</v>
       </c>
       <c r="X15" t="n">
-        <v>-25.68627450980393</v>
+        <v>-5.72</v>
       </c>
       <c r="Y15" t="n">
-        <v>-163.3333333333333</v>
-      </c>
-      <c r="Z15" t="n">
-        <v>-18.56249999999999</v>
+        <v>-73.84999999999999</v>
+      </c>
+      <c r="Z15" s="2" t="n">
+        <v>23.78</v>
       </c>
       <c r="AA15" t="n">
-        <v>-48.27659574468085</v>
+        <v>-8.119999999999999</v>
+      </c>
+      <c r="AB15" s="2" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="16">
@@ -1744,82 +1791,85 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-51.4375</v>
-      </c>
-      <c r="C16" t="n">
-        <v>-9.545454545454552</v>
+        <v>-13.12</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>45</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>17.86666666666666</v>
+        <v>54.59</v>
       </c>
       <c r="E16" t="n">
-        <v>-58.44444444444444</v>
+        <v>-29.05</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>35.40000000000001</v>
-      </c>
-      <c r="G16" t="n">
-        <v>-11.05263157894738</v>
+        <v>35</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>11.5</v>
       </c>
       <c r="H16" t="n">
-        <v>-28.22857142857143</v>
+        <v>-3.13</v>
       </c>
       <c r="I16" t="n">
-        <v>-76.71428571428571</v>
+        <v>-5.29</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>21.33333333333334</v>
-      </c>
-      <c r="K16" t="n">
-        <v>-20.76666666666666</v>
+        <v>40.79</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>18.23</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="M16" t="n">
-        <v>-23.94736842105264</v>
+        <v>100</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>1.63</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>800</v>
       </c>
       <c r="O16" t="n">
-        <v>-14.60975609756096</v>
-      </c>
-      <c r="P16" t="n">
-        <v>-27.71428571428571</v>
+        <v>-1.66</v>
+      </c>
+      <c r="P16" s="2" t="n">
+        <v>24.88</v>
       </c>
       <c r="Q16" t="n">
-        <v>-69.78571428571428</v>
+        <v>-12.9</v>
       </c>
       <c r="R16" t="n">
-        <v>-69</v>
-      </c>
-      <c r="S16" t="n">
-        <v>-39.17241379310344</v>
+        <v>-22.88</v>
+      </c>
+      <c r="S16" s="2" t="n">
+        <v>12.3</v>
       </c>
       <c r="T16" t="n">
-        <v>-146.6666666666667</v>
+        <v>-6.71</v>
       </c>
       <c r="U16" t="n">
-        <v>-41.08695652173913</v>
+        <v>-18.54</v>
       </c>
       <c r="V16" s="2" t="n">
-        <v>39.99999999999999</v>
-      </c>
-      <c r="W16" t="n">
-        <v>-19.33333333333334</v>
-      </c>
-      <c r="X16" t="n">
-        <v>-23.34782608695653</v>
+        <v>40</v>
+      </c>
+      <c r="W16" s="2" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="X16" s="2" t="n">
+        <v>7.58</v>
       </c>
       <c r="Y16" t="n">
-        <v>-119.6842105263158</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>-26.11111111111111</v>
+        <v>-40.74</v>
+      </c>
+      <c r="Z16" s="2" t="n">
+        <v>16.5</v>
       </c>
       <c r="AA16" t="n">
-        <v>-47.39393939393939</v>
+        <v>-12.11</v>
+      </c>
+      <c r="AB16" s="2" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="17">
@@ -1828,83 +1878,86 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>-28.45714285714286</v>
+      <c r="B17" s="2" t="n">
+        <v>8.69</v>
       </c>
       <c r="C17" t="n">
-        <v>-130</v>
+        <v>-45.38</v>
       </c>
       <c r="D17" t="n">
-        <v>-63.36363636363637</v>
+        <v>-9.67</v>
       </c>
       <c r="E17" t="n">
-        <v>-37.23076923076923</v>
+        <v>-11.59</v>
       </c>
       <c r="F17" t="n">
-        <v>-87.66666666666666</v>
+        <v>-37.67</v>
       </c>
       <c r="G17" t="n">
-        <v>-42.72</v>
+        <v>-8.039999999999999</v>
       </c>
       <c r="H17" t="n">
-        <v>-37.21212121212121</v>
+        <v>-9.4</v>
       </c>
       <c r="I17" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="J17" t="n">
-        <v>-53.3235294117647</v>
+        <v>-4.46</v>
       </c>
       <c r="K17" t="n">
-        <v>-53.66666666666666</v>
-      </c>
-      <c r="L17" t="n">
-        <v>-67.66666666666667</v>
+        <v>-4.46</v>
+      </c>
+      <c r="L17" s="2" t="n">
+        <v>9.69</v>
       </c>
       <c r="M17" t="n">
-        <v>-39.67241379310346</v>
+        <v>-8.07</v>
       </c>
       <c r="N17" s="2" t="n">
-        <v>177.6666666666667</v>
+        <v>211</v>
       </c>
       <c r="O17" t="n">
-        <v>-34.91044776119403</v>
-      </c>
-      <c r="P17" t="n">
-        <v>-45.68571428571429</v>
+        <v>-11.72</v>
+      </c>
+      <c r="P17" s="2" t="n">
+        <v>1.61</v>
       </c>
       <c r="Q17" t="n">
-        <v>-56.77142857142857</v>
+        <v>-5.75</v>
       </c>
       <c r="R17" t="n">
-        <v>-99.42307692307692</v>
+        <v>-34.04</v>
       </c>
       <c r="S17" t="n">
-        <v>-76.96428571428571</v>
+        <v>-16.25</v>
       </c>
       <c r="T17" s="2" t="n">
-        <v>1.437500000000003</v>
+        <v>40.72</v>
       </c>
       <c r="U17" t="n">
-        <v>-32.97368421052632</v>
+        <v>-9.289999999999999</v>
       </c>
       <c r="V17" t="n">
-        <v>-200</v>
-      </c>
-      <c r="W17" t="n">
-        <v>-16.16129032258065</v>
+        <v>-100</v>
+      </c>
+      <c r="W17" s="2" t="n">
+        <v>4.73</v>
       </c>
       <c r="X17" t="n">
-        <v>-30.09523809523812</v>
+        <v>-2.57</v>
       </c>
       <c r="Y17" t="n">
-        <v>-153.5714285714286</v>
+        <v>-67.86</v>
       </c>
       <c r="Z17" t="n">
-        <v>-113.5</v>
+        <v>-31.21</v>
       </c>
       <c r="AA17" t="n">
-        <v>-57.5344827586207</v>
+        <v>-17.88</v>
+      </c>
+      <c r="AB17" s="2" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="18">
@@ -1914,82 +1967,85 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-78.51063829787235</v>
-      </c>
-      <c r="C18" t="n">
-        <v>-15.55555555555555</v>
-      </c>
-      <c r="D18" t="n">
-        <v>-48.54166666666666</v>
+        <v>-23.52</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>5.4</v>
       </c>
       <c r="E18" t="n">
-        <v>-31.30232558139535</v>
+        <v>-3.17</v>
       </c>
       <c r="F18" t="n">
-        <v>-43.99999999999999</v>
-      </c>
-      <c r="G18" t="n">
-        <v>-6.799999999999998</v>
+        <v>-17.54</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>8.85</v>
       </c>
       <c r="H18" t="n">
-        <v>-52.95454545454545</v>
+        <v>-15.39</v>
       </c>
       <c r="I18" t="n">
-        <v>-83.92857142857143</v>
+        <v>-18.33</v>
       </c>
       <c r="J18" t="n">
-        <v>-88.11764705882354</v>
-      </c>
-      <c r="K18" t="n">
-        <v>-35.45652173913044</v>
+        <v>-24.95</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>3.51</v>
       </c>
       <c r="L18" t="n">
-        <v>-128.5714285714286</v>
+        <v>-42.86</v>
       </c>
       <c r="M18" t="n">
-        <v>-24.42465753424657</v>
+        <v>-3.87</v>
       </c>
       <c r="N18" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="O18" t="n">
-        <v>-10.55696202531644</v>
+        <v>-1.02</v>
       </c>
       <c r="P18" t="n">
-        <v>-78.02857142857144</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>-41.91111111111111</v>
+        <v>-18.74</v>
+      </c>
+      <c r="Q18" s="2" t="n">
+        <v>1.79</v>
       </c>
       <c r="R18" t="n">
-        <v>-94.56</v>
-      </c>
-      <c r="S18" t="n">
-        <v>-13.10000000000001</v>
+        <v>-30.86</v>
+      </c>
+      <c r="S18" s="2" t="n">
+        <v>32.12</v>
       </c>
       <c r="T18" t="n">
-        <v>-168.3333333333333</v>
-      </c>
-      <c r="U18" t="n">
-        <v>-16.93333333333334</v>
+        <v>-75</v>
+      </c>
+      <c r="U18" s="2" t="n">
+        <v>0.22</v>
       </c>
       <c r="V18" s="2" t="n">
-        <v>2.999999999999996</v>
+        <v>28</v>
       </c>
       <c r="W18" t="n">
-        <v>-38.17391304347826</v>
+        <v>-6.58</v>
       </c>
       <c r="X18" t="n">
-        <v>-52.41538461538462</v>
+        <v>-16.43</v>
       </c>
       <c r="Y18" t="n">
-        <v>-76.59999999999999</v>
+        <v>-15.56</v>
       </c>
       <c r="Z18" s="2" t="n">
-        <v>43.91666666666666</v>
+        <v>71.31</v>
       </c>
       <c r="AA18" t="n">
-        <v>-31.73529411764705</v>
+        <v>-3.21</v>
+      </c>
+      <c r="AB18" s="2" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="19">
@@ -1999,80 +2055,83 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-62.45</v>
+        <v>-12.45</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="D19" t="n">
-        <v>-77.625</v>
+        <v>-15.12</v>
       </c>
       <c r="E19" t="n">
-        <v>-19.82758620689655</v>
+        <v>-2.59</v>
       </c>
       <c r="F19" t="n">
-        <v>-74.59999999999999</v>
+        <v>-29.6</v>
       </c>
       <c r="G19" t="n">
-        <v>-48.00000000000001</v>
+        <v>-14.67</v>
       </c>
       <c r="H19" t="n">
-        <v>-35.77777777777778</v>
-      </c>
-      <c r="I19" t="n">
-        <v>-66.75</v>
+        <v>-9.85</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>8.25</v>
       </c>
       <c r="J19" t="n">
-        <v>-48.66666666666667</v>
+        <v>-5.33</v>
       </c>
       <c r="K19" t="n">
-        <v>-51.85714285714285</v>
-      </c>
-      <c r="L19" t="n">
-        <v>-47</v>
+        <v>-1.86</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>7.55</v>
       </c>
       <c r="M19" t="n">
-        <v>-52.70212765957447</v>
+        <v>-14.4</v>
       </c>
       <c r="N19" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="O19" t="n">
-        <v>-33.56140350877194</v>
+        <v>-10.75</v>
       </c>
       <c r="P19" t="n">
-        <v>-46.94736842105263</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>-38.25641025641026</v>
-      </c>
-      <c r="R19" t="n">
-        <v>-24.84210526315789</v>
+        <v>-4.84</v>
+      </c>
+      <c r="Q19" s="2" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="R19" s="2" t="n">
+        <v>22.53</v>
       </c>
       <c r="S19" t="n">
-        <v>-74.03225806451613</v>
+        <v>-12.74</v>
       </c>
       <c r="T19" t="n">
-        <v>-114.375</v>
+        <v>-39.38</v>
       </c>
       <c r="U19" t="n">
-        <v>-38.47500000000001</v>
+        <v>-10.98</v>
       </c>
       <c r="V19" t="inlineStr"/>
-      <c r="W19" t="n">
-        <v>-20.5</v>
+      <c r="W19" s="2" t="n">
+        <v>1.72</v>
       </c>
       <c r="X19" t="n">
-        <v>-31.44444444444445</v>
+        <v>-3.67</v>
       </c>
       <c r="Y19" s="2" t="n">
-        <v>106.25</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>-41.69230769230769</v>
-      </c>
-      <c r="AA19" t="n">
-        <v>-30.53333333333333</v>
+        <v>131.25</v>
+      </c>
+      <c r="Z19" s="2" t="n">
+        <v>12.15</v>
+      </c>
+      <c r="AA19" s="2" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="AB19" s="2" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="20">
@@ -2081,81 +2140,84 @@
           <t>Netherlands</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>-21.29411764705882</v>
+      <c r="B20" s="2" t="n">
+        <v>16.95</v>
       </c>
       <c r="C20" t="n">
-        <v>-100</v>
-      </c>
-      <c r="D20" t="n">
-        <v>-31.90909090909091</v>
-      </c>
-      <c r="E20" t="n">
-        <v>-13.77777777777778</v>
+        <v>-20</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>13.55</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>3.5</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>29</v>
       </c>
       <c r="G20" t="n">
-        <v>-51.16666666666667</v>
+        <v>-17.83</v>
       </c>
       <c r="H20" t="n">
-        <v>-48.65625000000001</v>
+        <v>-15.12</v>
       </c>
       <c r="I20" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="J20" t="n">
-        <v>-66.77777777777779</v>
+        <v>-7.95</v>
       </c>
       <c r="K20" t="n">
-        <v>-66.39999999999999</v>
+        <v>-13.07</v>
       </c>
       <c r="L20" t="n">
-        <v>-35</v>
-      </c>
-      <c r="M20" t="n">
-        <v>-10.06896551724138</v>
+        <v>-8</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>11.37</v>
       </c>
       <c r="N20" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="O20" t="n">
-        <v>-25.15625</v>
+        <v>-5.88</v>
       </c>
       <c r="P20" t="n">
-        <v>-49.00000000000001</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>-11.26315789473685</v>
-      </c>
-      <c r="R20" t="n">
-        <v>-49.42857142857143</v>
+        <v>-12.4</v>
+      </c>
+      <c r="Q20" s="2" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="R20" s="2" t="n">
+        <v>11.67</v>
       </c>
       <c r="S20" t="n">
-        <v>-82.72727272727273</v>
+        <v>-25.83</v>
       </c>
       <c r="T20" t="n">
-        <v>-123.375</v>
-      </c>
-      <c r="U20" t="n">
-        <v>-11.64999999999999</v>
+        <v>-48.38</v>
+      </c>
+      <c r="U20" s="2" t="n">
+        <v>3.43</v>
       </c>
       <c r="V20" t="inlineStr"/>
       <c r="W20" t="n">
-        <v>-9.769230769230766</v>
+        <v>-1.93</v>
       </c>
       <c r="X20" t="n">
-        <v>-40.44827586206895</v>
+        <v>-8.27</v>
       </c>
       <c r="Y20" t="n">
-        <v>-106.25</v>
+        <v>-45</v>
       </c>
       <c r="Z20" t="n">
-        <v>-92.22222222222223</v>
+        <v>-11</v>
       </c>
       <c r="AA20" t="n">
-        <v>-47.66666666666667</v>
+        <v>-13.76</v>
+      </c>
+      <c r="AB20" s="2" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="21">
@@ -2164,75 +2226,78 @@
           <t>Norway</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>-45.61538461538461</v>
+      <c r="B21" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="n">
-        <v>-48</v>
+      <c r="D21" s="2" t="n">
+        <v>12.41</v>
       </c>
       <c r="E21" t="n">
-        <v>-29.2</v>
+        <v>-7.09</v>
       </c>
       <c r="F21" t="n">
-        <v>-23.61111111111111</v>
+        <v>-0.17</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>21.8</v>
+        <v>19.33</v>
       </c>
       <c r="H21" t="n">
-        <v>-40.80392156862745</v>
+        <v>-11.02</v>
       </c>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="n">
-        <v>-15.3125</v>
+      <c r="J21" s="2" t="n">
+        <v>10.05</v>
       </c>
       <c r="K21" s="2" t="n">
-        <v>7.105263157894726</v>
+        <v>37.73</v>
       </c>
       <c r="L21" t="n">
-        <v>-49.75000000000001</v>
-      </c>
-      <c r="M21" t="n">
-        <v>-33.02127659574469</v>
+        <v>-19.8</v>
+      </c>
+      <c r="M21" s="2" t="n">
+        <v>2.39</v>
       </c>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>-23.76470588235293</v>
+        <v>-2.9</v>
       </c>
       <c r="P21" t="n">
-        <v>-69.28</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>-10.92307692307694</v>
-      </c>
-      <c r="R21" t="n">
-        <v>-4.199999999999999</v>
+        <v>-19.11</v>
+      </c>
+      <c r="Q21" s="2" t="n">
+        <v>26.16</v>
+      </c>
+      <c r="R21" s="2" t="n">
+        <v>13.17</v>
       </c>
       <c r="S21" t="n">
-        <v>-81.65116279069767</v>
+        <v>-18.82</v>
       </c>
       <c r="T21" t="n">
-        <v>-90</v>
+        <v>-23.33</v>
       </c>
       <c r="U21" t="n">
-        <v>-24.53333333333333</v>
+        <v>-8.34</v>
       </c>
       <c r="V21" t="inlineStr"/>
       <c r="W21" t="n">
-        <v>-45.61904761904763</v>
+        <v>-18.75</v>
       </c>
       <c r="X21" t="n">
-        <v>-39.3</v>
+        <v>-8.279999999999999</v>
       </c>
       <c r="Y21" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="Z21" s="2" t="n">
-        <v>10.00000000000001</v>
+        <v>43.33</v>
       </c>
       <c r="AA21" t="n">
-        <v>-54.97916666666667</v>
+        <v>-9.460000000000001</v>
+      </c>
+      <c r="AB21" s="2" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="22">
@@ -2241,81 +2306,84 @@
           <t>Poland</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>-36.52777777777778</v>
+      <c r="B22" s="2" t="n">
+        <v>3.46</v>
       </c>
       <c r="C22" t="n">
-        <v>-200</v>
-      </c>
-      <c r="D22" t="n">
-        <v>-4.6875</v>
+        <v>-100</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>42.06</v>
       </c>
       <c r="E22" t="n">
-        <v>-26.81818181818181</v>
-      </c>
-      <c r="F22" t="n">
-        <v>-0.3478260869565143</v>
+        <v>-2.29</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>13.88</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>5.624999999999991</v>
+        <v>18.12</v>
       </c>
       <c r="H22" t="n">
-        <v>-36.45454545454545</v>
-      </c>
-      <c r="I22" t="n">
-        <v>-65.22222222222223</v>
+        <v>-6.58</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>1.44</v>
       </c>
       <c r="J22" t="n">
-        <v>-71.94736842105263</v>
+        <v>-10.39</v>
       </c>
       <c r="K22" t="n">
-        <v>-49.58823529411764</v>
-      </c>
-      <c r="L22" t="n">
-        <v>-44.99999999999999</v>
+        <v>-2.53</v>
+      </c>
+      <c r="L22" s="2" t="n">
+        <v>5</v>
       </c>
       <c r="M22" t="n">
-        <v>-30.94117647058825</v>
+        <v>-2.69</v>
       </c>
       <c r="N22" s="2" t="n">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="O22" t="n">
-        <v>-17.09803921568626</v>
+        <v>-2</v>
       </c>
       <c r="P22" t="n">
-        <v>-92</v>
+        <v>-34.85</v>
       </c>
       <c r="Q22" t="n">
-        <v>-54.49999999999999</v>
+        <v>-7.08</v>
       </c>
       <c r="R22" t="n">
-        <v>-121.875</v>
+        <v>-37</v>
       </c>
       <c r="S22" t="n">
-        <v>-86.23809523809524</v>
+        <v>-25.5</v>
       </c>
       <c r="T22" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="U22" t="n">
-        <v>-38.22222222222222</v>
+        <v>-13.47</v>
       </c>
       <c r="V22" t="inlineStr"/>
       <c r="W22" t="n">
-        <v>-47.03846153846154</v>
-      </c>
-      <c r="X22" t="n">
-        <v>-23.1</v>
+        <v>-10.48</v>
+      </c>
+      <c r="X22" s="2" t="n">
+        <v>4.73</v>
       </c>
       <c r="Y22" t="n">
-        <v>-81.69230769230769</v>
+        <v>-12.46</v>
       </c>
       <c r="Z22" t="n">
-        <v>-64.375</v>
+        <v>-12.78</v>
       </c>
       <c r="AA22" t="n">
-        <v>-29.4</v>
+        <v>-3.81</v>
+      </c>
+      <c r="AB22" s="2" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="23">
@@ -2324,81 +2392,84 @@
           <t>Portugal</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>-30.52</v>
+      <c r="B23" s="2" t="n">
+        <v>5.48</v>
       </c>
       <c r="C23" t="n">
-        <v>-110</v>
+        <v>-30</v>
       </c>
       <c r="D23" t="n">
-        <v>-87.4375</v>
-      </c>
-      <c r="E23" t="n">
-        <v>-2.727272727272734</v>
+        <v>-31.19</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>6.36</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>1.857142857142868</v>
+        <v>16.14</v>
       </c>
       <c r="G23" t="n">
-        <v>-25.94117647058824</v>
+        <v>-2.41</v>
       </c>
       <c r="H23" t="n">
-        <v>-43.54285714285715</v>
+        <v>-12.11</v>
       </c>
       <c r="I23" t="n">
-        <v>-120.4545454545455</v>
-      </c>
-      <c r="J23" t="n">
-        <v>-39.00000000000001</v>
+        <v>-38.64</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>2.18</v>
       </c>
       <c r="K23" t="n">
-        <v>-55.72413793103447</v>
+        <v>-10.9</v>
       </c>
       <c r="L23" t="n">
-        <v>-106</v>
+        <v>-39.33</v>
       </c>
       <c r="M23" t="n">
-        <v>-33.70000000000001</v>
+        <v>-6.2</v>
       </c>
       <c r="N23" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="O23" t="n">
-        <v>-26.95454545454547</v>
+        <v>-8.77</v>
       </c>
       <c r="P23" t="n">
-        <v>-64.57142857142858</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>-31.69230769230769</v>
-      </c>
-      <c r="R23" t="n">
-        <v>-19.25</v>
-      </c>
-      <c r="S23" t="n">
-        <v>-44.07142857142857</v>
+        <v>-7.43</v>
+      </c>
+      <c r="Q23" s="2" t="n">
+        <v>6.77</v>
+      </c>
+      <c r="R23" s="2" t="n">
+        <v>14.08</v>
+      </c>
+      <c r="S23" s="2" t="n">
+        <v>5.93</v>
       </c>
       <c r="T23" t="n">
-        <v>-157.8333333333333</v>
+        <v>-74.5</v>
       </c>
       <c r="U23" s="2" t="n">
-        <v>4.999999999999989</v>
+        <v>8.85</v>
       </c>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="n">
-        <v>-35.24999999999999</v>
+        <v>-10.25</v>
       </c>
       <c r="X23" t="n">
-        <v>-33.83333333333334</v>
-      </c>
-      <c r="Y23" t="n">
-        <v>-30.375</v>
-      </c>
-      <c r="Z23" t="n">
-        <v>-9.999999999999993</v>
+        <v>-3.83</v>
+      </c>
+      <c r="Y23" s="2" t="n">
+        <v>25.88</v>
+      </c>
+      <c r="Z23" s="2" t="n">
+        <v>40</v>
       </c>
       <c r="AA23" t="n">
-        <v>-48.17647058823528</v>
+        <v>-12.88</v>
+      </c>
+      <c r="AB23" s="2" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="24">
@@ -2407,81 +2478,84 @@
           <t>Portugal2</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>-30.80000000000001</v>
+      <c r="B24" s="2" t="n">
+        <v>15.87</v>
       </c>
       <c r="C24" t="n">
-        <v>-118</v>
+        <v>-38</v>
       </c>
       <c r="D24" t="n">
-        <v>-89.11764705882352</v>
-      </c>
-      <c r="E24" t="n">
-        <v>-23.17647058823529</v>
+        <v>-7.78</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.35</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>34.50000000000002</v>
-      </c>
-      <c r="G24" t="n">
-        <v>-2.388888888888887</v>
-      </c>
-      <c r="H24" t="n">
-        <v>-12.40000000000001</v>
+        <v>34.5</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>21.58</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>8.19</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>12.5</v>
+        <v>62.5</v>
       </c>
       <c r="J24" t="n">
-        <v>-82</v>
-      </c>
-      <c r="K24" t="n">
-        <v>-31.52380952380954</v>
+        <v>-24.24</v>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>6.57</v>
       </c>
       <c r="L24" t="n">
-        <v>-81.25</v>
+        <v>-25</v>
       </c>
       <c r="M24" s="2" t="n">
-        <v>4.878787878787877</v>
+        <v>13.97</v>
       </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" s="2" t="n">
-        <v>8.189189189189211</v>
+        <v>8.26</v>
       </c>
       <c r="P24" t="n">
-        <v>-79.94736842105263</v>
+        <v>-25.95</v>
       </c>
       <c r="Q24" t="n">
-        <v>-105.1111111111111</v>
-      </c>
-      <c r="R24" t="n">
-        <v>-30.45454545454545</v>
+        <v>-38.44</v>
+      </c>
+      <c r="R24" s="2" t="n">
+        <v>24.09</v>
       </c>
       <c r="S24" t="n">
-        <v>-85.3125</v>
+        <v>-22.81</v>
       </c>
       <c r="T24" t="n">
-        <v>-161.2</v>
+        <v>-42.91</v>
       </c>
       <c r="U24" t="n">
-        <v>-42.47058823529412</v>
+        <v>-13.06</v>
       </c>
       <c r="V24" t="n">
-        <v>-60</v>
+        <v>-10</v>
       </c>
       <c r="W24" s="2" t="n">
-        <v>11.05555555555557</v>
-      </c>
-      <c r="X24" t="n">
-        <v>-4.032258064516141</v>
+        <v>22.89</v>
+      </c>
+      <c r="X24" s="2" t="n">
+        <v>16.09</v>
       </c>
       <c r="Y24" s="2" t="n">
-        <v>37.66666666666666</v>
+        <v>71</v>
       </c>
       <c r="Z24" t="n">
-        <v>-100</v>
+        <v>-30.77</v>
       </c>
       <c r="AA24" t="n">
-        <v>-41.99999999999999</v>
+        <v>-10</v>
+      </c>
+      <c r="AB24" s="2" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="25">
@@ -2490,83 +2564,86 @@
           <t>Scotland</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>-14.85714285714287</v>
+      <c r="B25" s="2" t="n">
+        <v>30.61</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="D25" t="n">
-        <v>-49.5</v>
-      </c>
-      <c r="E25" t="n">
-        <v>-11.05</v>
+        <v>-23.45</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>6.09</v>
       </c>
       <c r="F25" t="n">
-        <v>-46.5</v>
+        <v>-9.85</v>
       </c>
       <c r="G25" t="n">
-        <v>-18.88888888888888</v>
-      </c>
-      <c r="H25" t="n">
-        <v>-20.74358974358975</v>
+        <v>-13.33</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>0.42</v>
       </c>
       <c r="I25" t="n">
-        <v>-200</v>
-      </c>
-      <c r="J25" t="n">
-        <v>-32.40909090909091</v>
+        <v>-100</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>11</v>
       </c>
       <c r="K25" t="n">
-        <v>-121.7368421052632</v>
+        <v>-43.77</v>
       </c>
       <c r="L25" t="n">
-        <v>-67.22222222222223</v>
-      </c>
-      <c r="M25" t="n">
-        <v>-13.15625</v>
+        <v>-10.5</v>
+      </c>
+      <c r="M25" s="2" t="n">
+        <v>5.3</v>
       </c>
       <c r="N25" s="2" t="n">
-        <v>33.33333333333333</v>
+        <v>100</v>
       </c>
       <c r="O25" t="n">
-        <v>-18.63157894736843</v>
-      </c>
-      <c r="P25" t="n">
-        <v>-6.374999999999997</v>
+        <v>-5.75</v>
+      </c>
+      <c r="P25" s="2" t="n">
+        <v>23.42</v>
       </c>
       <c r="Q25" t="n">
-        <v>-73.84</v>
-      </c>
-      <c r="R25" t="n">
-        <v>-47.92857142857142</v>
-      </c>
-      <c r="S25" t="n">
-        <v>-49.76190476190476</v>
+        <v>-26.64</v>
+      </c>
+      <c r="R25" s="2" t="n">
+        <v>17.93</v>
+      </c>
+      <c r="S25" s="2" t="n">
+        <v>2.8</v>
       </c>
       <c r="T25" t="n">
-        <v>-70.16666666666667</v>
+        <v>-31.57</v>
       </c>
       <c r="U25" t="n">
-        <v>-20.50000000000001</v>
+        <v>-3.29</v>
       </c>
       <c r="V25" s="2" t="n">
-        <v>57.00000000000001</v>
+        <v>57</v>
       </c>
       <c r="W25" t="n">
-        <v>-69.08333333333333</v>
+        <v>-26</v>
       </c>
       <c r="X25" t="n">
-        <v>-19.33333333333333</v>
+        <v>-3.67</v>
       </c>
       <c r="Y25" t="n">
-        <v>-91.92857142857143</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>-57.07692307692308</v>
-      </c>
-      <c r="AA25" t="n">
-        <v>-34.28571428571429</v>
+        <v>-20.5</v>
+      </c>
+      <c r="Z25" s="2" t="n">
+        <v>4.46</v>
+      </c>
+      <c r="AA25" s="2" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="AB25" s="2" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="26">
@@ -2576,78 +2653,83 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-51.38888888888889</v>
+        <v>-4.46</v>
       </c>
       <c r="C26" t="n">
-        <v>-72.40000000000001</v>
+        <v>-8.08</v>
       </c>
       <c r="D26" t="n">
-        <v>-56.21428571428572</v>
+        <v>-17.94</v>
       </c>
       <c r="E26" t="n">
-        <v>-27.85185185185186</v>
+        <v>-6.31</v>
       </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
-        <v>-60.33333333333334</v>
+        <v>-23.87</v>
       </c>
       <c r="H26" t="n">
-        <v>-33.34426229508198</v>
+        <v>-2.39</v>
       </c>
       <c r="I26" t="n">
-        <v>-103.5714285714286</v>
-      </c>
-      <c r="J26" t="n">
-        <v>-38.17857142857143</v>
+        <v>-36.67</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>5.67</v>
       </c>
       <c r="K26" t="n">
-        <v>-35.95744680851063</v>
+        <v>-4.82</v>
       </c>
       <c r="L26" t="n">
-        <v>-70.19999999999999</v>
+        <v>-2.69</v>
       </c>
       <c r="M26" t="n">
-        <v>-18.56666666666667</v>
+        <v>-4.15</v>
       </c>
       <c r="N26" t="n">
-        <v>-112</v>
+        <v>-43.33</v>
       </c>
       <c r="O26" t="n">
-        <v>-14.97142857142858</v>
+        <v>-7.11</v>
       </c>
       <c r="P26" t="n">
-        <v>-55.12</v>
+        <v>-1.37</v>
       </c>
       <c r="Q26" t="n">
-        <v>-77.31999999999999</v>
-      </c>
-      <c r="R26" t="n">
-        <v>-3.176470588235289</v>
-      </c>
-      <c r="S26" t="n">
-        <v>-43.90196078431373</v>
-      </c>
-      <c r="T26" t="n">
-        <v>-54.57142857142857</v>
+        <v>-26.33</v>
+      </c>
+      <c r="R26" s="2" t="n">
+        <v>30.05</v>
+      </c>
+      <c r="S26" s="2" t="n">
+        <v>9.960000000000001</v>
+      </c>
+      <c r="T26" s="2" t="n">
+        <v>16</v>
       </c>
       <c r="U26" t="n">
-        <v>-28.125</v>
-      </c>
-      <c r="V26" t="inlineStr"/>
+        <v>-7.65</v>
+      </c>
+      <c r="V26" s="2" t="n">
+        <v>50</v>
+      </c>
       <c r="W26" t="n">
-        <v>-48.88888888888889</v>
-      </c>
-      <c r="X26" t="n">
-        <v>-14.95555555555556</v>
-      </c>
-      <c r="Y26" t="n">
-        <v>-49.46666666666668</v>
-      </c>
-      <c r="Z26" t="n">
-        <v>-7.071428571428561</v>
-      </c>
-      <c r="AA26" t="n">
-        <v>-13.24590163934426</v>
+        <v>-14.11</v>
+      </c>
+      <c r="X26" s="2" t="n">
+        <v>6.78</v>
+      </c>
+      <c r="Y26" s="2" t="n">
+        <v>7.37</v>
+      </c>
+      <c r="Z26" s="2" t="n">
+        <v>26.73</v>
+      </c>
+      <c r="AA26" s="2" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="AB26" s="2" t="n">
+        <v>81</v>
       </c>
     </row>
     <row r="27">
@@ -2657,82 +2739,85 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-57.25714285714285</v>
+        <v>-5.83</v>
       </c>
       <c r="C27" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="D27" t="n">
-        <v>-133.68</v>
+        <v>-50.41</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>2.5</v>
+        <v>12.5</v>
       </c>
       <c r="F27" t="n">
-        <v>-44.81249999999999</v>
+        <v>-11.49</v>
       </c>
       <c r="G27" t="n">
-        <v>-90.85714285714286</v>
-      </c>
-      <c r="H27" t="n">
-        <v>-15.34042553191489</v>
-      </c>
-      <c r="I27" t="n">
-        <v>-35.33333333333333</v>
-      </c>
-      <c r="J27" t="n">
-        <v>-1.961538461538481</v>
+        <v>-25</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>22.47</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>37.75</v>
       </c>
       <c r="K27" t="n">
-        <v>-68.58974358974359</v>
+        <v>-18.76</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>44.00000000000001</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="M27" t="n">
-        <v>-59</v>
-      </c>
-      <c r="N27" t="n">
-        <v>-16.66666666666666</v>
+        <v>-23.19</v>
+      </c>
+      <c r="N27" s="2" t="n">
+        <v>50</v>
       </c>
       <c r="O27" t="n">
-        <v>-23.29032258064515</v>
-      </c>
-      <c r="P27" t="n">
-        <v>-11.81818181818181</v>
+        <v>-7.79</v>
+      </c>
+      <c r="P27" s="2" t="n">
+        <v>25.13</v>
       </c>
       <c r="Q27" t="n">
-        <v>-79.58139534883721</v>
-      </c>
-      <c r="R27" t="n">
-        <v>-32.93333333333333</v>
+        <v>-21.69</v>
+      </c>
+      <c r="R27" s="2" t="n">
+        <v>27.07</v>
       </c>
       <c r="S27" t="n">
-        <v>-98.65853658536587</v>
+        <v>-29.76</v>
       </c>
       <c r="T27" t="n">
-        <v>-144.4444444444444</v>
-      </c>
-      <c r="U27" t="n">
-        <v>-4.038461538461542</v>
-      </c>
-      <c r="V27" t="n">
-        <v>-37.2</v>
+        <v>-66.67</v>
+      </c>
+      <c r="U27" s="2" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="V27" s="2" t="n">
+        <v>2.8</v>
       </c>
       <c r="W27" t="n">
-        <v>-68.0344827586207</v>
-      </c>
-      <c r="X27" t="n">
-        <v>-3.485714285714282</v>
+        <v>-17</v>
+      </c>
+      <c r="X27" s="2" t="n">
+        <v>11.74</v>
       </c>
       <c r="Y27" t="n">
-        <v>-124.2</v>
+        <v>-47.53</v>
       </c>
       <c r="Z27" s="2" t="n">
-        <v>23.88888888888889</v>
+        <v>68.33</v>
       </c>
       <c r="AA27" t="n">
-        <v>-61.64285714285715</v>
+        <v>-23.37</v>
+      </c>
+      <c r="AB27" s="2" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="28">
@@ -2742,74 +2827,77 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-57.26190476190476</v>
+        <v>-7.26</v>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="n">
-        <v>-98.1304347826087</v>
+        <v>-28.57</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>6.388888888888881</v>
+        <v>11.94</v>
       </c>
       <c r="F28" t="n">
-        <v>-42.22222222222222</v>
+        <v>-11.11</v>
       </c>
       <c r="G28" t="n">
-        <v>-91</v>
+        <v>-41</v>
       </c>
       <c r="H28" t="n">
-        <v>-39.20000000000001</v>
+        <v>-11.51</v>
       </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="n">
-        <v>-87.55</v>
-      </c>
-      <c r="K28" t="n">
-        <v>-10</v>
+        <v>-30.05</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>26</v>
       </c>
       <c r="L28" t="n">
-        <v>-84.72727272727273</v>
+        <v>-21.09</v>
       </c>
       <c r="M28" s="2" t="n">
-        <v>13.61111111111111</v>
+        <v>24.72</v>
       </c>
       <c r="N28" t="inlineStr"/>
       <c r="O28" s="2" t="n">
-        <v>10.07692307692305</v>
+        <v>13.15</v>
       </c>
       <c r="P28" t="n">
-        <v>-64.23684210526316</v>
+        <v>-14.24</v>
       </c>
       <c r="Q28" t="n">
-        <v>-54.59259259259258</v>
+        <v>-2.74</v>
       </c>
       <c r="R28" t="n">
-        <v>-106.0909090909091</v>
+        <v>-37.91</v>
       </c>
       <c r="S28" t="n">
-        <v>-68.56666666666666</v>
+        <v>-8.57</v>
       </c>
       <c r="T28" t="n">
-        <v>-118.4615384615385</v>
+        <v>-41.54</v>
       </c>
       <c r="U28" t="n">
-        <v>-26.45945945945946</v>
+        <v>-4.84</v>
       </c>
       <c r="V28" t="inlineStr"/>
-      <c r="W28" t="n">
-        <v>-22.96428571428571</v>
+      <c r="W28" s="2" t="n">
+        <v>2.04</v>
       </c>
       <c r="X28" t="n">
-        <v>-53.2258064516129</v>
+        <v>-16.13</v>
       </c>
       <c r="Y28" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="Z28" t="n">
-        <v>-77.83333333333333</v>
-      </c>
-      <c r="AA28" t="n">
-        <v>-13.84905660377358</v>
+        <v>-11.17</v>
+      </c>
+      <c r="AA28" s="2" t="n">
+        <v>10.68</v>
+      </c>
+      <c r="AB28" s="2" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="29">
@@ -2819,76 +2907,79 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-70.96774193548387</v>
+        <v>-17.91</v>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="n">
-        <v>-70.72222222222221</v>
+        <v>-9.609999999999999</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>13.75000000000002</v>
+        <v>14.11</v>
       </c>
       <c r="F29" t="n">
-        <v>-44.00000000000001</v>
+        <v>-13.81</v>
       </c>
       <c r="G29" t="n">
-        <v>-91.16666666666667</v>
+        <v>-41.17</v>
       </c>
       <c r="H29" t="n">
-        <v>-29.81632653061226</v>
+        <v>-8.1</v>
       </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="n">
-        <v>-50.13333333333333</v>
-      </c>
-      <c r="K29" t="n">
-        <v>-40.1578947368421</v>
-      </c>
-      <c r="L29" t="n">
-        <v>-56.2</v>
-      </c>
-      <c r="M29" t="n">
-        <v>-30.74358974358974</v>
+        <v>-9.81</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>16.43</v>
+      </c>
+      <c r="L29" s="2" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="M29" s="2" t="n">
+        <v>3.12</v>
       </c>
       <c r="N29" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="O29" t="n">
-        <v>-23.31250000000001</v>
+        <v>-3.39</v>
       </c>
       <c r="P29" t="n">
-        <v>-44.56000000000001</v>
+        <v>-5.96</v>
       </c>
       <c r="Q29" t="n">
-        <v>-59.24999999999999</v>
+        <v>-8.880000000000001</v>
       </c>
       <c r="R29" t="n">
-        <v>-56.44444444444444</v>
+        <v>-0.89</v>
       </c>
       <c r="S29" t="n">
-        <v>-125.7692307692308</v>
-      </c>
-      <c r="T29" t="n">
-        <v>-30.27777777777778</v>
-      </c>
-      <c r="U29" t="n">
-        <v>-7.347826086956527</v>
+        <v>-30</v>
+      </c>
+      <c r="T29" s="2" t="n">
+        <v>30.83</v>
+      </c>
+      <c r="U29" s="2" t="n">
+        <v>2.5</v>
       </c>
       <c r="V29" t="n">
-        <v>-116.6666666666667</v>
-      </c>
-      <c r="W29" t="n">
-        <v>-18.65217391304347</v>
+        <v>-50</v>
+      </c>
+      <c r="W29" s="2" t="n">
+        <v>3.09</v>
       </c>
       <c r="X29" t="n">
-        <v>-25.34693877551021</v>
+        <v>-4.08</v>
       </c>
       <c r="Y29" t="inlineStr"/>
       <c r="Z29" t="n">
-        <v>-157.75</v>
+        <v>-70.25</v>
       </c>
       <c r="AA29" t="n">
-        <v>-66.34146341463415</v>
+        <v>-15.5</v>
+      </c>
+      <c r="AB29" s="2" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="30">
@@ -2897,81 +2988,84 @@
           <t>Turkey</t>
         </is>
       </c>
-      <c r="B30" t="n">
-        <v>-9.346153846153857</v>
-      </c>
-      <c r="C30" t="n">
-        <v>-34.375</v>
+      <c r="B30" s="2" t="n">
+        <v>16.93</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>28.12</v>
       </c>
       <c r="D30" t="n">
-        <v>-55.00000000000001</v>
+        <v>-1.26</v>
       </c>
       <c r="E30" t="n">
-        <v>-27.63636363636364</v>
+        <v>-9.18</v>
       </c>
       <c r="F30" t="n">
-        <v>-46.66666666666666</v>
-      </c>
-      <c r="G30" t="n">
-        <v>-23.92592592592594</v>
+        <v>-7.14</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>2.55</v>
       </c>
       <c r="H30" t="n">
-        <v>-27.42622950819673</v>
-      </c>
-      <c r="I30" t="n">
-        <v>-57.40000000000001</v>
+        <v>-4.69</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>2.6</v>
       </c>
       <c r="J30" t="n">
-        <v>-58.52941176470588</v>
+        <v>-9.050000000000001</v>
       </c>
       <c r="K30" t="n">
-        <v>-95.4375</v>
+        <v>-34.97</v>
       </c>
       <c r="L30" t="n">
-        <v>-129.5</v>
+        <v>-54.5</v>
       </c>
       <c r="M30" t="n">
-        <v>-53.13793103448275</v>
+        <v>-14.06</v>
       </c>
       <c r="N30" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="O30" t="n">
-        <v>-27.29032258064515</v>
+        <v>-8.35</v>
       </c>
       <c r="P30" t="n">
-        <v>-57.05882352941176</v>
+        <v>-12.57</v>
       </c>
       <c r="Q30" t="n">
-        <v>-93.59375</v>
-      </c>
-      <c r="R30" t="n">
-        <v>-29.33333333333334</v>
+        <v>-31.77</v>
+      </c>
+      <c r="R30" s="2" t="n">
+        <v>15.11</v>
       </c>
       <c r="S30" t="n">
-        <v>-99.00000000000001</v>
-      </c>
-      <c r="T30" t="n">
-        <v>-43.37500000000001</v>
-      </c>
-      <c r="U30" t="n">
-        <v>-15.4375</v>
+        <v>-33.93</v>
+      </c>
+      <c r="T30" s="2" t="n">
+        <v>11.17</v>
+      </c>
+      <c r="U30" s="2" t="n">
+        <v>1.79</v>
       </c>
       <c r="V30" t="inlineStr"/>
       <c r="W30" t="n">
-        <v>-29.32352941176469</v>
+        <v>-2.11</v>
       </c>
       <c r="X30" t="n">
-        <v>-27.48888888888888</v>
+        <v>-0.55</v>
       </c>
       <c r="Y30" t="n">
-        <v>-85.66666666666669</v>
+        <v>-14.24</v>
       </c>
       <c r="Z30" t="n">
-        <v>-124.6</v>
+        <v>-47.24</v>
       </c>
       <c r="AA30" t="n">
-        <v>-39.93478260869566</v>
+        <v>-8.1</v>
+      </c>
+      <c r="AB30" s="2" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="31">
@@ -2981,80 +3075,83 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-71.53571428571429</v>
+        <v>-25.11</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>14.16666666666666</v>
-      </c>
-      <c r="D31" t="n">
-        <v>-44.28571428571429</v>
+        <v>64.17</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>5.71</v>
       </c>
       <c r="E31" t="n">
-        <v>-31.62068965517242</v>
+        <v>-10.93</v>
       </c>
       <c r="F31" t="n">
-        <v>-27.625</v>
-      </c>
-      <c r="G31" t="n">
-        <v>-14.99999999999999</v>
+        <v>-2.62</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>3.18</v>
       </c>
       <c r="H31" t="n">
-        <v>-45.79411764705883</v>
-      </c>
-      <c r="I31" t="n">
-        <v>-42.07142857142858</v>
-      </c>
-      <c r="J31" t="n">
-        <v>-35.63157894736842</v>
-      </c>
-      <c r="K31" t="n">
-        <v>-9.413793103448265</v>
-      </c>
-      <c r="L31" t="n">
-        <v>-10.39999999999999</v>
-      </c>
-      <c r="M31" t="n">
-        <v>-20.31578947368421</v>
+        <v>-13.44</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>15.07</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>6.47</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>21.62</v>
+      </c>
+      <c r="L31" s="2" t="n">
+        <v>39.6</v>
+      </c>
+      <c r="M31" s="2" t="n">
+        <v>0.74</v>
       </c>
       <c r="N31" s="2" t="n">
-        <v>175</v>
+        <v>208.33</v>
       </c>
       <c r="O31" t="n">
-        <v>-18.33333333333333</v>
-      </c>
-      <c r="P31" t="n">
-        <v>-27.83333333333333</v>
+        <v>-5</v>
+      </c>
+      <c r="P31" s="2" t="n">
+        <v>13.83</v>
       </c>
       <c r="Q31" t="n">
-        <v>-45.61111111111111</v>
+        <v>-3.94</v>
       </c>
       <c r="R31" t="n">
-        <v>-47</v>
+        <v>-1.55</v>
       </c>
       <c r="S31" t="n">
-        <v>-57.00000000000001</v>
-      </c>
-      <c r="T31" t="n">
-        <v>-19.66666666666666</v>
+        <v>-2.16</v>
+      </c>
+      <c r="T31" s="2" t="n">
+        <v>30.33</v>
       </c>
       <c r="U31" t="n">
-        <v>-30.93103448275862</v>
+        <v>-10.24</v>
       </c>
       <c r="V31" t="inlineStr"/>
-      <c r="W31" t="n">
-        <v>-19</v>
+      <c r="W31" s="2" t="n">
+        <v>2.05</v>
       </c>
       <c r="X31" t="n">
-        <v>-65.25000000000001</v>
-      </c>
-      <c r="Y31" t="n">
-        <v>-61.5</v>
+        <v>-21.5</v>
+      </c>
+      <c r="Y31" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="Z31" t="n">
-        <v>-87.47058823529412</v>
-      </c>
-      <c r="AA31" t="n">
-        <v>-13.64516129032257</v>
+        <v>-16.88</v>
+      </c>
+      <c r="AA31" s="2" t="n">
+        <v>5.71</v>
+      </c>
+      <c r="AB31" s="2" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="32">
@@ -3064,72 +3161,75 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-58.12244897959184</v>
+        <v>-11.18</v>
       </c>
       <c r="C32" t="inlineStr"/>
-      <c r="D32" t="n">
-        <v>-28.62499999999999</v>
-      </c>
-      <c r="E32" t="n">
-        <v>-14.17857142857144</v>
-      </c>
-      <c r="F32" t="n">
-        <v>-11.02702702702702</v>
+      <c r="D32" s="2" t="n">
+        <v>25.54</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>5.19</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>18.12500000000001</v>
-      </c>
-      <c r="H32" t="n">
-        <v>-11.8082191780822</v>
+        <v>30.62</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>0.52</v>
       </c>
       <c r="I32" t="inlineStr"/>
-      <c r="J32" t="n">
-        <v>-22.33333333333334</v>
+      <c r="J32" s="2" t="n">
+        <v>5.74</v>
       </c>
       <c r="K32" t="n">
-        <v>-84.625</v>
+        <v>-22.13</v>
       </c>
       <c r="L32" s="2" t="n">
-        <v>1.600000000000001</v>
+        <v>31.6</v>
       </c>
       <c r="M32" t="n">
-        <v>-43.96825396825398</v>
+        <v>-4.29</v>
       </c>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>-24.6027397260274</v>
-      </c>
-      <c r="P32" t="n">
-        <v>-32.00000000000001</v>
+        <v>-2.68</v>
+      </c>
+      <c r="P32" s="2" t="n">
+        <v>0.26</v>
       </c>
       <c r="Q32" t="n">
-        <v>-58.63636363636364</v>
-      </c>
-      <c r="R32" t="n">
-        <v>-35.4</v>
-      </c>
-      <c r="S32" t="n">
-        <v>-23.28</v>
-      </c>
-      <c r="T32" t="n">
-        <v>-57.99999999999999</v>
-      </c>
-      <c r="U32" t="n">
-        <v>-13.50909090909091</v>
+        <v>-4.09</v>
+      </c>
+      <c r="R32" s="2" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="S32" s="2" t="n">
+        <v>24.72</v>
+      </c>
+      <c r="T32" s="2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="U32" s="2" t="n">
+        <v>2.85</v>
       </c>
       <c r="V32" t="inlineStr"/>
-      <c r="W32" t="n">
-        <v>-26.27777777777778</v>
+      <c r="W32" s="2" t="n">
+        <v>1.5</v>
       </c>
       <c r="X32" t="n">
-        <v>-38.87671232876711</v>
+        <v>-10.11</v>
       </c>
       <c r="Y32" t="inlineStr"/>
-      <c r="Z32" t="n">
-        <v>-26.99999999999999</v>
-      </c>
-      <c r="AA32" t="n">
-        <v>-28.29032258064516</v>
+      <c r="Z32" s="2" t="n">
+        <v>18.45</v>
+      </c>
+      <c r="AA32" s="2" t="n">
+        <v>5.58</v>
+      </c>
+      <c r="AB32" s="2" t="n">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comparer updated to combining bets
</commit_message>
<xml_diff>
--- a/ROI_leagues.xlsx
+++ b/ROI_leagues.xlsx
@@ -583,79 +583,79 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-21.09</v>
+        <v>-15.51</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>47.07</v>
+        <v>21.12</v>
       </c>
       <c r="D2" t="n">
-        <v>-78.12</v>
+        <v>-70.79000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>-10.03</v>
+        <v>-10.1</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>-17.57</v>
+        <v>-17.12</v>
       </c>
       <c r="H2" t="n">
-        <v>-12.83</v>
+        <v>-12.16</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>8.449999999999999</v>
+        <v>10.88</v>
       </c>
       <c r="J2" t="n">
-        <v>-46.15</v>
+        <v>-22.67</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>0.95</v>
+        <v>1.55</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" s="2" t="n">
-        <v>2.88</v>
+        <v>1.85</v>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
-        <v>-1.77</v>
+        <v>-1.25</v>
       </c>
       <c r="P2" t="n">
-        <v>-59.5</v>
+        <v>-41.5</v>
       </c>
       <c r="Q2" t="n">
-        <v>-17.01</v>
+        <v>-9.42</v>
       </c>
       <c r="R2" t="n">
-        <v>-43.21</v>
+        <v>-23.82</v>
       </c>
       <c r="S2" s="2" t="n">
-        <v>22.12</v>
+        <v>17.5</v>
       </c>
       <c r="T2" t="n">
         <v>-100</v>
       </c>
       <c r="U2" t="n">
-        <v>-1.42</v>
+        <v>-3.48</v>
       </c>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="n">
-        <v>-0.29</v>
+        <v>-1.56</v>
       </c>
       <c r="X2" t="n">
-        <v>-6.57</v>
+        <v>-1.59</v>
       </c>
       <c r="Y2" s="2" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="Z2" s="2" t="n">
-        <v>37.5</v>
+        <v>34.96</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>-8.33</v>
       </c>
       <c r="AA2" t="n">
-        <v>-9.92</v>
+        <v>-8.98</v>
       </c>
       <c r="AB2" s="2" t="n">
-        <v>104</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3">
@@ -665,83 +665,83 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-35.84</v>
+        <v>-28.26</v>
       </c>
       <c r="C3" t="n">
         <v>-100</v>
       </c>
-      <c r="D3" t="n">
-        <v>-6.43</v>
+      <c r="D3" s="2" t="n">
+        <v>6.8</v>
       </c>
       <c r="E3" t="n">
-        <v>-14.88</v>
+        <v>-10.37</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>9.43</v>
+        <v>13.41</v>
       </c>
       <c r="G3" t="n">
-        <v>-64</v>
+        <v>-32.8</v>
       </c>
       <c r="H3" t="n">
-        <v>-8.289999999999999</v>
+        <v>-1.78</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>300</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>4.79</v>
+        <v>15.77</v>
       </c>
       <c r="K3" t="n">
-        <v>-11.44</v>
+        <v>-17.77</v>
       </c>
       <c r="L3" t="n">
-        <v>-16</v>
+        <v>-2.92</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>11.66</v>
+        <v>12.8</v>
       </c>
       <c r="N3" t="n">
         <v>-100</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>2.4</v>
+        <v>2.22</v>
       </c>
       <c r="P3" t="n">
-        <v>-20.44</v>
+        <v>-15.93</v>
       </c>
       <c r="Q3" t="n">
-        <v>-14.35</v>
+        <v>-7</v>
       </c>
       <c r="R3" t="n">
-        <v>-56.54</v>
+        <v>-59.64</v>
       </c>
       <c r="S3" s="2" t="n">
-        <v>28.32</v>
+        <v>0.25</v>
       </c>
       <c r="T3" s="2" t="n">
-        <v>90</v>
+        <v>64.17</v>
       </c>
       <c r="U3" s="2" t="n">
-        <v>7.64</v>
+        <v>1.1</v>
       </c>
       <c r="V3" t="inlineStr"/>
       <c r="W3" s="2" t="n">
-        <v>10.24</v>
+        <v>7.05</v>
       </c>
       <c r="X3" t="n">
-        <v>-17.22</v>
+        <v>-4.38</v>
       </c>
       <c r="Y3" s="2" t="n">
         <v>21.5</v>
       </c>
-      <c r="Z3" t="n">
-        <v>-9.710000000000001</v>
+      <c r="Z3" s="2" t="n">
+        <v>2.6</v>
       </c>
       <c r="AA3" s="2" t="n">
-        <v>20.07</v>
+        <v>17.32</v>
       </c>
       <c r="AB3" s="2" t="n">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -750,86 +750,86 @@
           <t>Belgium</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>-3.44</v>
+      <c r="B4" s="2" t="n">
+        <v>2.61</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>33.75</v>
+        <v>18.89</v>
       </c>
       <c r="D4" t="n">
-        <v>-45.31</v>
+        <v>-53.95</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>8.710000000000001</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="F4" t="n">
         <v>-7.64</v>
       </c>
       <c r="G4" t="n">
-        <v>-26.07</v>
+        <v>-23.94</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>3.11</v>
+        <v>0.91</v>
       </c>
       <c r="I4" t="n">
-        <v>-53.57</v>
+        <v>-59.38</v>
       </c>
       <c r="J4" t="n">
-        <v>-8.76</v>
+        <v>-4.12</v>
       </c>
       <c r="K4" t="n">
-        <v>-11.1</v>
+        <v>-10.19</v>
       </c>
       <c r="L4" t="n">
-        <v>-44.47</v>
+        <v>-33</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>7.1</v>
+        <v>2.72</v>
       </c>
       <c r="N4" t="n">
         <v>-100</v>
       </c>
-      <c r="O4" s="2" t="n">
-        <v>0.52</v>
+      <c r="O4" t="n">
+        <v>-1.19</v>
       </c>
       <c r="P4" t="n">
-        <v>-33.56</v>
+        <v>-25.26</v>
       </c>
       <c r="Q4" s="2" t="n">
-        <v>12.26</v>
+        <v>1.65</v>
       </c>
       <c r="R4" s="2" t="n">
-        <v>9.59</v>
+        <v>12</v>
       </c>
       <c r="S4" t="n">
-        <v>-10.3</v>
+        <v>-5.93</v>
       </c>
       <c r="T4" s="2" t="n">
-        <v>7.33</v>
+        <v>8.5</v>
       </c>
       <c r="U4" t="n">
-        <v>-0.93</v>
+        <v>-3.53</v>
       </c>
       <c r="V4" t="n">
         <v>-70</v>
       </c>
       <c r="W4" t="n">
-        <v>-6.71</v>
+        <v>-4.71</v>
       </c>
       <c r="X4" t="n">
-        <v>-6.29</v>
+        <v>-2.23</v>
       </c>
       <c r="Y4" t="n">
         <v>-21.55</v>
       </c>
       <c r="Z4" t="n">
-        <v>-80</v>
+        <v>-74</v>
       </c>
       <c r="AA4" t="n">
-        <v>-6.71</v>
+        <v>-12.77</v>
       </c>
       <c r="AB4" s="2" t="n">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
@@ -839,77 +839,77 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-22.29</v>
+        <v>-22.69</v>
       </c>
       <c r="C5" t="n">
         <v>-100</v>
       </c>
       <c r="D5" t="n">
-        <v>-22.92</v>
+        <v>-17.67</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.96</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-1.95</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>2.19</v>
+        <v>-4.39</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>2.31</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-5.7</v>
       </c>
       <c r="H5" t="n">
-        <v>-9.41</v>
+        <v>-4.65</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="J5" t="n">
-        <v>-16.65</v>
+        <v>-3.96</v>
       </c>
       <c r="K5" t="n">
-        <v>-9.27</v>
+        <v>-12.17</v>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
-        <v>-7.01</v>
+        <v>-4.46</v>
       </c>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>-0.89</v>
+        <v>-1.31</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>2.2</v>
+        <v>0.31</v>
       </c>
       <c r="Q5" t="n">
-        <v>-19.11</v>
+        <v>-20.74</v>
       </c>
       <c r="R5" t="n">
-        <v>-2</v>
+        <v>-17.08</v>
       </c>
       <c r="S5" s="2" t="n">
-        <v>24.03</v>
+        <v>4.38</v>
       </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="n">
-        <v>-1.66</v>
+        <v>-6.77</v>
       </c>
       <c r="V5" t="inlineStr"/>
       <c r="W5" s="2" t="n">
-        <v>15.28</v>
+        <v>6.48</v>
       </c>
       <c r="X5" t="n">
-        <v>-7.11</v>
+        <v>-1.29</v>
       </c>
       <c r="Y5" s="2" t="n">
-        <v>97.8</v>
+        <v>41.29</v>
       </c>
       <c r="Z5" t="n">
         <v>-100</v>
       </c>
       <c r="AA5" t="n">
-        <v>-8.84</v>
+        <v>-9.69</v>
       </c>
       <c r="AB5" s="2" t="n">
-        <v>80</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6">
@@ -919,83 +919,83 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>7.11</v>
+        <v>7.81</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>75</v>
       </c>
       <c r="D6" t="n">
-        <v>-71.75</v>
+        <v>-57.17</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>17.14</v>
+        <v>10.53</v>
       </c>
       <c r="F6" t="n">
-        <v>-26.92</v>
+        <v>-22.62</v>
       </c>
       <c r="G6" t="n">
-        <v>-16.64</v>
+        <v>-11.25</v>
       </c>
       <c r="H6" t="n">
-        <v>-1.63</v>
+        <v>-1.24</v>
       </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="n">
-        <v>-14.3</v>
+        <v>-9.970000000000001</v>
       </c>
       <c r="K6" t="n">
-        <v>-21.7</v>
+        <v>-2</v>
       </c>
       <c r="L6" s="2" t="n">
         <v>0.44</v>
       </c>
       <c r="M6" t="n">
-        <v>-16.39</v>
+        <v>-10</v>
       </c>
       <c r="N6" s="2" t="n">
         <v>33.33</v>
       </c>
       <c r="O6" t="n">
-        <v>-4.92</v>
+        <v>-1.7</v>
       </c>
       <c r="P6" s="2" t="n">
-        <v>8.640000000000001</v>
+        <v>7.15</v>
       </c>
       <c r="Q6" t="n">
-        <v>-11.75</v>
+        <v>-1.62</v>
       </c>
       <c r="R6" s="2" t="n">
-        <v>52.19</v>
+        <v>45.28</v>
       </c>
       <c r="S6" t="n">
-        <v>-14.38</v>
+        <v>-5</v>
       </c>
       <c r="T6" t="n">
-        <v>-100</v>
+        <v>-64.44</v>
       </c>
       <c r="U6" s="2" t="n">
-        <v>15.41</v>
+        <v>11.96</v>
       </c>
       <c r="V6" t="n">
         <v>-24.25</v>
       </c>
       <c r="W6" t="n">
-        <v>-5.64</v>
+        <v>-0.19</v>
       </c>
       <c r="X6" s="2" t="n">
-        <v>2.71</v>
+        <v>0.52</v>
       </c>
       <c r="Y6" s="2" t="n">
         <v>50</v>
       </c>
       <c r="Z6" s="2" t="n">
-        <v>16.06</v>
+        <v>23.79</v>
       </c>
       <c r="AA6" s="2" t="n">
-        <v>2.18</v>
+        <v>11.19</v>
       </c>
       <c r="AB6" s="2" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7">
@@ -1005,85 +1005,85 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-14.24</v>
+        <v>-1.63</v>
       </c>
       <c r="C7" t="n">
-        <v>-26</v>
+        <v>-8.33</v>
       </c>
       <c r="D7" t="n">
-        <v>-34.83</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
+        <v>-35.97</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>3.41</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>25.33</v>
+        <v>24.29</v>
       </c>
       <c r="G7" t="n">
-        <v>-9.880000000000001</v>
+        <v>-7.11</v>
       </c>
       <c r="H7" t="n">
-        <v>-6.58</v>
+        <v>-4.43</v>
       </c>
       <c r="I7" t="n">
         <v>-100</v>
       </c>
       <c r="J7" t="n">
-        <v>-10.21</v>
+        <v>-5.17</v>
       </c>
       <c r="K7" t="n">
-        <v>-8.800000000000001</v>
+        <v>-1.79</v>
       </c>
       <c r="L7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="M7" s="2" t="n">
-        <v>0.35</v>
+        <v>-23.78</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-4.57</v>
       </c>
       <c r="N7" t="n">
         <v>-100</v>
       </c>
-      <c r="O7" s="2" t="n">
-        <v>0.9399999999999999</v>
+      <c r="O7" t="n">
+        <v>-2.73</v>
       </c>
       <c r="P7" s="2" t="n">
-        <v>5.5</v>
+        <v>9.31</v>
       </c>
       <c r="Q7" t="n">
-        <v>-17.87</v>
+        <v>-17.32</v>
       </c>
       <c r="R7" t="n">
-        <v>-54.3</v>
+        <v>-29.5</v>
       </c>
       <c r="S7" s="2" t="n">
-        <v>13.83</v>
+        <v>14.58</v>
       </c>
       <c r="T7" s="2" t="n">
-        <v>45.92</v>
+        <v>24.25</v>
       </c>
       <c r="U7" t="n">
-        <v>-18.33</v>
+        <v>-4.4</v>
       </c>
       <c r="V7" s="2" t="n">
-        <v>22.83</v>
+        <v>27.14</v>
       </c>
       <c r="W7" t="n">
-        <v>-5.1</v>
+        <v>-15.79</v>
       </c>
       <c r="X7" t="n">
-        <v>-4.65</v>
+        <v>-0.83</v>
       </c>
       <c r="Y7" t="n">
-        <v>-40</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>-16.13</v>
+        <v>-14.29</v>
+      </c>
+      <c r="Z7" s="2" t="n">
+        <v>3.38</v>
       </c>
       <c r="AA7" s="2" t="n">
-        <v>1.77</v>
+        <v>3.11</v>
       </c>
       <c r="AB7" s="2" t="n">
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8">
@@ -1093,83 +1093,83 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-8.789999999999999</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-2.65</v>
+        <v>-9.68</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>-52.54</v>
+        <v>-37.19</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>4.47</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>8.83</v>
+        <v>5.18</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-2.12</v>
       </c>
       <c r="G8" t="n">
-        <v>-10.68</v>
+        <v>-2.97</v>
       </c>
       <c r="H8" t="n">
-        <v>-14.66</v>
+        <v>-13.96</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>44.2</v>
+        <v>29.63</v>
       </c>
       <c r="J8" t="n">
-        <v>-23.58</v>
+        <v>-19.54</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>5.63</v>
+        <v>7.95</v>
       </c>
       <c r="L8" t="n">
-        <v>-81.69</v>
+        <v>-83</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.16</v>
+        <v>-1.05</v>
       </c>
       <c r="N8" t="n">
         <v>-100</v>
       </c>
       <c r="O8" s="2" t="n">
-        <v>0.9399999999999999</v>
+        <v>2.61</v>
       </c>
       <c r="P8" t="n">
-        <v>-17.97</v>
-      </c>
-      <c r="Q8" s="2" t="n">
-        <v>7.24</v>
+        <v>-21.34</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
       </c>
       <c r="R8" s="2" t="n">
-        <v>13.62</v>
+        <v>10.46</v>
       </c>
       <c r="S8" t="n">
-        <v>-16.98</v>
+        <v>-13.07</v>
       </c>
       <c r="T8" t="n">
-        <v>-100</v>
+        <v>-77.27</v>
       </c>
       <c r="U8" t="n">
-        <v>-9.25</v>
+        <v>-7.95</v>
       </c>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="n">
-        <v>-21.5</v>
+        <v>-13.63</v>
       </c>
       <c r="X8" t="n">
-        <v>-12.57</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>-6.29</v>
+        <v>-9.779999999999999</v>
+      </c>
+      <c r="Y8" s="2" t="n">
+        <v>15.94</v>
       </c>
       <c r="Z8" s="2" t="n">
-        <v>26.18</v>
+        <v>15.67</v>
       </c>
       <c r="AA8" s="2" t="n">
-        <v>1.61</v>
+        <v>1.3</v>
       </c>
       <c r="AB8" s="2" t="n">
-        <v>101</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9">
@@ -1179,85 +1179,85 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>22.57</v>
+        <v>20.36</v>
       </c>
       <c r="C9" t="n">
         <v>-2</v>
       </c>
       <c r="D9" t="n">
-        <v>-13.15</v>
+        <v>-12.77</v>
       </c>
       <c r="E9" t="n">
-        <v>-9.279999999999999</v>
+        <v>-10.78</v>
       </c>
       <c r="F9" t="n">
-        <v>-3.22</v>
+        <v>-2.42</v>
       </c>
       <c r="G9" t="n">
-        <v>-9.41</v>
+        <v>-9.970000000000001</v>
       </c>
       <c r="H9" t="n">
-        <v>-5.34</v>
+        <v>-5.49</v>
       </c>
       <c r="I9" t="n">
-        <v>-4.93</v>
+        <v>-10.88</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>6.27</v>
+        <v>8.19</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>17.09</v>
+        <v>10.46</v>
       </c>
       <c r="L9" t="n">
-        <v>-35.11</v>
+        <v>-41.29</v>
       </c>
       <c r="M9" t="n">
-        <v>-5.41</v>
+        <v>-3.57</v>
       </c>
       <c r="N9" t="n">
         <v>-58.33</v>
       </c>
       <c r="O9" t="n">
-        <v>-7.54</v>
-      </c>
-      <c r="P9" t="n">
-        <v>-1.51</v>
+        <v>-5.44</v>
+      </c>
+      <c r="P9" s="2" t="n">
+        <v>0.65</v>
       </c>
       <c r="Q9" s="2" t="n">
-        <v>8.369999999999999</v>
+        <v>6.52</v>
       </c>
       <c r="R9" t="n">
-        <v>-5.16</v>
+        <v>-13.53</v>
       </c>
       <c r="S9" t="n">
-        <v>-28</v>
-      </c>
-      <c r="T9" s="2" t="n">
-        <v>11.5</v>
+        <v>-27.02</v>
+      </c>
+      <c r="T9" t="n">
+        <v>-0.03</v>
       </c>
       <c r="U9" t="n">
-        <v>-8.390000000000001</v>
+        <v>-6.22</v>
       </c>
       <c r="V9" s="2" t="n">
         <v>9</v>
       </c>
       <c r="W9" t="n">
-        <v>-6.79</v>
+        <v>-9.56</v>
       </c>
       <c r="X9" t="n">
-        <v>-1.02</v>
+        <v>-2.83</v>
       </c>
       <c r="Y9" t="n">
-        <v>-22.45</v>
+        <v>-13.46</v>
       </c>
       <c r="Z9" t="n">
-        <v>-3.17</v>
+        <v>-7.56</v>
       </c>
       <c r="AA9" t="n">
-        <v>-3.44</v>
+        <v>-5.1</v>
       </c>
       <c r="AB9" s="2" t="n">
-        <v>110</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10">
@@ -1267,85 +1267,85 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-41.3</v>
+        <v>-37.42</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>118.33</v>
       </c>
       <c r="D10" t="n">
-        <v>-5.12</v>
+        <v>-3.04</v>
       </c>
       <c r="E10" t="n">
-        <v>-22.5</v>
+        <v>-13.24</v>
       </c>
       <c r="F10" t="n">
-        <v>-12.83</v>
+        <v>-9.300000000000001</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.5</v>
+        <v>-1.08</v>
       </c>
       <c r="H10" t="n">
-        <v>-17.24</v>
-      </c>
-      <c r="I10" t="n">
-        <v>-10.44</v>
+        <v>-11.86</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0.47</v>
       </c>
       <c r="J10" t="n">
-        <v>-19.87</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>5.24</v>
+        <v>-12.1</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-1.64</v>
       </c>
       <c r="L10" s="2" t="n">
         <v>9.58</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>6.96</v>
+        <v>1.82</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>116.67</v>
       </c>
       <c r="O10" s="2" t="n">
-        <v>4.79</v>
+        <v>2.72</v>
       </c>
       <c r="P10" t="n">
-        <v>-27.53</v>
+        <v>-18.22</v>
       </c>
       <c r="Q10" t="n">
-        <v>-13.62</v>
+        <v>-14.07</v>
       </c>
       <c r="R10" t="n">
-        <v>-26.88</v>
+        <v>-25.7</v>
       </c>
       <c r="S10" t="n">
-        <v>-12.18</v>
+        <v>-6.7</v>
       </c>
       <c r="T10" t="n">
-        <v>-52.31</v>
+        <v>-58.67</v>
       </c>
       <c r="U10" t="n">
-        <v>-18.27</v>
+        <v>-16.22</v>
       </c>
       <c r="V10" t="n">
-        <v>-33.14</v>
+        <v>-26.8</v>
       </c>
       <c r="W10" t="n">
-        <v>-17.1</v>
+        <v>-21.17</v>
       </c>
       <c r="X10" t="n">
-        <v>-13.22</v>
+        <v>-12.39</v>
       </c>
       <c r="Y10" t="n">
-        <v>-33.25</v>
+        <v>-12.4</v>
       </c>
       <c r="Z10" t="n">
-        <v>-23.53</v>
-      </c>
-      <c r="AA10" s="2" t="n">
-        <v>1.47</v>
+        <v>-13.17</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>-2.43</v>
       </c>
       <c r="AB10" s="2" t="n">
-        <v>94</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11">
@@ -1355,85 +1355,85 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-16.59</v>
+        <v>-10.94</v>
       </c>
       <c r="C11" t="n">
         <v>-100</v>
       </c>
       <c r="D11" t="n">
-        <v>-17.7</v>
+        <v>-24.56</v>
       </c>
       <c r="E11" t="n">
-        <v>-3.33</v>
+        <v>-1.73</v>
       </c>
       <c r="F11" t="n">
-        <v>-4.68</v>
+        <v>-11.89</v>
       </c>
       <c r="G11" t="n">
-        <v>-18.61</v>
+        <v>-15</v>
       </c>
       <c r="H11" t="n">
-        <v>-2.37</v>
+        <v>-2.34</v>
       </c>
       <c r="I11" t="n">
         <v>-59.38</v>
       </c>
       <c r="J11" t="n">
-        <v>-1.85</v>
+        <v>-6.02</v>
       </c>
       <c r="K11" t="n">
-        <v>-27.94</v>
+        <v>-28.84</v>
       </c>
       <c r="L11" t="n">
-        <v>-53.36</v>
+        <v>-60.54</v>
       </c>
       <c r="M11" t="n">
-        <v>-12</v>
+        <v>-12.68</v>
       </c>
       <c r="N11" t="n">
         <v>-100</v>
       </c>
       <c r="O11" t="n">
-        <v>-2.16</v>
+        <v>-2.9</v>
       </c>
       <c r="P11" t="n">
-        <v>-8.1</v>
+        <v>-13.5</v>
       </c>
       <c r="Q11" t="n">
-        <v>-26.38</v>
+        <v>-28.37</v>
       </c>
       <c r="R11" s="2" t="n">
-        <v>1.82</v>
+        <v>2.8</v>
       </c>
       <c r="S11" t="n">
-        <v>-21.12</v>
-      </c>
-      <c r="T11" s="2" t="n">
-        <v>10.8</v>
+        <v>-19.7</v>
+      </c>
+      <c r="T11" t="n">
+        <v>-1.07</v>
       </c>
       <c r="U11" t="n">
-        <v>-8.85</v>
+        <v>-7.25</v>
       </c>
       <c r="V11" t="n">
         <v>-33</v>
       </c>
       <c r="W11" t="n">
-        <v>-14.23</v>
+        <v>-9.359999999999999</v>
       </c>
       <c r="X11" t="n">
-        <v>-1.55</v>
+        <v>-3.88</v>
       </c>
       <c r="Y11" t="n">
-        <v>-53.08</v>
+        <v>-56.69</v>
       </c>
       <c r="Z11" t="n">
         <v>-39</v>
       </c>
       <c r="AA11" t="n">
-        <v>-8.85</v>
+        <v>-8.41</v>
       </c>
       <c r="AB11" s="2" t="n">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12">
@@ -1442,84 +1442,86 @@
           <t>France</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>-6.47</v>
+      <c r="B12" s="2" t="n">
+        <v>8.4</v>
       </c>
       <c r="C12" t="n">
         <v>-34</v>
       </c>
       <c r="D12" t="n">
-        <v>-4.53</v>
+        <v>-0.65</v>
       </c>
       <c r="E12" t="n">
-        <v>-9.69</v>
+        <v>-9</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>6.83</v>
+        <v>7.58</v>
       </c>
       <c r="G12" t="n">
-        <v>-20.15</v>
+        <v>-17.29</v>
       </c>
       <c r="H12" t="n">
-        <v>-3.1</v>
+        <v>-2.31</v>
       </c>
       <c r="I12" t="n">
         <v>-100</v>
       </c>
       <c r="J12" t="n">
-        <v>-17.17</v>
+        <v>-6.46</v>
       </c>
       <c r="K12" t="n">
-        <v>-15.48</v>
+        <v>-0.52</v>
       </c>
       <c r="L12" t="n">
-        <v>-32.29</v>
+        <v>-26.45</v>
       </c>
       <c r="M12" t="n">
-        <v>-5.43</v>
+        <v>-4.67</v>
       </c>
       <c r="N12" t="n">
         <v>-38.14</v>
       </c>
       <c r="O12" s="2" t="n">
-        <v>4.71</v>
+        <v>3.62</v>
       </c>
       <c r="P12" t="n">
-        <v>-29.29</v>
+        <v>-28.43</v>
       </c>
       <c r="Q12" t="n">
-        <v>-27.79</v>
+        <v>-12.58</v>
       </c>
       <c r="R12" t="n">
-        <v>-13.91</v>
+        <v>-10.46</v>
       </c>
       <c r="S12" t="n">
-        <v>-47.94</v>
+        <v>-39.64</v>
       </c>
       <c r="T12" t="n">
-        <v>-39.62</v>
+        <v>-15.83</v>
       </c>
       <c r="U12" t="n">
-        <v>-24.26</v>
-      </c>
-      <c r="V12" t="inlineStr"/>
+        <v>-17.05</v>
+      </c>
+      <c r="V12" s="2" t="n">
+        <v>53</v>
+      </c>
       <c r="W12" t="n">
-        <v>-26.41</v>
-      </c>
-      <c r="X12" s="2" t="n">
-        <v>2.02</v>
+        <v>-25.32</v>
+      </c>
+      <c r="X12" t="n">
+        <v>-0.48</v>
       </c>
       <c r="Y12" t="n">
         <v>-100</v>
       </c>
-      <c r="Z12" t="n">
-        <v>-3.39</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>-0.68</v>
+      <c r="Z12" s="2" t="n">
+        <v>17.14</v>
+      </c>
+      <c r="AA12" s="2" t="n">
+        <v>1.35</v>
       </c>
       <c r="AB12" s="2" t="n">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
@@ -1529,85 +1531,85 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>21.13</v>
+        <v>24.42</v>
       </c>
       <c r="C13" t="n">
         <v>-100</v>
       </c>
       <c r="D13" t="n">
-        <v>-57.19</v>
+        <v>-51.34</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>-2.09</v>
       </c>
       <c r="F13" t="n">
-        <v>-6.49</v>
+        <v>-7.04</v>
       </c>
       <c r="G13" t="n">
-        <v>-65.91</v>
+        <v>-53</v>
       </c>
       <c r="H13" t="n">
-        <v>-8</v>
-      </c>
-      <c r="I13" s="2" t="n">
-        <v>5.25</v>
+        <v>-9.470000000000001</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-2.85</v>
       </c>
       <c r="J13" t="n">
-        <v>-14.3</v>
+        <v>-21.44</v>
       </c>
       <c r="K13" t="n">
-        <v>-19.39</v>
+        <v>-10.61</v>
       </c>
       <c r="L13" s="2" t="n">
         <v>31.43</v>
       </c>
-      <c r="M13" t="n">
-        <v>-1.6</v>
+      <c r="M13" s="2" t="n">
+        <v>1.51</v>
       </c>
       <c r="N13" t="n">
         <v>-100</v>
       </c>
       <c r="O13" t="n">
-        <v>-3.2</v>
+        <v>-2.04</v>
       </c>
       <c r="P13" t="n">
-        <v>-42.59</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>-1.47</v>
+        <v>-47.38</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <v>5.89</v>
       </c>
       <c r="R13" s="2" t="n">
-        <v>20.43</v>
+        <v>29.1</v>
       </c>
       <c r="S13" t="n">
-        <v>-24.92</v>
+        <v>-14.41</v>
       </c>
       <c r="T13" t="n">
-        <v>-59.5</v>
+        <v>-61</v>
       </c>
       <c r="U13" s="2" t="n">
-        <v>4.88</v>
+        <v>7.03</v>
       </c>
       <c r="V13" t="n">
         <v>-3.12</v>
       </c>
       <c r="W13" t="n">
-        <v>-13.15</v>
-      </c>
-      <c r="X13" s="2" t="n">
-        <v>1.85</v>
+        <v>-8.960000000000001</v>
+      </c>
+      <c r="X13" t="n">
+        <v>-3.51</v>
       </c>
       <c r="Y13" t="n">
         <v>-24.93</v>
       </c>
       <c r="Z13" t="n">
-        <v>-7.06</v>
+        <v>-12.22</v>
       </c>
       <c r="AA13" t="n">
-        <v>-8.789999999999999</v>
+        <v>-4.43</v>
       </c>
       <c r="AB13" s="2" t="n">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14">
@@ -1617,83 +1619,83 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-9.67</v>
+        <v>-0.83</v>
       </c>
       <c r="C14" t="n">
-        <v>-49.62</v>
+        <v>-61.47</v>
       </c>
       <c r="D14" t="n">
-        <v>-10</v>
+        <v>-12.72</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>2.96</v>
+        <v>2.85</v>
       </c>
       <c r="F14" t="n">
-        <v>-37.25</v>
+        <v>-49.8</v>
       </c>
       <c r="G14" t="n">
-        <v>-19.33</v>
+        <v>-11.53</v>
       </c>
       <c r="H14" t="n">
-        <v>-11.62</v>
+        <v>-7.68</v>
       </c>
       <c r="I14" t="n">
         <v>-8.33</v>
       </c>
       <c r="J14" t="n">
-        <v>-4.47</v>
+        <v>-10.9</v>
       </c>
       <c r="K14" s="2" t="n">
-        <v>29.27</v>
+        <v>2.05</v>
       </c>
       <c r="L14" t="n">
-        <v>-16.14</v>
+        <v>-22.64</v>
       </c>
       <c r="M14" t="n">
-        <v>-6.62</v>
+        <v>-14.89</v>
       </c>
       <c r="N14" t="n">
-        <v>-75.56</v>
+        <v>-78</v>
       </c>
       <c r="O14" t="n">
-        <v>-6.59</v>
+        <v>-8</v>
       </c>
       <c r="P14" s="2" t="n">
-        <v>4.84</v>
+        <v>1.36</v>
       </c>
       <c r="Q14" s="2" t="n">
-        <v>32.41</v>
+        <v>7.19</v>
       </c>
       <c r="R14" t="n">
-        <v>-44.7</v>
+        <v>-26.77</v>
       </c>
       <c r="S14" t="n">
-        <v>-17.54</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="T14" s="2" t="n">
-        <v>19.7</v>
+        <v>27.85</v>
       </c>
       <c r="U14" t="n">
-        <v>-1.42</v>
+        <v>-0.73</v>
       </c>
       <c r="V14" t="inlineStr"/>
       <c r="W14" s="2" t="n">
-        <v>5.71</v>
+        <v>6.26</v>
       </c>
       <c r="X14" t="n">
-        <v>-10.71</v>
+        <v>-7.13</v>
       </c>
       <c r="Y14" t="n">
-        <v>-52.5</v>
+        <v>-55.67</v>
       </c>
       <c r="Z14" t="n">
-        <v>-25.18</v>
+        <v>-22.94</v>
       </c>
       <c r="AA14" t="n">
-        <v>-26.19</v>
+        <v>-18.38</v>
       </c>
       <c r="AB14" s="2" t="n">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
@@ -1703,85 +1705,85 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-31.19</v>
+        <v>-33.18</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>75</v>
       </c>
-      <c r="D15" t="n">
-        <v>-8</v>
+      <c r="D15" s="2" t="n">
+        <v>9.369999999999999</v>
       </c>
       <c r="E15" t="n">
-        <v>-5.86</v>
+        <v>-8.4</v>
       </c>
       <c r="F15" t="n">
-        <v>-9.789999999999999</v>
+        <v>-9.140000000000001</v>
       </c>
       <c r="G15" t="n">
-        <v>-22.45</v>
+        <v>-18.04</v>
       </c>
       <c r="H15" t="n">
-        <v>-6.59</v>
+        <v>-5.83</v>
       </c>
       <c r="I15" t="n">
         <v>-100</v>
       </c>
-      <c r="J15" t="n">
-        <v>-5.38</v>
+      <c r="J15" s="2" t="n">
+        <v>3.27</v>
       </c>
       <c r="K15" t="n">
-        <v>-24.36</v>
+        <v>-23.53</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>9.220000000000001</v>
+        <v>18.28</v>
       </c>
       <c r="M15" t="n">
-        <v>-15.08</v>
+        <v>-17.59</v>
       </c>
       <c r="N15" t="n">
         <v>-6.25</v>
       </c>
       <c r="O15" t="n">
-        <v>-2.09</v>
+        <v>-1.71</v>
       </c>
       <c r="P15" s="2" t="n">
-        <v>3.36</v>
+        <v>5.19</v>
       </c>
       <c r="Q15" s="2" t="n">
-        <v>14.22</v>
+        <v>4.79</v>
       </c>
       <c r="R15" t="n">
-        <v>-5.23</v>
+        <v>-9.33</v>
       </c>
       <c r="S15" s="2" t="n">
-        <v>17.59</v>
+        <v>11.02</v>
       </c>
       <c r="T15" t="n">
-        <v>-34.07</v>
-      </c>
-      <c r="U15" t="n">
-        <v>-0.42</v>
+        <v>-13.35</v>
+      </c>
+      <c r="U15" s="2" t="n">
+        <v>0.73</v>
       </c>
       <c r="V15" s="2" t="n">
         <v>21.2</v>
       </c>
       <c r="W15" t="n">
-        <v>-5.84</v>
+        <v>-2.65</v>
       </c>
       <c r="X15" t="n">
-        <v>-4.41</v>
+        <v>-2.04</v>
       </c>
       <c r="Y15" t="n">
-        <v>-73.84999999999999</v>
+        <v>-77.33</v>
       </c>
       <c r="Z15" s="2" t="n">
-        <v>17.26</v>
+        <v>11.46</v>
       </c>
       <c r="AA15" t="n">
-        <v>-9.85</v>
+        <v>-14.11</v>
       </c>
       <c r="AB15" s="2" t="n">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16">
@@ -1791,85 +1793,85 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-8.33</v>
+        <v>-12.88</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>32.92</v>
+        <v>22.69</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>54.61</v>
+        <v>52.96</v>
       </c>
       <c r="E16" t="n">
-        <v>-32.6</v>
+        <v>-24.08</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>34.14</v>
+        <v>32.6</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>11.48</v>
-      </c>
-      <c r="H16" t="n">
-        <v>-1.25</v>
-      </c>
-      <c r="I16" t="n">
-        <v>-17.12</v>
+        <v>10.11</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>22.6</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>46.07</v>
+        <v>48.71</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>11.06</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>100</v>
+        <v>112.6</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>3.25</v>
+        <v>2.32</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>800</v>
       </c>
       <c r="O16" t="n">
-        <v>-1.06</v>
+        <v>-1.93</v>
       </c>
       <c r="P16" s="2" t="n">
-        <v>29.59</v>
+        <v>36.09</v>
       </c>
       <c r="Q16" t="n">
-        <v>-18.52</v>
+        <v>-16.6</v>
       </c>
       <c r="R16" t="n">
-        <v>-31.44</v>
+        <v>-5.23</v>
       </c>
       <c r="S16" s="2" t="n">
-        <v>12.16</v>
+        <v>7.24</v>
       </c>
       <c r="T16" t="n">
         <v>-6.71</v>
       </c>
       <c r="U16" t="n">
-        <v>-24.81</v>
+        <v>-18.03</v>
       </c>
       <c r="V16" s="2" t="n">
         <v>40</v>
       </c>
       <c r="W16" s="2" t="n">
-        <v>6.29</v>
+        <v>1.41</v>
       </c>
       <c r="X16" s="2" t="n">
-        <v>5.04</v>
+        <v>5.9</v>
       </c>
       <c r="Y16" t="n">
-        <v>-43.7</v>
+        <v>-46.38</v>
       </c>
       <c r="Z16" s="2" t="n">
-        <v>5.91</v>
+        <v>25.42</v>
       </c>
       <c r="AA16" t="n">
-        <v>-9.59</v>
+        <v>-11.64</v>
       </c>
       <c r="AB16" s="2" t="n">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17">
@@ -1879,85 +1881,85 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>6.77</v>
+        <v>7.71</v>
       </c>
       <c r="C17" t="n">
-        <v>-28.57</v>
+        <v>-33.33</v>
       </c>
       <c r="D17" t="n">
-        <v>-8.539999999999999</v>
+        <v>-8.880000000000001</v>
       </c>
       <c r="E17" t="n">
-        <v>-10.3</v>
+        <v>-12.92</v>
       </c>
       <c r="F17" t="n">
-        <v>-37.67</v>
-      </c>
-      <c r="G17" t="n">
-        <v>-4.66</v>
+        <v>-20.5</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>1.41</v>
       </c>
       <c r="H17" t="n">
-        <v>-8.1</v>
+        <v>-7.17</v>
       </c>
       <c r="I17" t="n">
         <v>-43.33</v>
       </c>
       <c r="J17" t="n">
-        <v>-3.95</v>
+        <v>-6.42</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.74</v>
+        <v>-6.02</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>9.69</v>
+        <v>4.44</v>
       </c>
       <c r="M17" t="n">
-        <v>-6.48</v>
+        <v>-6.64</v>
       </c>
       <c r="N17" s="2" t="n">
         <v>211</v>
       </c>
       <c r="O17" t="n">
-        <v>-9.869999999999999</v>
+        <v>-7.61</v>
       </c>
       <c r="P17" t="n">
-        <v>-1.14</v>
+        <v>-0.64</v>
       </c>
       <c r="Q17" t="n">
-        <v>-5.52</v>
+        <v>-6.21</v>
       </c>
       <c r="R17" t="n">
-        <v>-34.04</v>
+        <v>-28.69</v>
       </c>
       <c r="S17" t="n">
-        <v>-0.71</v>
+        <v>-11.09</v>
       </c>
       <c r="T17" s="2" t="n">
-        <v>47.79</v>
+        <v>32.62</v>
       </c>
       <c r="U17" t="n">
-        <v>-6.38</v>
+        <v>-7.76</v>
       </c>
       <c r="V17" t="n">
         <v>-100</v>
       </c>
       <c r="W17" s="2" t="n">
-        <v>7.06</v>
+        <v>0.09</v>
       </c>
       <c r="X17" t="n">
-        <v>-7.53</v>
+        <v>-5.34</v>
       </c>
       <c r="Y17" t="n">
-        <v>-75</v>
+        <v>-61.42</v>
       </c>
       <c r="Z17" t="n">
-        <v>-35.8</v>
+        <v>-36.16</v>
       </c>
       <c r="AA17" t="n">
-        <v>-15.53</v>
+        <v>-11.27</v>
       </c>
       <c r="AB17" s="2" t="n">
-        <v>79</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18">
@@ -1967,85 +1969,85 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-19.25</v>
+        <v>-16</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>5.4</v>
+        <v>14.55</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.88</v>
       </c>
       <c r="E18" t="n">
-        <v>-1.39</v>
+        <v>-1.6</v>
       </c>
       <c r="F18" t="n">
-        <v>-17.54</v>
+        <v>-28.53</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>8.85</v>
+        <v>1.54</v>
       </c>
       <c r="H18" t="n">
-        <v>-14.32</v>
+        <v>-9</v>
       </c>
       <c r="I18" t="n">
-        <v>-18.33</v>
+        <v>-10.29</v>
       </c>
       <c r="J18" t="n">
-        <v>-26.92</v>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>0.87</v>
+        <v>-24.05</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-5.29</v>
       </c>
       <c r="L18" t="n">
         <v>-42.86</v>
       </c>
       <c r="M18" t="n">
-        <v>-4.12</v>
+        <v>-9.57</v>
       </c>
       <c r="N18" t="n">
         <v>-100</v>
       </c>
       <c r="O18" t="n">
-        <v>-1.88</v>
+        <v>-6.14</v>
       </c>
       <c r="P18" t="n">
-        <v>-18.74</v>
-      </c>
-      <c r="Q18" s="2" t="n">
-        <v>0.41</v>
+        <v>-15.24</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>-3.03</v>
       </c>
       <c r="R18" t="n">
-        <v>-24.62</v>
+        <v>-11.29</v>
       </c>
       <c r="S18" s="2" t="n">
-        <v>32.52</v>
+        <v>16.49</v>
       </c>
       <c r="T18" t="n">
         <v>-75</v>
       </c>
       <c r="U18" s="2" t="n">
-        <v>1.35</v>
+        <v>0.71</v>
       </c>
       <c r="V18" s="2" t="n">
         <v>28</v>
       </c>
       <c r="W18" t="n">
-        <v>-6.58</v>
+        <v>-5.48</v>
       </c>
       <c r="X18" t="n">
-        <v>-14.85</v>
+        <v>-7.1</v>
       </c>
       <c r="Y18" t="n">
-        <v>-15.56</v>
+        <v>-20.53</v>
       </c>
       <c r="Z18" s="2" t="n">
-        <v>71.31</v>
+        <v>39.19</v>
       </c>
       <c r="AA18" t="n">
-        <v>-6.47</v>
+        <v>-12.15</v>
       </c>
       <c r="AB18" s="2" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19">
@@ -2140,84 +2142,84 @@
           <t>Netherlands</t>
         </is>
       </c>
-      <c r="B20" s="2" t="n">
-        <v>5.81</v>
+      <c r="B20" t="n">
+        <v>-5.56</v>
       </c>
       <c r="C20" t="n">
         <v>-20</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>13.55</v>
+        <v>10.07</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.14</v>
-      </c>
-      <c r="F20" s="2" t="n">
-        <v>29</v>
+        <v>-1.63</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-3.25</v>
       </c>
       <c r="G20" t="n">
-        <v>-17.83</v>
+        <v>-19.4</v>
       </c>
       <c r="H20" t="n">
-        <v>-12.47</v>
+        <v>-13.36</v>
       </c>
       <c r="I20" t="n">
         <v>-100</v>
       </c>
       <c r="J20" t="n">
-        <v>-7.95</v>
+        <v>-16.92</v>
       </c>
       <c r="K20" t="n">
-        <v>-23.29</v>
+        <v>-17.3</v>
       </c>
       <c r="L20" t="n">
-        <v>-8</v>
+        <v>-4.29</v>
       </c>
       <c r="M20" s="2" t="n">
-        <v>8.66</v>
+        <v>9.51</v>
       </c>
       <c r="N20" t="n">
         <v>-100</v>
       </c>
       <c r="O20" t="n">
-        <v>-5</v>
+        <v>-3.86</v>
       </c>
       <c r="P20" t="n">
-        <v>-12.4</v>
+        <v>-1.41</v>
       </c>
       <c r="Q20" s="2" t="n">
-        <v>16.64</v>
+        <v>14.21</v>
       </c>
       <c r="R20" t="n">
-        <v>-1.47</v>
+        <v>-10.48</v>
       </c>
       <c r="S20" t="n">
-        <v>-25.83</v>
+        <v>-26</v>
       </c>
       <c r="T20" t="n">
-        <v>-48.38</v>
+        <v>-36.2</v>
       </c>
       <c r="U20" t="n">
-        <v>-5.57</v>
+        <v>-4.72</v>
       </c>
       <c r="V20" t="inlineStr"/>
       <c r="W20" t="n">
-        <v>-1.93</v>
+        <v>-6.41</v>
       </c>
       <c r="X20" t="n">
-        <v>-5.06</v>
+        <v>-6.27</v>
       </c>
       <c r="Y20" t="n">
         <v>-45</v>
       </c>
       <c r="Z20" t="n">
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="AA20" t="n">
-        <v>-10.19</v>
+        <v>-2.4</v>
       </c>
       <c r="AB20" s="2" t="n">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21">
@@ -2227,77 +2229,77 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>2</v>
+        <v>2.19</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" s="2" t="n">
-        <v>12.41</v>
+        <v>16.17</v>
       </c>
       <c r="E21" t="n">
-        <v>-7.09</v>
-      </c>
-      <c r="F21" t="n">
-        <v>-0.17</v>
+        <v>-6.25</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>1.12</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>19.33</v>
       </c>
       <c r="H21" t="n">
-        <v>-11.02</v>
+        <v>-11.15</v>
       </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" s="2" t="n">
-        <v>10.05</v>
+        <v>6.61</v>
       </c>
       <c r="K21" s="2" t="n">
-        <v>37.73</v>
+        <v>31.35</v>
       </c>
       <c r="L21" t="n">
-        <v>-19.8</v>
+        <v>-5.33</v>
       </c>
       <c r="M21" s="2" t="n">
-        <v>2.39</v>
+        <v>5.41</v>
       </c>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>-2.9</v>
+        <v>-2.07</v>
       </c>
       <c r="P21" t="n">
-        <v>-19.11</v>
+        <v>-19.35</v>
       </c>
       <c r="Q21" s="2" t="n">
-        <v>26.16</v>
+        <v>24.58</v>
       </c>
       <c r="R21" s="2" t="n">
-        <v>13.17</v>
+        <v>2.88</v>
       </c>
       <c r="S21" t="n">
-        <v>-18.82</v>
+        <v>-22.2</v>
       </c>
       <c r="T21" t="n">
-        <v>-23.33</v>
+        <v>-42.5</v>
       </c>
       <c r="U21" t="n">
-        <v>-8.34</v>
+        <v>-8.640000000000001</v>
       </c>
       <c r="V21" t="inlineStr"/>
       <c r="W21" t="n">
-        <v>-18.75</v>
+        <v>-11.64</v>
       </c>
       <c r="X21" t="n">
-        <v>-8.279999999999999</v>
+        <v>-9.52</v>
       </c>
       <c r="Y21" t="n">
         <v>-100</v>
       </c>
       <c r="Z21" s="2" t="n">
-        <v>43.33</v>
+        <v>7.5</v>
       </c>
       <c r="AA21" t="n">
-        <v>-9.460000000000001</v>
+        <v>-5.37</v>
       </c>
       <c r="AB21" s="2" t="n">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22">
@@ -2307,83 +2309,83 @@
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>2.26</v>
+        <v>1.18</v>
       </c>
       <c r="C22" t="n">
         <v>-100</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>34.17</v>
+        <v>20</v>
       </c>
       <c r="E22" t="n">
-        <v>-4</v>
+        <v>-2.72</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>13.88</v>
+        <v>1.85</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>5</v>
+        <v>5.79</v>
       </c>
       <c r="H22" t="n">
-        <v>-7.1</v>
+        <v>-11.94</v>
       </c>
       <c r="I22" t="n">
-        <v>-8.699999999999999</v>
+        <v>-17</v>
       </c>
       <c r="J22" t="n">
-        <v>-10.39</v>
-      </c>
-      <c r="K22" s="2" t="n">
-        <v>0.71</v>
+        <v>-28.93</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-3.15</v>
       </c>
       <c r="L22" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="M22" t="n">
-        <v>-0.71</v>
+      <c r="M22" s="2" t="n">
+        <v>1.14</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>75</v>
       </c>
       <c r="O22" t="n">
-        <v>-1.25</v>
+        <v>-1.46</v>
       </c>
       <c r="P22" t="n">
-        <v>-34.85</v>
+        <v>-31.46</v>
       </c>
       <c r="Q22" t="n">
-        <v>-6.88</v>
+        <v>-8.34</v>
       </c>
       <c r="R22" t="n">
-        <v>-37</v>
+        <v>-47.5</v>
       </c>
       <c r="S22" t="n">
-        <v>-27.65</v>
+        <v>-24.37</v>
       </c>
       <c r="T22" t="n">
-        <v>-100</v>
+        <v>-34.25</v>
       </c>
       <c r="U22" t="n">
-        <v>-14.27</v>
+        <v>-9.58</v>
       </c>
       <c r="V22" t="inlineStr"/>
       <c r="W22" t="n">
-        <v>-13.68</v>
+        <v>-15.63</v>
       </c>
       <c r="X22" s="2" t="n">
-        <v>4</v>
+        <v>2.33</v>
       </c>
       <c r="Y22" t="n">
-        <v>-18.71</v>
+        <v>-6.6</v>
       </c>
       <c r="Z22" t="n">
         <v>-12.78</v>
       </c>
       <c r="AA22" t="n">
-        <v>-6.17</v>
+        <v>-6.42</v>
       </c>
       <c r="AB22" s="2" t="n">
-        <v>61</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23">
@@ -2393,83 +2395,83 @@
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>5.48</v>
-      </c>
-      <c r="C23" t="n">
-        <v>-30</v>
+        <v>11.88</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>42.86</v>
       </c>
       <c r="D23" t="n">
-        <v>-31.19</v>
+        <v>-41.62</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>6.36</v>
+        <v>6.3</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>16.14</v>
+        <v>19</v>
       </c>
       <c r="G23" t="n">
-        <v>-2.41</v>
+        <v>-5.95</v>
       </c>
       <c r="H23" t="n">
-        <v>-12.11</v>
+        <v>-9.640000000000001</v>
       </c>
       <c r="I23" t="n">
-        <v>-38.64</v>
-      </c>
-      <c r="J23" s="2" t="n">
-        <v>2.18</v>
+        <v>-28.57</v>
+      </c>
+      <c r="J23" t="n">
+        <v>-6.87</v>
       </c>
       <c r="K23" t="n">
-        <v>-10.9</v>
+        <v>-9.869999999999999</v>
       </c>
       <c r="L23" t="n">
-        <v>-39.33</v>
+        <v>-54.5</v>
       </c>
       <c r="M23" t="n">
-        <v>-6.2</v>
+        <v>-2.02</v>
       </c>
       <c r="N23" t="n">
         <v>-100</v>
       </c>
       <c r="O23" t="n">
-        <v>-8.77</v>
-      </c>
-      <c r="P23" t="n">
-        <v>-7.43</v>
+        <v>-5.46</v>
+      </c>
+      <c r="P23" s="2" t="n">
+        <v>4.8</v>
       </c>
       <c r="Q23" s="2" t="n">
-        <v>6.77</v>
+        <v>1.78</v>
       </c>
       <c r="R23" s="2" t="n">
-        <v>14.08</v>
-      </c>
-      <c r="S23" s="2" t="n">
-        <v>5.93</v>
+        <v>16.81</v>
+      </c>
+      <c r="S23" t="n">
+        <v>-11.29</v>
       </c>
       <c r="T23" t="n">
-        <v>-74.5</v>
+        <v>-78.14</v>
       </c>
       <c r="U23" s="2" t="n">
-        <v>8.85</v>
+        <v>4.65</v>
       </c>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="n">
-        <v>-10.25</v>
-      </c>
-      <c r="X23" t="n">
-        <v>-3.83</v>
+        <v>-20.83</v>
+      </c>
+      <c r="X23" s="2" t="n">
+        <v>3.26</v>
       </c>
       <c r="Y23" s="2" t="n">
-        <v>25.88</v>
+        <v>25.11</v>
       </c>
       <c r="Z23" s="2" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="AA23" t="n">
-        <v>-12.88</v>
+        <v>-5.17</v>
       </c>
       <c r="AB23" s="2" t="n">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24">
@@ -2479,83 +2481,83 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>8.630000000000001</v>
+        <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>-38</v>
+        <v>-48.33</v>
       </c>
       <c r="D24" t="n">
-        <v>-7.78</v>
+        <v>-13.15</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>0.9399999999999999</v>
+        <v>1.96</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>34.5</v>
+        <v>35</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>21.58</v>
+        <v>8.93</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>5.27</v>
+        <v>8.85</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>62.5</v>
+        <v>8.33</v>
       </c>
       <c r="J24" t="n">
-        <v>-24.24</v>
-      </c>
-      <c r="K24" s="2" t="n">
-        <v>10.82</v>
+        <v>-31.68</v>
+      </c>
+      <c r="K24" t="n">
+        <v>-16.52</v>
       </c>
       <c r="L24" t="n">
-        <v>-25</v>
+        <v>-37.5</v>
       </c>
       <c r="M24" s="2" t="n">
-        <v>14.62</v>
+        <v>7.51</v>
       </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" s="2" t="n">
-        <v>8.380000000000001</v>
+        <v>2.29</v>
       </c>
       <c r="P24" t="n">
-        <v>-25.95</v>
+        <v>-17.11</v>
       </c>
       <c r="Q24" t="n">
-        <v>-32.05</v>
+        <v>-47.36</v>
       </c>
       <c r="R24" s="2" t="n">
-        <v>24.09</v>
+        <v>5</v>
       </c>
       <c r="S24" t="n">
-        <v>-13.82</v>
+        <v>-15.74</v>
       </c>
       <c r="T24" t="n">
-        <v>-42.91</v>
+        <v>-10.07</v>
       </c>
       <c r="U24" t="n">
-        <v>-11.72</v>
+        <v>-5.27</v>
       </c>
       <c r="V24" t="n">
-        <v>-10</v>
+        <v>-40</v>
       </c>
       <c r="W24" s="2" t="n">
-        <v>22.89</v>
+        <v>10.65</v>
       </c>
       <c r="X24" s="2" t="n">
-        <v>16.09</v>
+        <v>19.4</v>
       </c>
       <c r="Y24" s="2" t="n">
-        <v>89.43000000000001</v>
+        <v>65.75</v>
       </c>
       <c r="Z24" t="n">
-        <v>-30.77</v>
+        <v>-8.82</v>
       </c>
       <c r="AA24" t="n">
-        <v>-7.92</v>
+        <v>-16.16</v>
       </c>
       <c r="AB24" s="2" t="n">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25">
@@ -2565,85 +2567,85 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>30.61</v>
+        <v>18.71</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>120</v>
       </c>
       <c r="D25" t="n">
-        <v>-29.83</v>
+        <v>-22.81</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>6.09</v>
+        <v>1.71</v>
       </c>
       <c r="F25" t="n">
-        <v>-9.85</v>
+        <v>-18.94</v>
       </c>
       <c r="G25" t="n">
-        <v>-9.23</v>
+        <v>-6</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>1.04</v>
+        <v>0.34</v>
       </c>
       <c r="I25" t="n">
         <v>-100</v>
       </c>
-      <c r="J25" s="2" t="n">
-        <v>14.04</v>
+      <c r="J25" t="n">
+        <v>-2.7</v>
       </c>
       <c r="K25" t="n">
-        <v>-43.77</v>
+        <v>-33.19</v>
       </c>
       <c r="L25" t="n">
-        <v>-10.5</v>
+        <v>-17.85</v>
       </c>
       <c r="M25" s="2" t="n">
-        <v>2.53</v>
+        <v>6.3</v>
       </c>
       <c r="N25" s="2" t="n">
         <v>100</v>
       </c>
       <c r="O25" t="n">
-        <v>-7.84</v>
+        <v>-7.37</v>
       </c>
       <c r="P25" s="2" t="n">
-        <v>23.42</v>
+        <v>16.73</v>
       </c>
       <c r="Q25" t="n">
-        <v>-29.17</v>
+        <v>-9.59</v>
       </c>
       <c r="R25" s="2" t="n">
-        <v>17.93</v>
+        <v>1.41</v>
       </c>
       <c r="S25" t="n">
-        <v>-1.15</v>
+        <v>-3.55</v>
       </c>
       <c r="T25" t="n">
-        <v>-31.57</v>
+        <v>-52.1</v>
       </c>
       <c r="U25" t="n">
-        <v>-3.29</v>
+        <v>-5.08</v>
       </c>
       <c r="V25" s="2" t="n">
         <v>57</v>
       </c>
       <c r="W25" t="n">
-        <v>-30.62</v>
+        <v>-22.32</v>
       </c>
       <c r="X25" t="n">
-        <v>-2.38</v>
+        <v>-6.35</v>
       </c>
       <c r="Y25" t="n">
-        <v>-20.5</v>
-      </c>
-      <c r="Z25" s="2" t="n">
-        <v>4.46</v>
+        <v>-7.47</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>-4.65</v>
       </c>
       <c r="AA25" s="2" t="n">
-        <v>2.89</v>
+        <v>0.63</v>
       </c>
       <c r="AB25" s="2" t="n">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26">
@@ -2653,85 +2655,85 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-3.51</v>
+        <v>-4.04</v>
       </c>
       <c r="C26" t="n">
-        <v>-11.48</v>
+        <v>-14.64</v>
       </c>
       <c r="D26" t="n">
-        <v>-14.65</v>
+        <v>-4.61</v>
       </c>
       <c r="E26" t="n">
-        <v>-5.12</v>
+        <v>-4.33</v>
       </c>
       <c r="F26" t="n">
-        <v>-100</v>
+        <v>-56.67</v>
       </c>
       <c r="G26" t="n">
-        <v>-22.54</v>
-      </c>
-      <c r="H26" t="n">
-        <v>-3.01</v>
+        <v>-18.13</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>2.66</v>
       </c>
       <c r="I26" t="n">
-        <v>-25</v>
+        <v>-24.74</v>
       </c>
       <c r="J26" s="2" t="n">
-        <v>8.06</v>
+        <v>17.47</v>
       </c>
       <c r="K26" t="n">
-        <v>-4.24</v>
+        <v>-6.15</v>
       </c>
       <c r="L26" s="2" t="n">
-        <v>9.24</v>
+        <v>11.58</v>
       </c>
       <c r="M26" t="n">
-        <v>-2.76</v>
+        <v>-2.85</v>
       </c>
       <c r="N26" t="n">
-        <v>-43.33</v>
+        <v>-51.43</v>
       </c>
       <c r="O26" t="n">
-        <v>-6.19</v>
+        <v>-5.48</v>
       </c>
       <c r="P26" s="2" t="n">
-        <v>0.89</v>
+        <v>7.16</v>
       </c>
       <c r="Q26" t="n">
-        <v>-21.19</v>
+        <v>-20.07</v>
       </c>
       <c r="R26" s="2" t="n">
-        <v>47.19</v>
-      </c>
-      <c r="S26" s="2" t="n">
-        <v>6.04</v>
-      </c>
-      <c r="T26" s="2" t="n">
-        <v>16</v>
+        <v>37.27</v>
+      </c>
+      <c r="S26" t="n">
+        <v>-1.77</v>
+      </c>
+      <c r="T26" t="n">
+        <v>-7.2</v>
       </c>
       <c r="U26" t="n">
-        <v>-6.33</v>
+        <v>-8.449999999999999</v>
       </c>
       <c r="V26" s="2" t="n">
-        <v>50</v>
+        <v>53.5</v>
       </c>
       <c r="W26" t="n">
-        <v>-16.27</v>
+        <v>-17.97</v>
       </c>
       <c r="X26" s="2" t="n">
-        <v>8.33</v>
-      </c>
-      <c r="Y26" s="2" t="n">
-        <v>1.06</v>
+        <v>7.73</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>-13.12</v>
       </c>
       <c r="Z26" s="2" t="n">
-        <v>35.25</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="AA26" s="2" t="n">
-        <v>5.42</v>
+        <v>0.76</v>
       </c>
       <c r="AB26" s="2" t="n">
-        <v>85</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27">
@@ -2741,85 +2743,85 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>0.93</v>
+        <v>11.37</v>
       </c>
       <c r="C27" t="n">
         <v>-100</v>
       </c>
       <c r="D27" t="n">
-        <v>-50.41</v>
+        <v>-49.61</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>13.77</v>
+        <v>15.68</v>
       </c>
       <c r="F27" t="n">
-        <v>-10.82</v>
+        <v>-9.619999999999999</v>
       </c>
       <c r="G27" t="n">
-        <v>-25</v>
+        <v>-13.1</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>3.68</v>
+        <v>1.39</v>
       </c>
       <c r="I27" s="2" t="n">
-        <v>22.47</v>
+        <v>16.35</v>
       </c>
       <c r="J27" s="2" t="n">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="K27" t="n">
-        <v>-18.24</v>
+        <v>-19.4</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>79.18000000000001</v>
+        <v>40.79</v>
       </c>
       <c r="M27" t="n">
-        <v>-22.49</v>
+        <v>-18.41</v>
       </c>
       <c r="N27" s="2" t="n">
         <v>50</v>
       </c>
       <c r="O27" t="n">
-        <v>-7.67</v>
+        <v>-6.03</v>
       </c>
       <c r="P27" s="2" t="n">
-        <v>25.04</v>
+        <v>18.1</v>
       </c>
       <c r="Q27" t="n">
-        <v>-17.67</v>
+        <v>-18.76</v>
       </c>
       <c r="R27" s="2" t="n">
-        <v>20.5</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="S27" t="n">
-        <v>-21.3</v>
+        <v>-25.54</v>
       </c>
       <c r="T27" t="n">
-        <v>-66.67</v>
+        <v>-69.23</v>
       </c>
       <c r="U27" s="2" t="n">
-        <v>8.880000000000001</v>
+        <v>3.44</v>
       </c>
       <c r="V27" s="2" t="n">
         <v>2.8</v>
       </c>
       <c r="W27" t="n">
-        <v>-15.44</v>
+        <v>-16</v>
       </c>
       <c r="X27" s="2" t="n">
-        <v>4.54</v>
+        <v>2.18</v>
       </c>
       <c r="Y27" t="n">
-        <v>-47.53</v>
+        <v>-50.81</v>
       </c>
       <c r="Z27" s="2" t="n">
-        <v>68.33</v>
+        <v>37.73</v>
       </c>
       <c r="AA27" t="n">
-        <v>-21.24</v>
+        <v>-15.64</v>
       </c>
       <c r="AB27" s="2" t="n">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28">
@@ -2909,79 +2911,81 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-13.35</v>
+        <v>-11.39</v>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="n">
-        <v>-9.609999999999999</v>
+        <v>-4.9</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>14.91</v>
+        <v>15</v>
       </c>
       <c r="F29" t="n">
-        <v>-12.66</v>
+        <v>-10.05</v>
       </c>
       <c r="G29" t="n">
-        <v>-41.17</v>
+        <v>-32.14</v>
       </c>
       <c r="H29" t="n">
-        <v>-8.619999999999999</v>
+        <v>-6.02</v>
       </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="n">
-        <v>-10.36</v>
+        <v>-13.77</v>
       </c>
       <c r="K29" s="2" t="n">
-        <v>11.14</v>
+        <v>5.92</v>
       </c>
       <c r="L29" s="2" t="n">
         <v>17.09</v>
       </c>
-      <c r="M29" s="2" t="n">
-        <v>2.23</v>
+      <c r="M29" t="n">
+        <v>-0.5</v>
       </c>
       <c r="N29" t="n">
         <v>-100</v>
       </c>
       <c r="O29" t="n">
-        <v>-4.15</v>
+        <v>-2.55</v>
       </c>
       <c r="P29" t="n">
-        <v>-7.17</v>
+        <v>-5.71</v>
       </c>
       <c r="Q29" t="n">
-        <v>-12.38</v>
-      </c>
-      <c r="R29" s="2" t="n">
-        <v>2.2</v>
+        <v>-24.07</v>
+      </c>
+      <c r="R29" t="n">
+        <v>-3.3</v>
       </c>
       <c r="S29" t="n">
-        <v>-34.12</v>
+        <v>-35.33</v>
       </c>
       <c r="T29" s="2" t="n">
-        <v>30.83</v>
+        <v>26.43</v>
       </c>
       <c r="U29" s="2" t="n">
-        <v>3.5</v>
+        <v>7.56</v>
       </c>
       <c r="V29" t="n">
         <v>-50</v>
       </c>
       <c r="W29" t="n">
-        <v>-1.21</v>
+        <v>-6.18</v>
       </c>
       <c r="X29" t="n">
-        <v>-4.42</v>
-      </c>
-      <c r="Y29" t="inlineStr"/>
+        <v>-3.48</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>-100</v>
+      </c>
       <c r="Z29" t="n">
         <v>-73.56</v>
       </c>
       <c r="AA29" t="n">
-        <v>-15.54</v>
+        <v>-14.61</v>
       </c>
       <c r="AB29" s="2" t="n">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30">
@@ -2991,83 +2995,83 @@
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>3.03</v>
+        <v>3.35</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>28.12</v>
+        <v>20.59</v>
       </c>
       <c r="D30" t="n">
-        <v>-1.26</v>
+        <v>-16.75</v>
       </c>
       <c r="E30" t="n">
-        <v>-9.470000000000001</v>
+        <v>-3.64</v>
       </c>
       <c r="F30" t="n">
-        <v>-18.75</v>
-      </c>
-      <c r="G30" s="2" t="n">
-        <v>2.55</v>
+        <v>-13.33</v>
+      </c>
+      <c r="G30" t="n">
+        <v>-9.949999999999999</v>
       </c>
       <c r="H30" t="n">
-        <v>-4.39</v>
+        <v>-2.97</v>
       </c>
       <c r="I30" s="2" t="n">
         <v>2.6</v>
       </c>
       <c r="J30" t="n">
-        <v>-9.92</v>
+        <v>-5.02</v>
       </c>
       <c r="K30" t="n">
-        <v>-30.53</v>
+        <v>-30.81</v>
       </c>
       <c r="L30" t="n">
-        <v>-54.5</v>
+        <v>-7.82</v>
       </c>
       <c r="M30" t="n">
-        <v>-14.7</v>
+        <v>-11.98</v>
       </c>
       <c r="N30" t="n">
         <v>-100</v>
       </c>
       <c r="O30" t="n">
-        <v>-10.17</v>
+        <v>-7.52</v>
       </c>
       <c r="P30" t="n">
-        <v>-12.62</v>
+        <v>-11.02</v>
       </c>
       <c r="Q30" t="n">
-        <v>-31.63</v>
+        <v>-30.81</v>
       </c>
       <c r="R30" s="2" t="n">
-        <v>15.11</v>
+        <v>9.91</v>
       </c>
       <c r="S30" t="n">
-        <v>-31.27</v>
-      </c>
-      <c r="T30" s="2" t="n">
-        <v>11.17</v>
+        <v>-18.47</v>
+      </c>
+      <c r="T30" t="n">
+        <v>-0.86</v>
       </c>
       <c r="U30" s="2" t="n">
-        <v>2.39</v>
+        <v>3.59</v>
       </c>
       <c r="V30" t="inlineStr"/>
       <c r="W30" t="n">
-        <v>-6.33</v>
-      </c>
-      <c r="X30" s="2" t="n">
-        <v>0.35</v>
+        <v>-5.96</v>
+      </c>
+      <c r="X30" t="n">
+        <v>-0.57</v>
       </c>
       <c r="Y30" t="n">
         <v>-14.24</v>
       </c>
       <c r="Z30" t="n">
-        <v>-47.24</v>
+        <v>-17.64</v>
       </c>
       <c r="AA30" t="n">
-        <v>-5.94</v>
+        <v>-4.54</v>
       </c>
       <c r="AB30" s="2" t="n">
-        <v>75</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31">

</xml_diff>

<commit_message>
added mexico, updated until 04.02.2025
</commit_message>
<xml_diff>
--- a/ROI_leagues.xlsx
+++ b/ROI_leagues.xlsx
@@ -2999,85 +2999,85 @@
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>43.1</v>
+        <v>32.88</v>
       </c>
       <c r="C30" t="n">
         <v>-100</v>
       </c>
-      <c r="D30" s="2" t="n">
-        <v>8.199999999999999</v>
+      <c r="D30" t="n">
+        <v>-21.04</v>
       </c>
       <c r="E30" t="n">
-        <v>-8.83</v>
+        <v>-0.5</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>3.67</v>
+        <v>5.4</v>
       </c>
       <c r="G30" t="n">
-        <v>-7.75</v>
+        <v>-36.36</v>
       </c>
       <c r="H30" t="n">
-        <v>-14.18</v>
+        <v>-9.199999999999999</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>73.2</v>
-      </c>
-      <c r="J30" t="n">
-        <v>-9.300000000000001</v>
+        <v>6</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>1.07</v>
       </c>
       <c r="K30" t="n">
-        <v>-30</v>
+        <v>-27.59</v>
       </c>
       <c r="L30" t="n">
-        <v>-60.33</v>
+        <v>-28.56</v>
       </c>
       <c r="M30" t="n">
-        <v>-25.2</v>
+        <v>-10.51</v>
       </c>
       <c r="N30" s="2" t="n">
-        <v>116.5</v>
+        <v>27.55</v>
       </c>
       <c r="O30" t="n">
-        <v>-22.86</v>
+        <v>-11.52</v>
       </c>
       <c r="P30" s="2" t="n">
-        <v>3.12</v>
+        <v>13.35</v>
       </c>
       <c r="Q30" s="2" t="n">
-        <v>26.88</v>
+        <v>8.9</v>
       </c>
       <c r="R30" s="2" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="S30" s="2" t="n">
-        <v>49.67</v>
-      </c>
-      <c r="T30" t="n">
-        <v>-100</v>
-      </c>
-      <c r="U30" s="2" t="n">
-        <v>26.62</v>
+        <v>9.24</v>
+      </c>
+      <c r="S30" t="n">
+        <v>-6.88</v>
+      </c>
+      <c r="T30" s="2" t="n">
+        <v>11.69</v>
+      </c>
+      <c r="U30" t="n">
+        <v>-7.37</v>
       </c>
       <c r="V30" t="n">
-        <v>-50</v>
-      </c>
-      <c r="W30" s="2" t="n">
-        <v>23.4</v>
-      </c>
-      <c r="X30" t="n">
-        <v>-22.8</v>
-      </c>
-      <c r="Y30" s="2" t="n">
-        <v>8.33</v>
+        <v>-27.25</v>
+      </c>
+      <c r="W30" t="n">
+        <v>-14.11</v>
+      </c>
+      <c r="X30" s="2" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>-3.62</v>
       </c>
       <c r="Z30" t="n">
-        <v>-28.67</v>
+        <v>-32</v>
       </c>
       <c r="AA30" t="n">
-        <v>-7.4</v>
+        <v>-8.17</v>
       </c>
       <c r="AB30" s="2" t="n">
-        <v>16</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31">

</xml_diff>

<commit_message>
added article calculations next time will add combined bets
</commit_message>
<xml_diff>
--- a/ROI_leagues.xlsx
+++ b/ROI_leagues.xlsx
@@ -588,39 +588,43 @@
       <c r="C2" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" s="2" t="n">
+        <v>275</v>
+      </c>
       <c r="E2" s="2" t="n">
         <v>1.69</v>
       </c>
       <c r="F2" t="n">
         <v>-100</v>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" s="2" t="n">
+        <v>53</v>
+      </c>
       <c r="H2" t="n">
         <v>-2.73</v>
       </c>
       <c r="I2" t="n">
-        <v>-25</v>
+        <v>-43.75</v>
       </c>
       <c r="J2" t="n">
         <v>-100</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2.15</v>
+        <v>4.57</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>-1.07</v>
+        <v>-0.27</v>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
-        <v>-3.14</v>
+        <v>-2.73</v>
       </c>
       <c r="P2" t="n">
         <v>-100</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>23.77</v>
+        <v>26.14</v>
       </c>
       <c r="R2" t="n">
         <v>-100</v>
@@ -628,26 +632,28 @@
       <c r="S2" t="n">
         <v>-13.27</v>
       </c>
-      <c r="T2" t="inlineStr"/>
+      <c r="T2" s="2" t="n">
+        <v>333</v>
+      </c>
       <c r="U2" t="n">
         <v>-0.08</v>
       </c>
       <c r="V2" t="inlineStr"/>
       <c r="W2" s="2" t="n">
-        <v>46.5</v>
+        <v>42</v>
       </c>
       <c r="X2" s="2" t="n">
-        <v>7.89</v>
+        <v>13.8</v>
       </c>
       <c r="Y2" s="2" t="n">
         <v>39.6</v>
       </c>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="n">
-        <v>-2.36</v>
+        <v>-0.87</v>
       </c>
       <c r="AB2" s="2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -989,7 +995,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>14.2</v>
+        <v>8.76</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>75</v>
@@ -998,7 +1004,7 @@
         <v>-22.68</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>12.44</v>
+        <v>12.32</v>
       </c>
       <c r="F7" t="n">
         <v>-29.56</v>
@@ -1007,44 +1013,44 @@
         <v>6.94</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.14</v>
+        <v>-0.67</v>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="n">
         <v>-3.9</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>4.08</v>
+        <v>12.36</v>
       </c>
       <c r="L7" s="2" t="n">
         <v>5.33</v>
       </c>
       <c r="M7" t="n">
-        <v>-18.8</v>
+        <v>-17.06</v>
       </c>
       <c r="N7" t="n">
         <v>-100</v>
       </c>
       <c r="O7" t="n">
-        <v>-8</v>
+        <v>-7.41</v>
       </c>
       <c r="P7" s="2" t="n">
         <v>25.63</v>
       </c>
       <c r="Q7" s="2" t="n">
-        <v>20.21</v>
+        <v>12.2</v>
       </c>
       <c r="R7" s="2" t="n">
         <v>43.41</v>
       </c>
       <c r="S7" s="2" t="n">
-        <v>22.5</v>
+        <v>29.21</v>
       </c>
       <c r="T7" t="n">
         <v>-38</v>
       </c>
       <c r="U7" s="2" t="n">
-        <v>3.13</v>
+        <v>3.33</v>
       </c>
       <c r="V7" t="n">
         <v>-24.25</v>
@@ -1053,7 +1059,7 @@
         <v>19.71</v>
       </c>
       <c r="X7" t="n">
-        <v>-9.59</v>
+        <v>-11.74</v>
       </c>
       <c r="Y7" t="n">
         <v>0</v>
@@ -1062,10 +1068,10 @@
         <v>49.5</v>
       </c>
       <c r="AA7" s="2" t="n">
-        <v>16.21</v>
+        <v>17.38</v>
       </c>
       <c r="AB7" s="2" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
@@ -2209,81 +2215,81 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>25.09</v>
+        <v>25.17</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>-28.27</v>
+        <v>-32.75</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>13.14</v>
+        <v>12.73</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>10.8</v>
       </c>
       <c r="G21" t="n">
-        <v>-47.89</v>
+        <v>-53.1</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>0.51</v>
+        <v>1.59</v>
       </c>
       <c r="I21" t="n">
         <v>-100</v>
       </c>
       <c r="J21" s="2" t="n">
-        <v>23.42</v>
+        <v>24.45</v>
       </c>
       <c r="K21" t="n">
-        <v>-47.37</v>
+        <v>-41</v>
       </c>
       <c r="L21" t="n">
         <v>-50</v>
       </c>
       <c r="M21" t="n">
-        <v>-13.64</v>
+        <v>-14.89</v>
       </c>
       <c r="N21" t="n">
         <v>-100</v>
       </c>
       <c r="O21" t="n">
-        <v>-4.92</v>
+        <v>-6.97</v>
       </c>
       <c r="P21" s="2" t="n">
-        <v>5.28</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="Q21" t="n">
-        <v>-51.1</v>
+        <v>-44.14</v>
       </c>
       <c r="R21" t="n">
-        <v>-54</v>
+        <v>-59.11</v>
       </c>
       <c r="S21" t="n">
-        <v>-20.07</v>
+        <v>-22.83</v>
       </c>
       <c r="T21" t="n">
         <v>-100</v>
       </c>
       <c r="U21" t="n">
-        <v>-3.71</v>
+        <v>-3.32</v>
       </c>
       <c r="V21" t="inlineStr"/>
       <c r="W21" t="n">
-        <v>-34.93</v>
+        <v>-39.27</v>
       </c>
       <c r="X21" s="2" t="n">
-        <v>8.6</v>
+        <v>9.92</v>
       </c>
       <c r="Y21" t="n">
         <v>-100</v>
       </c>
       <c r="Z21" s="2" t="n">
-        <v>1.73</v>
+        <v>8.5</v>
       </c>
       <c r="AA21" t="n">
-        <v>-45.22</v>
+        <v>-41.83</v>
       </c>
       <c r="AB21" s="2" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22">
@@ -2461,81 +2467,81 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-18.99</v>
+        <v>-18.85</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" s="2" t="n">
-        <v>17.38</v>
+        <v>23.24</v>
       </c>
       <c r="E24" t="n">
-        <v>-6.43</v>
-      </c>
-      <c r="F24" t="n">
-        <v>-0.29</v>
+        <v>-6.85</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>1.36</v>
       </c>
       <c r="G24" s="2" t="n">
         <v>8.67</v>
       </c>
       <c r="H24" t="n">
-        <v>-9.359999999999999</v>
+        <v>-10.09</v>
       </c>
       <c r="I24" t="n">
         <v>-23.92</v>
       </c>
       <c r="J24" t="n">
-        <v>-18.18</v>
+        <v>-21.23</v>
       </c>
       <c r="K24" t="n">
-        <v>-1.21</v>
+        <v>-2.17</v>
       </c>
       <c r="L24" t="n">
-        <v>-28.12</v>
+        <v>-4.17</v>
       </c>
       <c r="M24" t="n">
-        <v>-1.78</v>
+        <v>-0.58</v>
       </c>
       <c r="N24" t="n">
         <v>-100</v>
       </c>
       <c r="O24" t="n">
-        <v>-2.67</v>
+        <v>-2.52</v>
       </c>
       <c r="P24" t="n">
-        <v>-21.82</v>
+        <v>-22.81</v>
       </c>
       <c r="Q24" t="n">
         <v>-8.33</v>
       </c>
-      <c r="R24" s="2" t="n">
-        <v>2.4</v>
+      <c r="R24" t="n">
+        <v>-2.17</v>
       </c>
       <c r="S24" t="n">
-        <v>-32.69</v>
+        <v>-36.49</v>
       </c>
       <c r="T24" t="n">
-        <v>-4.11</v>
+        <v>-12.43</v>
       </c>
       <c r="U24" t="n">
-        <v>-10.74</v>
+        <v>-13.29</v>
       </c>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="n">
-        <v>-10.48</v>
+        <v>-9.84</v>
       </c>
       <c r="X24" s="2" t="n">
-        <v>7.05</v>
+        <v>6.44</v>
       </c>
       <c r="Y24" t="n">
         <v>-12.44</v>
       </c>
       <c r="Z24" s="2" t="n">
-        <v>16.76</v>
+        <v>12.59</v>
       </c>
       <c r="AA24" t="n">
-        <v>-5.76</v>
+        <v>-5.16</v>
       </c>
       <c r="AB24" s="2" t="n">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25">
@@ -2628,8 +2634,8 @@
           <t>Portugal2</t>
         </is>
       </c>
-      <c r="B26" s="2" t="n">
-        <v>1.98</v>
+      <c r="B26" t="n">
+        <v>-0.02</v>
       </c>
       <c r="C26" t="n">
         <v>-81.76000000000001</v>
@@ -2638,7 +2644,7 @@
         <v>-19.52</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.32</v>
+        <v>-2.17</v>
       </c>
       <c r="F26" t="n">
         <v>-8.69</v>
@@ -2647,13 +2653,13 @@
         <v>-5.32</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>1.18</v>
+        <v>0.28</v>
       </c>
       <c r="I26" s="2" t="n">
         <v>20.63</v>
       </c>
       <c r="J26" t="n">
-        <v>-27.45</v>
+        <v>-29.07</v>
       </c>
       <c r="K26" t="n">
         <v>-17.96</v>
@@ -2661,21 +2667,21 @@
       <c r="L26" t="n">
         <v>-53.12</v>
       </c>
-      <c r="M26" t="n">
-        <v>-0.05</v>
+      <c r="M26" s="2" t="n">
+        <v>0.24</v>
       </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>-3.08</v>
+        <v>-2.96</v>
       </c>
       <c r="P26" t="n">
-        <v>-16.25</v>
+        <v>-17.72</v>
       </c>
       <c r="Q26" t="n">
         <v>-31.03</v>
       </c>
       <c r="R26" s="2" t="n">
-        <v>14.17</v>
+        <v>10.37</v>
       </c>
       <c r="S26" t="n">
         <v>-11.38</v>
@@ -2684,7 +2690,7 @@
         <v>-32.04</v>
       </c>
       <c r="U26" t="n">
-        <v>-0.38</v>
+        <v>-0.11</v>
       </c>
       <c r="V26" t="n">
         <v>-10</v>
@@ -2693,19 +2699,19 @@
         <v>2.65</v>
       </c>
       <c r="X26" s="2" t="n">
-        <v>1.69</v>
+        <v>0.72</v>
       </c>
       <c r="Y26" s="2" t="n">
         <v>0.93</v>
       </c>
       <c r="Z26" s="2" t="n">
-        <v>26.83</v>
+        <v>22.74</v>
       </c>
       <c r="AA26" t="n">
         <v>-8.130000000000001</v>
       </c>
       <c r="AB26" s="2" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27">
@@ -3163,7 +3169,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-2.07</v>
+        <v>-1.11</v>
       </c>
       <c r="C33" t="n">
         <v>-45</v>
@@ -3172,7 +3178,7 @@
         <v>-2</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>0.41</v>
+        <v>0.76</v>
       </c>
       <c r="F33" t="n">
         <v>-6.92</v>
@@ -3181,7 +3187,7 @@
         <v>-0.42</v>
       </c>
       <c r="H33" t="n">
-        <v>-7.09</v>
+        <v>-6.67</v>
       </c>
       <c r="I33" s="2" t="n">
         <v>35.32</v>
@@ -3190,37 +3196,37 @@
         <v>15.81</v>
       </c>
       <c r="K33" t="n">
-        <v>-8.720000000000001</v>
+        <v>-8.24</v>
       </c>
       <c r="L33" t="n">
         <v>-6.82</v>
       </c>
       <c r="M33" t="n">
-        <v>-8.460000000000001</v>
+        <v>-8.31</v>
       </c>
       <c r="N33" s="2" t="n">
         <v>50</v>
       </c>
       <c r="O33" t="n">
-        <v>-2.6</v>
+        <v>-2.56</v>
       </c>
       <c r="P33" t="n">
         <v>-1.57</v>
       </c>
       <c r="Q33" t="n">
-        <v>-9</v>
+        <v>-8.44</v>
       </c>
       <c r="R33" s="2" t="n">
         <v>3.57</v>
       </c>
       <c r="S33" t="n">
-        <v>-13.95</v>
+        <v>-14.77</v>
       </c>
       <c r="T33" t="n">
         <v>-52.5</v>
       </c>
       <c r="U33" t="n">
-        <v>-1.54</v>
+        <v>-1.35</v>
       </c>
       <c r="V33" s="2" t="n">
         <v>0.7</v>
@@ -3229,7 +3235,7 @@
         <v>-19.46</v>
       </c>
       <c r="X33" t="n">
-        <v>-8.699999999999999</v>
+        <v>-8.15</v>
       </c>
       <c r="Y33" t="n">
         <v>-47.09</v>
@@ -3238,10 +3244,10 @@
         <v>26.25</v>
       </c>
       <c r="AA33" t="n">
-        <v>-2.63</v>
+        <v>-2.47</v>
       </c>
       <c r="AB33" s="2" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34">
@@ -3415,71 +3421,71 @@
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>8.800000000000001</v>
+        <v>8.039999999999999</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>33.89</v>
       </c>
       <c r="D36" t="n">
-        <v>-27.81</v>
+        <v>-30.25</v>
       </c>
       <c r="E36" t="n">
-        <v>-2.48</v>
+        <v>-1.82</v>
       </c>
       <c r="F36" t="n">
         <v>-20.69</v>
       </c>
       <c r="G36" t="n">
-        <v>-17.32</v>
+        <v>-20.17</v>
       </c>
       <c r="H36" t="n">
-        <v>-5.05</v>
+        <v>-5.9</v>
       </c>
       <c r="I36" s="2" t="n">
         <v>28.25</v>
       </c>
       <c r="J36" t="n">
-        <v>-11.55</v>
+        <v>-13.65</v>
       </c>
       <c r="K36" t="n">
-        <v>-25.21</v>
+        <v>-27.7</v>
       </c>
       <c r="L36" t="n">
         <v>-9.56</v>
       </c>
       <c r="M36" t="n">
-        <v>-8.609999999999999</v>
+        <v>-9.390000000000001</v>
       </c>
       <c r="N36" t="n">
         <v>-100</v>
       </c>
       <c r="O36" t="n">
-        <v>-9.9</v>
+        <v>-9.300000000000001</v>
       </c>
       <c r="P36" t="n">
-        <v>-14.66</v>
+        <v>-15.45</v>
       </c>
       <c r="Q36" t="n">
-        <v>-25.48</v>
+        <v>-26.68</v>
       </c>
       <c r="R36" t="n">
-        <v>-10.46</v>
+        <v>-5.62</v>
       </c>
       <c r="S36" t="n">
-        <v>-17.04</v>
+        <v>-14.76</v>
       </c>
       <c r="T36" t="n">
         <v>-4.06</v>
       </c>
       <c r="U36" s="2" t="n">
-        <v>0.05</v>
+        <v>0.45</v>
       </c>
       <c r="V36" t="inlineStr"/>
       <c r="W36" t="n">
-        <v>-10.52</v>
+        <v>-9.17</v>
       </c>
       <c r="X36" t="n">
-        <v>-0.93</v>
+        <v>-1.79</v>
       </c>
       <c r="Y36" t="n">
         <v>-28.57</v>
@@ -3488,10 +3494,10 @@
         <v>-28.48</v>
       </c>
       <c r="AA36" t="n">
-        <v>-7.91</v>
+        <v>-6.34</v>
       </c>
       <c r="AB36" s="2" t="n">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37">

</xml_diff>

<commit_message>
updated after a while
</commit_message>
<xml_diff>
--- a/ROI_leagues.xlsx
+++ b/ROI_leagues.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB51"/>
+  <dimension ref="A1:AB50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,83 +583,83 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-41.14</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>27.6</v>
+        <v>-33.08</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>8.67</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-29.11</v>
       </c>
       <c r="E2" t="n">
-        <v>-3.08</v>
+        <v>-4.36</v>
       </c>
       <c r="F2" t="n">
-        <v>-100</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>24.25</v>
-      </c>
-      <c r="H2" t="n">
-        <v>-7.19</v>
+        <v>-66</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-4.65</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0.16</v>
       </c>
       <c r="I2" t="n">
-        <v>-17.45</v>
+        <v>-11.13</v>
       </c>
       <c r="J2" t="n">
-        <v>-43.33</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>4.29</v>
+        <v>-2.08</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-5.17</v>
       </c>
       <c r="L2" t="n">
         <v>-100</v>
       </c>
-      <c r="M2" s="2" t="n">
-        <v>5.75</v>
+      <c r="M2" t="n">
+        <v>-4.6</v>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
-        <v>-1.16</v>
+        <v>-2.43</v>
       </c>
       <c r="P2" t="n">
-        <v>-50</v>
-      </c>
-      <c r="Q2" s="2" t="n">
-        <v>9.380000000000001</v>
+        <v>-2.22</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-1.12</v>
       </c>
       <c r="R2" t="n">
-        <v>-59.38</v>
+        <v>-46.82</v>
       </c>
       <c r="S2" s="2" t="n">
-        <v>8.800000000000001</v>
+        <v>14.33</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>93.25</v>
+        <v>78.83</v>
       </c>
       <c r="U2" t="n">
-        <v>-6</v>
+        <v>-5.31</v>
       </c>
       <c r="V2" t="n">
         <v>-100</v>
       </c>
       <c r="W2" s="2" t="n">
-        <v>28.57</v>
+        <v>7.75</v>
       </c>
       <c r="X2" s="2" t="n">
-        <v>16.77</v>
+        <v>9.92</v>
       </c>
       <c r="Y2" s="2" t="n">
-        <v>27.4</v>
+        <v>12.57</v>
       </c>
       <c r="Z2" t="n">
         <v>-100</v>
       </c>
       <c r="AA2" t="n">
-        <v>-13.45</v>
+        <v>-15.88</v>
       </c>
       <c r="AB2" s="2" t="n">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
@@ -669,27 +669,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-41.12</v>
+        <v>-44.59</v>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" s="2" t="n">
-        <v>1.46</v>
+      <c r="D3" t="n">
+        <v>-18.77</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>2.78</v>
       </c>
       <c r="F3" t="n">
-        <v>-5.31</v>
+        <v>-12.07</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>31.29</v>
+        <v>10.71</v>
       </c>
       <c r="H3" t="n">
-        <v>-3.76</v>
+        <v>-3.17</v>
       </c>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
-        <v>-4.3</v>
+      <c r="J3" s="2" t="n">
+        <v>6.52</v>
       </c>
       <c r="K3" s="2" t="n">
         <v>51.22</v>
@@ -698,46 +698,46 @@
         <v>-34.33</v>
       </c>
       <c r="M3" t="n">
-        <v>-24.4</v>
+        <v>-34.86</v>
       </c>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="n">
-        <v>-5.1</v>
-      </c>
-      <c r="P3" t="n">
-        <v>-1.39</v>
+        <v>-12.17</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>9.26</v>
       </c>
       <c r="Q3" t="n">
         <v>-24.55</v>
       </c>
       <c r="R3" s="2" t="n">
-        <v>11.44</v>
+        <v>0.3</v>
       </c>
       <c r="S3" t="n">
         <v>-1.58</v>
       </c>
-      <c r="T3" s="2" t="n">
-        <v>27.25</v>
+      <c r="T3" t="n">
+        <v>-11.5</v>
       </c>
       <c r="U3" s="2" t="n">
-        <v>9.789999999999999</v>
+        <v>2.47</v>
       </c>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="n">
-        <v>-11.67</v>
+        <v>-20.73</v>
       </c>
       <c r="X3" t="n">
-        <v>-8.34</v>
+        <v>-7.23</v>
       </c>
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" s="2" t="n">
-        <v>3.83</v>
+        <v>20.43</v>
       </c>
       <c r="AA3" t="n">
         <v>-25.7</v>
       </c>
       <c r="AB3" s="2" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-35.15</v>
+        <v>-30.36</v>
       </c>
       <c r="C4" t="n">
         <v>-22.5</v>
@@ -756,62 +756,62 @@
         <v>-24.82</v>
       </c>
       <c r="E4" t="n">
-        <v>-8.65</v>
+        <v>-5.07</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>9.109999999999999</v>
+        <v>9.75</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>8.890000000000001</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>3.42</v>
+        <v>2.68</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>300</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>29.91</v>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>4.95</v>
+        <v>26.09</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-4.17</v>
       </c>
       <c r="L4" s="2" t="n">
         <v>5.91</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>8.56</v>
+        <v>4.61</v>
       </c>
       <c r="N4" t="n">
         <v>-100</v>
       </c>
       <c r="O4" t="n">
-        <v>-1.13</v>
+        <v>-2.43</v>
       </c>
       <c r="P4" t="n">
-        <v>-10.55</v>
+        <v>-13.34</v>
       </c>
       <c r="Q4" t="n">
-        <v>-31.26</v>
+        <v>-36.76</v>
       </c>
       <c r="R4" t="n">
         <v>-50.09</v>
       </c>
       <c r="S4" t="n">
-        <v>-7.71</v>
+        <v>-9.470000000000001</v>
       </c>
       <c r="T4" t="n">
         <v>-33.13</v>
       </c>
       <c r="U4" t="n">
-        <v>-3.5</v>
+        <v>-5.26</v>
       </c>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="n">
         <v>-3.96</v>
       </c>
       <c r="X4" s="2" t="n">
-        <v>2.24</v>
+        <v>4.69</v>
       </c>
       <c r="Y4" s="2" t="n">
         <v>62.78</v>
@@ -820,10 +820,10 @@
         <v>6.92</v>
       </c>
       <c r="AA4" s="2" t="n">
-        <v>4.88</v>
+        <v>1.22</v>
       </c>
       <c r="AB4" s="2" t="n">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
@@ -833,73 +833,73 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>7.07</v>
+        <v>9.539999999999999</v>
       </c>
       <c r="C5" t="n">
         <v>-2.14</v>
       </c>
       <c r="D5" t="n">
-        <v>-36.55</v>
+        <v>-32.44</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>6.14</v>
+        <v>5.43</v>
       </c>
       <c r="F5" t="n">
         <v>-36.12</v>
       </c>
       <c r="G5" t="n">
-        <v>-10.27</v>
+        <v>-9.119999999999999</v>
       </c>
       <c r="H5" t="n">
-        <v>-10.71</v>
+        <v>-9.19</v>
       </c>
       <c r="I5" t="n">
         <v>-35</v>
       </c>
       <c r="J5" t="n">
-        <v>-15.53</v>
+        <v>-9.31</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>7.93</v>
+        <v>5.93</v>
       </c>
       <c r="L5" t="n">
         <v>-31.42</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>7.74</v>
+        <v>7.88</v>
       </c>
       <c r="N5" t="n">
         <v>-100</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>1.33</v>
+        <v>0.89</v>
       </c>
       <c r="P5" t="n">
-        <v>-23.52</v>
+        <v>-17.76</v>
       </c>
       <c r="Q5" t="n">
-        <v>-1.06</v>
+        <v>-1.1</v>
       </c>
       <c r="R5" t="n">
-        <v>-8.57</v>
+        <v>-10.98</v>
       </c>
       <c r="S5" t="n">
-        <v>-13.37</v>
+        <v>-13.48</v>
       </c>
       <c r="T5" t="n">
-        <v>-26.11</v>
+        <v>-19.46</v>
       </c>
       <c r="U5" s="2" t="n">
-        <v>2.58</v>
+        <v>1.67</v>
       </c>
       <c r="V5" t="n">
         <v>-68.59999999999999</v>
       </c>
       <c r="W5" t="n">
-        <v>-10.14</v>
+        <v>-9.460000000000001</v>
       </c>
       <c r="X5" t="n">
-        <v>-8.07</v>
+        <v>-7.32</v>
       </c>
       <c r="Y5" s="2" t="n">
         <v>23.29</v>
@@ -907,11 +907,11 @@
       <c r="Z5" t="n">
         <v>-77.37</v>
       </c>
-      <c r="AA5" t="n">
-        <v>-0.35</v>
+      <c r="AA5" s="2" t="n">
+        <v>0.37</v>
       </c>
       <c r="AB5" s="2" t="n">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6">
@@ -921,77 +921,69 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-24.6</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-100</v>
-      </c>
+        <v>-15.08</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>-19.82</v>
-      </c>
-      <c r="E6" t="n">
-        <v>-3.09</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>5.46</v>
+        <v>-54.25</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>18.67</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-66</v>
       </c>
       <c r="G6" t="n">
-        <v>-10.22</v>
+        <v>-70</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.64</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>175</v>
-      </c>
-      <c r="J6" t="n">
-        <v>-5.52</v>
+        <v>-3.53</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" s="2" t="n">
+        <v>110</v>
       </c>
       <c r="K6" t="n">
-        <v>-12.92</v>
+        <v>-10.93</v>
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>-4.05</v>
+        <v>-3.29</v>
       </c>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>-0.03</v>
+        <v>-3.94</v>
       </c>
       <c r="P6" s="2" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="Q6" t="n">
-        <v>-22.83</v>
+        <v>-4.5</v>
       </c>
       <c r="R6" t="n">
-        <v>-2.62</v>
-      </c>
-      <c r="S6" s="2" t="n">
-        <v>2.58</v>
+        <v>-8.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>-45.67</v>
       </c>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="n">
-        <v>-10.99</v>
+        <v>-10.75</v>
       </c>
       <c r="V6" t="inlineStr"/>
-      <c r="W6" s="2" t="n">
-        <v>4.86</v>
+      <c r="W6" t="n">
+        <v>-44.8</v>
       </c>
       <c r="X6" s="2" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="Y6" s="2" t="n">
-        <v>41.29</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>-100</v>
-      </c>
+        <v>10.71</v>
+      </c>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="n">
-        <v>-10</v>
+        <v>-7.29</v>
       </c>
       <c r="AB6" s="2" t="n">
-        <v>106</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
@@ -1001,83 +993,83 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>29.27</v>
+        <v>22.64</v>
       </c>
       <c r="C7" t="n">
-        <v>-100</v>
+        <v>-22.5</v>
       </c>
       <c r="D7" t="n">
-        <v>-50</v>
+        <v>-57.14</v>
       </c>
       <c r="E7" t="n">
-        <v>-4.64</v>
+        <v>-9.210000000000001</v>
       </c>
       <c r="F7" t="n">
         <v>-35.5</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>4.86</v>
+        <v>14.33</v>
       </c>
       <c r="H7" t="n">
-        <v>-17.79</v>
+        <v>-29.11</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>76.33</v>
+        <v>51.14</v>
       </c>
       <c r="J7" t="n">
-        <v>-50</v>
+        <v>-37.43</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>23.53</v>
+        <v>27.83</v>
       </c>
       <c r="L7" t="n">
         <v>-100</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>11.33</v>
+        <v>11.81</v>
       </c>
       <c r="N7" t="n">
         <v>-100</v>
       </c>
-      <c r="O7" t="n">
-        <v>-0.16</v>
+      <c r="O7" s="2" t="n">
+        <v>1.13</v>
       </c>
       <c r="P7" t="n">
-        <v>-47.5</v>
+        <v>-58</v>
       </c>
       <c r="Q7" s="2" t="n">
-        <v>20.25</v>
+        <v>18.45</v>
       </c>
       <c r="R7" s="2" t="n">
-        <v>52.2</v>
+        <v>16.75</v>
       </c>
       <c r="S7" t="n">
-        <v>-26.46</v>
+        <v>-17.43</v>
       </c>
       <c r="T7" t="n">
         <v>-100</v>
       </c>
       <c r="U7" t="n">
-        <v>-3.07</v>
+        <v>-7.47</v>
       </c>
       <c r="V7" t="inlineStr"/>
       <c r="W7" s="2" t="n">
-        <v>26.67</v>
-      </c>
-      <c r="X7" s="2" t="n">
-        <v>5.38</v>
+        <v>27.25</v>
+      </c>
+      <c r="X7" t="n">
+        <v>-7.83</v>
       </c>
       <c r="Y7" t="n">
         <v>-64.29000000000001</v>
       </c>
-      <c r="Z7" s="2" t="n">
-        <v>23.33</v>
+      <c r="Z7" t="n">
+        <v>-7.5</v>
       </c>
       <c r="AA7" t="n">
-        <v>-7.71</v>
+        <v>-9.65</v>
       </c>
       <c r="AB7" s="2" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -1086,84 +1078,84 @@
           <t>Denmark</t>
         </is>
       </c>
-      <c r="B8" s="2" t="n">
-        <v>8.84</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>75</v>
+      <c r="B8" t="n">
+        <v>-13.15</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-100</v>
       </c>
       <c r="D8" t="n">
-        <v>-22.68</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>7.05</v>
+        <v>-18.08</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-6.64</v>
       </c>
       <c r="F8" t="n">
-        <v>-23.7</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>6.94</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-1.35</v>
+        <v>-25.25</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-10.95</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0.9399999999999999</v>
       </c>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="n">
-        <v>-2.44</v>
+      <c r="J8" s="2" t="n">
+        <v>13.11</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>17.4</v>
-      </c>
-      <c r="L8" s="2" t="n">
-        <v>17.3</v>
+        <v>40.25</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-32.7</v>
       </c>
       <c r="M8" t="n">
-        <v>-16.69</v>
+        <v>-21.6</v>
       </c>
       <c r="N8" t="n">
         <v>-100</v>
       </c>
       <c r="O8" t="n">
-        <v>-8.039999999999999</v>
+        <v>-6.27</v>
       </c>
       <c r="P8" s="2" t="n">
-        <v>30.36</v>
-      </c>
-      <c r="Q8" s="2" t="n">
-        <v>17.38</v>
+        <v>19.17</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-8.06</v>
       </c>
       <c r="R8" s="2" t="n">
-        <v>21.9</v>
+        <v>13.62</v>
       </c>
       <c r="S8" s="2" t="n">
-        <v>22.75</v>
-      </c>
-      <c r="T8" t="n">
-        <v>-38</v>
+        <v>4.17</v>
+      </c>
+      <c r="T8" s="2" t="n">
+        <v>8.5</v>
       </c>
       <c r="U8" s="2" t="n">
-        <v>1.57</v>
+        <v>7.13</v>
       </c>
       <c r="V8" t="n">
-        <v>-24.25</v>
-      </c>
-      <c r="W8" s="2" t="n">
-        <v>19.71</v>
+        <v>-22</v>
+      </c>
+      <c r="W8" t="n">
+        <v>-0.37</v>
       </c>
       <c r="X8" t="n">
-        <v>-13.57</v>
+        <v>-6.84</v>
       </c>
       <c r="Y8" t="n">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="Z8" s="2" t="n">
-        <v>40.71</v>
+        <v>42.88</v>
       </c>
       <c r="AA8" s="2" t="n">
-        <v>15.13</v>
+        <v>1.42</v>
       </c>
       <c r="AB8" s="2" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">
@@ -1179,7 +1171,7 @@
         <v>-26.67</v>
       </c>
       <c r="D9" t="n">
-        <v>-18.38</v>
+        <v>-16.66</v>
       </c>
       <c r="E9" t="n">
         <v>-7.37</v>
@@ -1188,10 +1180,10 @@
         <v>8.91</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.45</v>
+        <v>-0.98</v>
       </c>
       <c r="H9" t="n">
-        <v>-3.38</v>
+        <v>-3.16</v>
       </c>
       <c r="I9" t="n">
         <v>-100</v>
@@ -1200,31 +1192,31 @@
         <v>-9.77</v>
       </c>
       <c r="K9" t="n">
-        <v>-7.04</v>
+        <v>-8.94</v>
       </c>
       <c r="L9" t="n">
         <v>-54.07</v>
       </c>
       <c r="M9" t="n">
-        <v>-7.34</v>
+        <v>-6.94</v>
       </c>
       <c r="N9" t="n">
         <v>-100</v>
       </c>
       <c r="O9" s="2" t="n">
-        <v>2.83</v>
+        <v>2.92</v>
       </c>
       <c r="P9" t="n">
         <v>-5.73</v>
       </c>
       <c r="Q9" t="n">
-        <v>-16.44</v>
+        <v>-14.27</v>
       </c>
       <c r="R9" t="n">
         <v>-12.46</v>
       </c>
-      <c r="S9" s="2" t="n">
-        <v>1.76</v>
+      <c r="S9" t="n">
+        <v>-0.67</v>
       </c>
       <c r="T9" s="2" t="n">
         <v>27.51</v>
@@ -1236,10 +1228,10 @@
         <v>22.83</v>
       </c>
       <c r="W9" t="n">
-        <v>-19.36</v>
+        <v>-18.65</v>
       </c>
       <c r="X9" s="2" t="n">
-        <v>2.76</v>
+        <v>3.02</v>
       </c>
       <c r="Y9" t="n">
         <v>-2.78</v>
@@ -1248,10 +1240,10 @@
         <v>1.65</v>
       </c>
       <c r="AA9" s="2" t="n">
-        <v>0.99</v>
+        <v>1.42</v>
       </c>
       <c r="AB9" s="2" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10">
@@ -1261,7 +1253,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-8.42</v>
+        <v>-7.74</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>13.46</v>
@@ -1270,7 +1262,7 @@
         <v>-19.16</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>1.34</v>
+        <v>1.51</v>
       </c>
       <c r="F10" t="n">
         <v>-1.93</v>
@@ -1279,7 +1271,7 @@
         <v>-0.11</v>
       </c>
       <c r="H10" t="n">
-        <v>-4.73</v>
+        <v>-4.57</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>6.29</v>
@@ -1288,26 +1280,26 @@
         <v>-9.19</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>6.59</v>
+        <v>5.98</v>
       </c>
       <c r="L10" t="n">
         <v>-24.33</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>2.28</v>
+        <v>1.88</v>
       </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" s="2" t="n">
-        <v>0.9</v>
+        <v>0.93</v>
       </c>
       <c r="P10" t="n">
         <v>-6.74</v>
       </c>
       <c r="Q10" t="n">
-        <v>-8.470000000000001</v>
+        <v>-9</v>
       </c>
       <c r="R10" s="2" t="n">
-        <v>5.89</v>
+        <v>7.77</v>
       </c>
       <c r="S10" t="n">
         <v>-9.880000000000001</v>
@@ -1315,15 +1307,15 @@
       <c r="T10" t="n">
         <v>-71.56</v>
       </c>
-      <c r="U10" t="n">
-        <v>-0.03</v>
+      <c r="U10" s="2" t="n">
+        <v>0.08</v>
       </c>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="n">
         <v>-15.23</v>
       </c>
       <c r="X10" t="n">
-        <v>-5.98</v>
+        <v>-5.77</v>
       </c>
       <c r="Y10" s="2" t="n">
         <v>3.96</v>
@@ -1332,10 +1324,10 @@
         <v>31.65</v>
       </c>
       <c r="AA10" t="n">
-        <v>-6.87</v>
+        <v>-7.24</v>
       </c>
       <c r="AB10" s="2" t="n">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11">
@@ -1345,73 +1337,73 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>1.12</v>
+        <v>2.01</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>49.85</v>
       </c>
       <c r="D11" t="n">
-        <v>-8.24</v>
+        <v>-6.57</v>
       </c>
       <c r="E11" t="n">
-        <v>-4</v>
+        <v>-2.86</v>
       </c>
       <c r="F11" t="n">
-        <v>-4.55</v>
+        <v>-3.86</v>
       </c>
       <c r="G11" t="n">
-        <v>-10.61</v>
+        <v>-11.25</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.88</v>
+        <v>-8.75</v>
       </c>
       <c r="I11" s="2" t="n">
         <v>0.62</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.8</v>
+        <v>-3.5</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>6.06</v>
+        <v>6.03</v>
       </c>
       <c r="L11" t="n">
         <v>-30.32</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>2.11</v>
+        <v>2.43</v>
       </c>
       <c r="N11" t="n">
         <v>-46.43</v>
       </c>
       <c r="O11" t="n">
-        <v>-1.93</v>
-      </c>
-      <c r="P11" s="2" t="n">
-        <v>1.03</v>
+        <v>-1.99</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-1.71</v>
       </c>
       <c r="Q11" s="2" t="n">
-        <v>3.06</v>
+        <v>3.28</v>
       </c>
       <c r="R11" t="n">
-        <v>-29.58</v>
+        <v>-31.97</v>
       </c>
       <c r="S11" t="n">
-        <v>-9.94</v>
+        <v>-11.97</v>
       </c>
       <c r="T11" t="n">
         <v>-3.07</v>
       </c>
       <c r="U11" t="n">
-        <v>-3.66</v>
+        <v>-3.88</v>
       </c>
       <c r="V11" s="2" t="n">
         <v>15</v>
       </c>
       <c r="W11" t="n">
-        <v>-12.22</v>
+        <v>-13.01</v>
       </c>
       <c r="X11" t="n">
-        <v>-9.1</v>
+        <v>-8.58</v>
       </c>
       <c r="Y11" t="n">
         <v>-17.21</v>
@@ -1420,10 +1412,10 @@
         <v>-2.63</v>
       </c>
       <c r="AA11" t="n">
-        <v>-2.8</v>
+        <v>-2.16</v>
       </c>
       <c r="AB11" s="2" t="n">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12">
@@ -1433,85 +1425,85 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-6.44</v>
+        <v>-9.210000000000001</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>61.67</v>
       </c>
       <c r="D12" t="n">
-        <v>-16.18</v>
+        <v>-18.72</v>
       </c>
       <c r="E12" t="n">
-        <v>-4.33</v>
+        <v>-4.45</v>
       </c>
       <c r="F12" t="n">
-        <v>-6.36</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>2.89</v>
+        <v>-7.01</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-0.62</v>
       </c>
       <c r="H12" t="n">
-        <v>-9.84</v>
+        <v>-11.77</v>
       </c>
       <c r="I12" t="n">
         <v>-28.18</v>
       </c>
       <c r="J12" t="n">
-        <v>-7.71</v>
+        <v>-9.880000000000001</v>
       </c>
       <c r="K12" t="n">
-        <v>-5.33</v>
+        <v>-4.41</v>
       </c>
       <c r="L12" s="2" t="n">
         <v>9.58</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>0.63</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="N12" s="2" t="n">
         <v>116.67</v>
       </c>
       <c r="O12" s="2" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="P12" t="n">
-        <v>-17.76</v>
+        <v>-19.51</v>
       </c>
       <c r="Q12" t="n">
-        <v>-15.52</v>
+        <v>-13.58</v>
       </c>
       <c r="R12" t="n">
-        <v>-6.33</v>
+        <v>-10.59</v>
       </c>
       <c r="S12" s="2" t="n">
-        <v>1.03</v>
+        <v>3.13</v>
       </c>
       <c r="T12" t="n">
         <v>-54</v>
       </c>
       <c r="U12" t="n">
-        <v>-6.29</v>
+        <v>-5.53</v>
       </c>
       <c r="V12" t="n">
         <v>-16</v>
       </c>
       <c r="W12" t="n">
-        <v>-9.619999999999999</v>
+        <v>-8.32</v>
       </c>
       <c r="X12" t="n">
-        <v>-12.06</v>
+        <v>-14.36</v>
       </c>
       <c r="Y12" t="n">
         <v>-32</v>
       </c>
       <c r="Z12" t="n">
-        <v>-13.67</v>
+        <v>-17.59</v>
       </c>
       <c r="AA12" t="n">
-        <v>-2.3</v>
+        <v>-1.7</v>
       </c>
       <c r="AB12" s="2" t="n">
-        <v>246</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13">
@@ -1521,85 +1513,85 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-14.84</v>
+        <v>-16.37</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D13" t="n">
-        <v>-19.44</v>
+        <v>-14.66</v>
       </c>
       <c r="E13" t="n">
-        <v>-6.07</v>
+        <v>-8.369999999999999</v>
       </c>
       <c r="F13" t="n">
-        <v>-11.71</v>
+        <v>-7.67</v>
       </c>
       <c r="G13" t="n">
-        <v>-4.17</v>
+        <v>-8.619999999999999</v>
       </c>
       <c r="H13" t="n">
-        <v>-4.07</v>
+        <v>-3.97</v>
       </c>
       <c r="I13" t="n">
         <v>-100</v>
       </c>
       <c r="J13" t="n">
-        <v>-13.5</v>
+        <v>-14.37</v>
       </c>
       <c r="K13" t="n">
-        <v>-17.75</v>
+        <v>-20.33</v>
       </c>
       <c r="L13" t="n">
-        <v>-56.5</v>
+        <v>-59.06</v>
       </c>
       <c r="M13" t="n">
-        <v>-7.76</v>
+        <v>-7.66</v>
       </c>
       <c r="N13" t="n">
         <v>-100</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.48</v>
+        <v>-0.76</v>
       </c>
       <c r="P13" t="n">
-        <v>-4.99</v>
+        <v>-7.54</v>
       </c>
       <c r="Q13" t="n">
-        <v>-24.11</v>
+        <v>-23.44</v>
       </c>
       <c r="R13" t="n">
-        <v>-13.24</v>
+        <v>-9.779999999999999</v>
       </c>
       <c r="S13" t="n">
-        <v>-13.28</v>
+        <v>-18.48</v>
       </c>
       <c r="T13" t="n">
-        <v>-3.65</v>
+        <v>-8.58</v>
       </c>
       <c r="U13" t="n">
-        <v>-10.07</v>
+        <v>-11.1</v>
       </c>
       <c r="V13" t="n">
         <v>-40</v>
       </c>
       <c r="W13" t="n">
-        <v>-3.97</v>
+        <v>-6.6</v>
       </c>
       <c r="X13" t="n">
-        <v>-1.98</v>
+        <v>-1.28</v>
       </c>
       <c r="Y13" t="n">
         <v>-24.91</v>
       </c>
       <c r="Z13" t="n">
-        <v>-20.63</v>
+        <v>-28.19</v>
       </c>
       <c r="AA13" t="n">
-        <v>-7.76</v>
+        <v>-6.67</v>
       </c>
       <c r="AB13" s="2" t="n">
-        <v>208</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14">
@@ -1609,64 +1601,64 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-2.19</v>
+        <v>-1.16</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>11.67</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>18.3</v>
+        <v>15.83</v>
       </c>
       <c r="E14" t="n">
-        <v>-12.33</v>
+        <v>-10.6</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0.27</v>
+        <v>1.52</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>1.21</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.63</v>
+        <v>-0.86</v>
       </c>
       <c r="I14" t="n">
         <v>-100</v>
       </c>
       <c r="J14" t="n">
-        <v>-2.96</v>
+        <v>-2.51</v>
       </c>
       <c r="K14" s="2" t="n">
-        <v>3.66</v>
+        <v>1.63</v>
       </c>
       <c r="L14" t="n">
         <v>-20.64</v>
       </c>
       <c r="M14" t="n">
-        <v>-3.96</v>
+        <v>-5.13</v>
       </c>
       <c r="N14" t="n">
         <v>-27.83</v>
       </c>
       <c r="O14" s="2" t="n">
-        <v>2.56</v>
+        <v>0.97</v>
       </c>
       <c r="P14" t="n">
-        <v>-19.77</v>
+        <v>-19.87</v>
       </c>
       <c r="Q14" t="n">
-        <v>-8.19</v>
+        <v>-11.94</v>
       </c>
       <c r="R14" t="n">
-        <v>-25.91</v>
+        <v>-29.13</v>
       </c>
       <c r="S14" t="n">
-        <v>-18.3</v>
+        <v>-16.82</v>
       </c>
       <c r="T14" t="n">
         <v>-3.39</v>
       </c>
       <c r="U14" t="n">
-        <v>-15.94</v>
+        <v>-17.19</v>
       </c>
       <c r="V14" s="2" t="n">
         <v>62.67</v>
@@ -1675,19 +1667,19 @@
         <v>-12.52</v>
       </c>
       <c r="X14" t="n">
-        <v>-5.03</v>
+        <v>-6.32</v>
       </c>
       <c r="Y14" t="n">
         <v>-100</v>
       </c>
       <c r="Z14" s="2" t="n">
-        <v>24.64</v>
+        <v>20.34</v>
       </c>
       <c r="AA14" t="n">
-        <v>-0.45</v>
+        <v>-0.61</v>
       </c>
       <c r="AB14" s="2" t="n">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15">
@@ -1697,73 +1689,73 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>19.01</v>
+        <v>19.92</v>
       </c>
       <c r="C15" t="n">
         <v>-100</v>
       </c>
       <c r="D15" t="n">
-        <v>-21.07</v>
+        <v>-23.57</v>
       </c>
       <c r="E15" t="n">
-        <v>-4.64</v>
+        <v>-4.21</v>
       </c>
       <c r="F15" t="n">
-        <v>-3.25</v>
+        <v>-3.96</v>
       </c>
       <c r="G15" t="n">
         <v>-29.67</v>
       </c>
       <c r="H15" t="n">
-        <v>-10.18</v>
+        <v>-9.27</v>
       </c>
       <c r="I15" t="n">
         <v>-5.88</v>
       </c>
       <c r="J15" t="n">
-        <v>-18.34</v>
+        <v>-19.66</v>
       </c>
       <c r="K15" t="n">
-        <v>-10.93</v>
+        <v>-9</v>
       </c>
       <c r="L15" t="n">
         <v>-19.8</v>
       </c>
       <c r="M15" t="n">
-        <v>-7.42</v>
+        <v>-6.21</v>
       </c>
       <c r="N15" t="n">
         <v>-100</v>
       </c>
       <c r="O15" t="n">
-        <v>-3.62</v>
+        <v>-3.23</v>
       </c>
       <c r="P15" t="n">
-        <v>-20.73</v>
+        <v>-18.78</v>
       </c>
       <c r="Q15" s="2" t="n">
-        <v>2.94</v>
+        <v>2.96</v>
       </c>
       <c r="R15" s="2" t="n">
         <v>3.58</v>
       </c>
       <c r="S15" t="n">
-        <v>-8.35</v>
+        <v>-11.33</v>
       </c>
       <c r="T15" t="n">
-        <v>-17</v>
+        <v>-19.24</v>
       </c>
       <c r="U15" t="n">
-        <v>-4.16</v>
+        <v>-3.21</v>
       </c>
       <c r="V15" s="2" t="n">
-        <v>7.65</v>
+        <v>3.67</v>
       </c>
       <c r="W15" t="n">
-        <v>-9.98</v>
+        <v>-10.63</v>
       </c>
       <c r="X15" t="n">
-        <v>-1.13</v>
+        <v>-0.24</v>
       </c>
       <c r="Y15" t="n">
         <v>-32.25</v>
@@ -1772,10 +1764,10 @@
         <v>-9.24</v>
       </c>
       <c r="AA15" t="n">
-        <v>-2.86</v>
+        <v>-3.21</v>
       </c>
       <c r="AB15" s="2" t="n">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16">
@@ -1785,83 +1777,85 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-28.95</v>
+        <v>-28</v>
       </c>
       <c r="C16" t="n">
         <v>-78.33</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2.65</v>
+        <v>3.14</v>
       </c>
       <c r="E16" t="n">
-        <v>-7.33</v>
+        <v>-9.289999999999999</v>
       </c>
       <c r="F16" t="n">
-        <v>-19.09</v>
+        <v>-17</v>
       </c>
       <c r="G16" t="n">
-        <v>-13.04</v>
+        <v>-12.02</v>
       </c>
       <c r="H16" t="n">
-        <v>-10.51</v>
+        <v>-9.76</v>
       </c>
       <c r="I16" s="2" t="n">
         <v>37.5</v>
       </c>
       <c r="J16" t="n">
-        <v>-19.46</v>
+        <v>-16.76</v>
       </c>
       <c r="K16" t="n">
         <v>-11.88</v>
       </c>
       <c r="L16" t="n">
-        <v>-34</v>
+        <v>-28</v>
       </c>
       <c r="M16" t="n">
-        <v>-7.9</v>
+        <v>-10.1</v>
       </c>
       <c r="N16" t="n">
         <v>-62.64</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.99</v>
+        <v>-1.47</v>
       </c>
       <c r="P16" t="n">
-        <v>-9.09</v>
+        <v>-7.59</v>
       </c>
       <c r="Q16" s="2" t="n">
-        <v>6</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="R16" t="n">
-        <v>-24.5</v>
+        <v>-21.47</v>
       </c>
       <c r="S16" t="n">
         <v>-12.19</v>
       </c>
       <c r="T16" s="2" t="n">
-        <v>8.27</v>
+        <v>5.09</v>
       </c>
       <c r="U16" t="n">
-        <v>-7.88</v>
-      </c>
-      <c r="V16" t="inlineStr"/>
+        <v>-7.66</v>
+      </c>
+      <c r="V16" s="2" t="n">
+        <v>57</v>
+      </c>
       <c r="W16" s="2" t="n">
-        <v>3.13</v>
+        <v>1.49</v>
       </c>
       <c r="X16" t="n">
-        <v>-9.24</v>
+        <v>-9.369999999999999</v>
       </c>
       <c r="Y16" t="n">
         <v>-44.58</v>
       </c>
       <c r="Z16" t="n">
-        <v>-9.779999999999999</v>
+        <v>-9.039999999999999</v>
       </c>
       <c r="AA16" t="n">
-        <v>-7.71</v>
+        <v>-4.83</v>
       </c>
       <c r="AB16" s="2" t="n">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17">
@@ -1871,49 +1865,49 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-12.41</v>
+        <v>-13.31</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>8.33</v>
       </c>
       <c r="D17" t="n">
-        <v>-5.07</v>
+        <v>-6.8</v>
       </c>
       <c r="E17" t="n">
-        <v>-4.07</v>
+        <v>-3.69</v>
       </c>
       <c r="F17" t="n">
         <v>-8.18</v>
       </c>
       <c r="G17" t="n">
-        <v>-5.75</v>
+        <v>-8.300000000000001</v>
       </c>
       <c r="H17" t="n">
-        <v>-7.71</v>
+        <v>-8.050000000000001</v>
       </c>
       <c r="I17" t="n">
         <v>-100</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.19</v>
+        <v>-1.12</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>12.26</v>
+        <v>9.92</v>
       </c>
       <c r="L17" s="2" t="n">
         <v>12.18</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>5.87</v>
+        <v>6.47</v>
       </c>
       <c r="N17" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="O17" t="n">
-        <v>-0.18</v>
+      <c r="O17" s="2" t="n">
+        <v>0.02</v>
       </c>
       <c r="P17" t="n">
-        <v>-5.38</v>
+        <v>-5.46</v>
       </c>
       <c r="Q17" s="2" t="n">
         <v>10.51</v>
@@ -1922,13 +1916,13 @@
         <v>13.88</v>
       </c>
       <c r="S17" s="2" t="n">
-        <v>19.19</v>
+        <v>21.94</v>
       </c>
       <c r="T17" t="n">
         <v>-4.14</v>
       </c>
       <c r="U17" s="2" t="n">
-        <v>5.49</v>
+        <v>5.95</v>
       </c>
       <c r="V17" s="2" t="n">
         <v>21.2</v>
@@ -1937,7 +1931,7 @@
         <v>-3.41</v>
       </c>
       <c r="X17" t="n">
-        <v>-9.76</v>
+        <v>-11.04</v>
       </c>
       <c r="Y17" t="n">
         <v>-73.84999999999999</v>
@@ -1946,10 +1940,10 @@
         <v>24.59</v>
       </c>
       <c r="AA17" t="n">
-        <v>-2.86</v>
+        <v>-2.04</v>
       </c>
       <c r="AB17" s="2" t="n">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18">
@@ -1958,81 +1952,81 @@
           <t>Greece</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>-6.53</v>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>14.58</v>
+      <c r="B18" s="2" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-20.42</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>31.47</v>
+        <v>18.76</v>
       </c>
       <c r="E18" t="n">
-        <v>-19.06</v>
-      </c>
-      <c r="F18" t="n">
-        <v>-0.5600000000000001</v>
+        <v>-30.76</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>7.75</v>
       </c>
       <c r="G18" t="n">
-        <v>-2.49</v>
+        <v>-3.57</v>
       </c>
       <c r="H18" t="n">
-        <v>-7.72</v>
+        <v>-6.5</v>
       </c>
       <c r="I18" t="n">
-        <v>-11.6</v>
+        <v>-48.44</v>
       </c>
       <c r="J18" s="2" t="n">
-        <v>19.83</v>
+        <v>38.17</v>
       </c>
       <c r="K18" t="n">
-        <v>-1.11</v>
+        <v>-16.81</v>
       </c>
       <c r="L18" s="2" t="n">
         <v>112.6</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>8.460000000000001</v>
+        <v>3.95</v>
       </c>
       <c r="N18" s="2" t="n">
         <v>800</v>
       </c>
       <c r="O18" t="n">
-        <v>-1.55</v>
+        <v>-4.11</v>
       </c>
       <c r="P18" s="2" t="n">
-        <v>21.83</v>
+        <v>13.35</v>
       </c>
       <c r="Q18" t="n">
-        <v>-4.14</v>
+        <v>-9.050000000000001</v>
       </c>
       <c r="R18" t="n">
         <v>-18.83</v>
       </c>
-      <c r="S18" s="2" t="n">
-        <v>3.89</v>
+      <c r="S18" t="n">
+        <v>-6.27</v>
       </c>
       <c r="T18" t="n">
         <v>-8.33</v>
       </c>
       <c r="U18" t="n">
-        <v>-11</v>
+        <v>-14.04</v>
       </c>
       <c r="V18" t="inlineStr"/>
       <c r="W18" t="n">
-        <v>-0.32</v>
+        <v>-7.97</v>
       </c>
       <c r="X18" t="n">
-        <v>-11.11</v>
+        <v>-4.63</v>
       </c>
       <c r="Y18" t="n">
-        <v>-38.16</v>
+        <v>-41.04</v>
       </c>
       <c r="Z18" s="2" t="n">
-        <v>24.17</v>
+        <v>52.5</v>
       </c>
       <c r="AA18" t="n">
-        <v>-5.38</v>
+        <v>-10.23</v>
       </c>
       <c r="AB18" s="2" t="n">
         <v>86</v>
@@ -2045,22 +2039,22 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-4.45</v>
+        <v>-3.84</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>17.14</v>
       </c>
       <c r="D19" t="n">
-        <v>-12.55</v>
+        <v>-15.09</v>
       </c>
       <c r="E19" t="n">
-        <v>-7.71</v>
-      </c>
-      <c r="F19" t="n">
-        <v>-0.85</v>
+        <v>-7.5</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>1.79</v>
       </c>
       <c r="G19" t="n">
-        <v>-2.82</v>
+        <v>-4.25</v>
       </c>
       <c r="H19" t="n">
         <v>-7.81</v>
@@ -2069,49 +2063,49 @@
         <v>-51.43</v>
       </c>
       <c r="J19" t="n">
-        <v>-15.27</v>
+        <v>-13.45</v>
       </c>
       <c r="K19" t="n">
-        <v>-4.35</v>
+        <v>-4.36</v>
       </c>
       <c r="L19" s="2" t="n">
         <v>24.39</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>0.83</v>
+        <v>0.52</v>
       </c>
       <c r="N19" s="2" t="n">
         <v>211</v>
       </c>
       <c r="O19" t="n">
-        <v>-3.32</v>
+        <v>-3.75</v>
       </c>
       <c r="P19" t="n">
-        <v>-10.92</v>
+        <v>-12.12</v>
       </c>
       <c r="Q19" t="n">
-        <v>-13.98</v>
+        <v>-12.16</v>
       </c>
       <c r="R19" t="n">
         <v>-35.23</v>
       </c>
       <c r="S19" t="n">
-        <v>-9.65</v>
+        <v>-10.11</v>
       </c>
       <c r="T19" s="2" t="n">
         <v>23.94</v>
       </c>
       <c r="U19" t="n">
-        <v>-12.1</v>
+        <v>-11.84</v>
       </c>
       <c r="V19" t="n">
         <v>-100</v>
       </c>
-      <c r="W19" s="2" t="n">
-        <v>0.72</v>
+      <c r="W19" t="n">
+        <v>-1.65</v>
       </c>
       <c r="X19" t="n">
-        <v>-5.54</v>
+        <v>-5.44</v>
       </c>
       <c r="Y19" t="n">
         <v>-43</v>
@@ -2120,10 +2114,10 @@
         <v>-35.63</v>
       </c>
       <c r="AA19" t="n">
-        <v>-0.85</v>
+        <v>-1.04</v>
       </c>
       <c r="AB19" s="2" t="n">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20">
@@ -2133,7 +2127,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-13.7</v>
+        <v>-14.23</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>18.46</v>
@@ -2142,7 +2136,7 @@
         <v>-10.26</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.82</v>
+        <v>-0.68</v>
       </c>
       <c r="F20" t="n">
         <v>-18.8</v>
@@ -2151,55 +2145,55 @@
         <v>8.15</v>
       </c>
       <c r="H20" t="n">
-        <v>-5.44</v>
+        <v>-4.95</v>
       </c>
       <c r="I20" t="n">
         <v>-18.33</v>
       </c>
       <c r="J20" t="n">
-        <v>-19.82</v>
+        <v>-14.91</v>
       </c>
       <c r="K20" t="n">
-        <v>-2.93</v>
+        <v>-3.76</v>
       </c>
       <c r="L20" t="n">
         <v>-50</v>
       </c>
       <c r="M20" t="n">
-        <v>-6.63</v>
+        <v>-8.48</v>
       </c>
       <c r="N20" t="n">
         <v>-100</v>
       </c>
       <c r="O20" t="n">
-        <v>-3.12</v>
+        <v>-2.84</v>
       </c>
       <c r="P20" t="n">
-        <v>-10.09</v>
+        <v>-6.97</v>
       </c>
       <c r="Q20" t="n">
-        <v>-14.78</v>
-      </c>
-      <c r="R20" s="2" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="S20" s="2" t="n">
-        <v>0.19</v>
+        <v>-14.01</v>
+      </c>
+      <c r="R20" t="n">
+        <v>-1.49</v>
+      </c>
+      <c r="S20" t="n">
+        <v>-2.87</v>
       </c>
       <c r="T20" t="n">
         <v>-65.91</v>
       </c>
       <c r="U20" t="n">
-        <v>-1.45</v>
+        <v>-2.81</v>
       </c>
       <c r="V20" s="2" t="n">
         <v>32.22</v>
       </c>
       <c r="W20" t="n">
-        <v>-2.43</v>
+        <v>-3.95</v>
       </c>
       <c r="X20" t="n">
-        <v>-2.84</v>
+        <v>-1.38</v>
       </c>
       <c r="Y20" t="n">
         <v>-32</v>
@@ -2208,10 +2202,10 @@
         <v>39.19</v>
       </c>
       <c r="AA20" t="n">
-        <v>-9.369999999999999</v>
+        <v>-8.99</v>
       </c>
       <c r="AB20" s="2" t="n">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21">
@@ -2307,47 +2301,47 @@
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>14.61</v>
+        <v>15.5</v>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>-41.29</v>
+        <v>-33.73</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>11.67</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>4.59</v>
+        <v>6.17</v>
       </c>
       <c r="G22" t="n">
         <v>-48.36</v>
       </c>
-      <c r="H22" t="n">
-        <v>0</v>
+      <c r="H22" s="2" t="n">
+        <v>0.8</v>
       </c>
       <c r="I22" t="n">
         <v>-100</v>
       </c>
       <c r="J22" s="2" t="n">
-        <v>27.22</v>
+        <v>30.34</v>
       </c>
       <c r="K22" t="n">
         <v>-20.93</v>
       </c>
       <c r="L22" t="n">
-        <v>-18.56</v>
+        <v>-6.7</v>
       </c>
       <c r="M22" t="n">
-        <v>-5.64</v>
+        <v>-7.7</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>87.5</v>
       </c>
       <c r="O22" t="n">
-        <v>-3.88</v>
+        <v>-5.44</v>
       </c>
       <c r="P22" s="2" t="n">
-        <v>8.720000000000001</v>
+        <v>13.15</v>
       </c>
       <c r="Q22" t="n">
         <v>-34.34</v>
@@ -2356,32 +2350,32 @@
         <v>-33.25</v>
       </c>
       <c r="S22" t="n">
-        <v>-22.03</v>
+        <v>-20.67</v>
       </c>
       <c r="T22" t="n">
         <v>-100</v>
       </c>
       <c r="U22" t="n">
-        <v>-1.38</v>
+        <v>-0.97</v>
       </c>
       <c r="V22" t="inlineStr"/>
       <c r="W22" t="n">
-        <v>-35.9</v>
+        <v>-33</v>
       </c>
       <c r="X22" s="2" t="n">
-        <v>6.22</v>
+        <v>4.51</v>
       </c>
       <c r="Y22" t="n">
         <v>-100</v>
       </c>
       <c r="Z22" s="2" t="n">
-        <v>10.5</v>
+        <v>14.83</v>
       </c>
       <c r="AA22" t="n">
-        <v>-25.37</v>
+        <v>-23.61</v>
       </c>
       <c r="AB22" s="2" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23">
@@ -2479,14 +2473,14 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-4.5</v>
+        <v>-3</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" s="2" t="n">
         <v>28.27</v>
       </c>
       <c r="E24" t="n">
-        <v>-6.25</v>
+        <v>-4.62</v>
       </c>
       <c r="F24" t="n">
         <v>-1.15</v>
@@ -2495,33 +2489,33 @@
         <v>19.33</v>
       </c>
       <c r="H24" t="n">
-        <v>-13.88</v>
+        <v>-15.34</v>
       </c>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="n">
-        <v>-0.6899999999999999</v>
+        <v>-3.38</v>
       </c>
       <c r="K24" s="2" t="n">
         <v>36.68</v>
       </c>
       <c r="L24" t="n">
-        <v>-5.33</v>
+        <v>-18.86</v>
       </c>
       <c r="M24" s="2" t="n">
         <v>12.42</v>
       </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" s="2" t="n">
-        <v>0.76</v>
+        <v>1.42</v>
       </c>
       <c r="P24" t="n">
-        <v>-21.34</v>
+        <v>-23.97</v>
       </c>
       <c r="Q24" s="2" t="n">
         <v>12.76</v>
       </c>
-      <c r="R24" s="2" t="n">
-        <v>2.88</v>
+      <c r="R24" t="n">
+        <v>-8.56</v>
       </c>
       <c r="S24" t="n">
         <v>-16.87</v>
@@ -2530,14 +2524,14 @@
         <v>-42.5</v>
       </c>
       <c r="U24" t="n">
-        <v>-11.63</v>
+        <v>-10.92</v>
       </c>
       <c r="V24" t="inlineStr"/>
       <c r="W24" s="2" t="n">
         <v>2.65</v>
       </c>
       <c r="X24" t="n">
-        <v>-11.19</v>
+        <v>-12.72</v>
       </c>
       <c r="Y24" t="n">
         <v>-100</v>
@@ -2546,10 +2540,10 @@
         <v>-26.67</v>
       </c>
       <c r="AA24" s="2" t="n">
-        <v>3.13</v>
+        <v>4.68</v>
       </c>
       <c r="AB24" s="2" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25">
@@ -2559,81 +2553,81 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-12.97</v>
+        <v>-13.97</v>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" s="2" t="n">
-        <v>22.56</v>
+        <v>17.11</v>
       </c>
       <c r="E25" t="n">
-        <v>-6.92</v>
+        <v>-8.710000000000001</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>4.93</v>
+        <v>3.56</v>
       </c>
       <c r="G25" s="2" t="n">
         <v>6.1</v>
       </c>
       <c r="H25" t="n">
-        <v>-9.59</v>
+        <v>-8.51</v>
       </c>
       <c r="I25" t="n">
         <v>-34.79</v>
       </c>
       <c r="J25" t="n">
-        <v>-10.47</v>
+        <v>-8.869999999999999</v>
       </c>
       <c r="K25" t="n">
-        <v>-3.32</v>
+        <v>-1.61</v>
       </c>
       <c r="L25" t="n">
         <v>-17.86</v>
       </c>
       <c r="M25" t="n">
-        <v>-1.55</v>
+        <v>-0.85</v>
       </c>
       <c r="N25" t="n">
         <v>-100</v>
       </c>
       <c r="O25" t="n">
-        <v>-2.73</v>
+        <v>-2.47</v>
       </c>
       <c r="P25" t="n">
-        <v>-19.94</v>
+        <v>-18.43</v>
       </c>
       <c r="Q25" t="n">
-        <v>-11.62</v>
+        <v>-11.74</v>
       </c>
       <c r="R25" t="n">
-        <v>-3.35</v>
+        <v>-10.25</v>
       </c>
       <c r="S25" t="n">
-        <v>-33.48</v>
+        <v>-34.18</v>
       </c>
       <c r="T25" t="n">
         <v>-2.67</v>
       </c>
       <c r="U25" t="n">
-        <v>-9.970000000000001</v>
+        <v>-10.56</v>
       </c>
       <c r="V25" t="inlineStr"/>
       <c r="W25" t="n">
-        <v>-9.359999999999999</v>
+        <v>-10.95</v>
       </c>
       <c r="X25" s="2" t="n">
-        <v>6.08</v>
+        <v>6.73</v>
       </c>
       <c r="Y25" t="n">
-        <v>-22.17</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>-4.3</v>
+        <v>-26.26</v>
+      </c>
+      <c r="Z25" s="2" t="n">
+        <v>3.67</v>
       </c>
       <c r="AA25" t="n">
-        <v>-7.29</v>
+        <v>-7.77</v>
       </c>
       <c r="AB25" s="2" t="n">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26">
@@ -2643,81 +2637,81 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-3.97</v>
+        <v>-3.41</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>8.33</v>
       </c>
       <c r="D26" t="n">
-        <v>-22.21</v>
+        <v>-21.24</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>3.02</v>
+        <v>3.41</v>
       </c>
       <c r="F26" t="n">
-        <v>-5.9</v>
+        <v>-8.41</v>
       </c>
       <c r="G26" t="n">
-        <v>-10.3</v>
+        <v>-9.359999999999999</v>
       </c>
       <c r="H26" t="n">
-        <v>-5.37</v>
+        <v>-4.63</v>
       </c>
       <c r="I26" t="n">
         <v>-18.71</v>
       </c>
       <c r="J26" s="2" t="n">
-        <v>7.45</v>
+        <v>7.79</v>
       </c>
       <c r="K26" s="2" t="n">
-        <v>1.96</v>
+        <v>2.28</v>
       </c>
       <c r="L26" s="2" t="n">
         <v>22.37</v>
       </c>
       <c r="M26" t="n">
-        <v>-2.19</v>
+        <v>-2.95</v>
       </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>-2.52</v>
+        <v>-2.88</v>
       </c>
       <c r="P26" s="2" t="n">
-        <v>32.94</v>
+        <v>38.2</v>
       </c>
       <c r="Q26" t="n">
-        <v>-7.39</v>
+        <v>-6.13</v>
       </c>
       <c r="R26" s="2" t="n">
-        <v>2.79</v>
+        <v>7.12</v>
       </c>
       <c r="S26" s="2" t="n">
-        <v>12.94</v>
+        <v>8.1</v>
       </c>
       <c r="T26" t="n">
-        <v>-27.75</v>
+        <v>-11.36</v>
       </c>
       <c r="U26" t="n">
-        <v>-3.74</v>
+        <v>-2.64</v>
       </c>
       <c r="V26" t="inlineStr"/>
       <c r="W26" t="n">
-        <v>-15.4</v>
+        <v>-14.33</v>
       </c>
       <c r="X26" t="n">
-        <v>-8.67</v>
+        <v>-5.71</v>
       </c>
       <c r="Y26" s="2" t="n">
         <v>24.21</v>
       </c>
       <c r="Z26" s="2" t="n">
-        <v>45.62</v>
+        <v>39</v>
       </c>
       <c r="AA26" s="2" t="n">
-        <v>0.18</v>
+        <v>1.93</v>
       </c>
       <c r="AB26" s="2" t="n">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27">
@@ -2727,83 +2721,83 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>3.18</v>
+        <v>5.27</v>
       </c>
       <c r="C27" t="n">
         <v>-82.78</v>
       </c>
       <c r="D27" t="n">
-        <v>-18.42</v>
+        <v>-14.67</v>
       </c>
       <c r="E27" t="n">
-        <v>-1.47</v>
+        <v>-0.87</v>
       </c>
       <c r="F27" t="n">
         <v>-13.35</v>
       </c>
-      <c r="G27" t="n">
-        <v>-0.73</v>
+      <c r="G27" s="2" t="n">
+        <v>0.48</v>
       </c>
       <c r="H27" t="n">
-        <v>-3.06</v>
+        <v>-3.28</v>
       </c>
       <c r="I27" s="2" t="n">
         <v>20.63</v>
       </c>
       <c r="J27" t="n">
-        <v>-27.89</v>
+        <v>-25.74</v>
       </c>
       <c r="K27" t="n">
-        <v>-19.18</v>
+        <v>-19.14</v>
       </c>
       <c r="L27" t="n">
         <v>-53.12</v>
       </c>
       <c r="M27" t="n">
-        <v>-0.82</v>
+        <v>-1.15</v>
       </c>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>-2.58</v>
+        <v>-2.33</v>
       </c>
       <c r="P27" t="n">
         <v>-16.34</v>
       </c>
       <c r="Q27" t="n">
-        <v>-24.83</v>
+        <v>-25.45</v>
       </c>
       <c r="R27" s="2" t="n">
-        <v>20.03</v>
+        <v>22.6</v>
       </c>
       <c r="S27" t="n">
-        <v>-12.74</v>
+        <v>-12.27</v>
       </c>
       <c r="T27" t="n">
         <v>-39.32</v>
       </c>
       <c r="U27" t="n">
-        <v>-1</v>
+        <v>-0.64</v>
       </c>
       <c r="V27" t="n">
         <v>-10</v>
       </c>
       <c r="W27" s="2" t="n">
-        <v>5.24</v>
+        <v>5.76</v>
       </c>
       <c r="X27" s="2" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="Y27" s="2" t="n">
-        <v>0.93</v>
+        <v>1.05</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>-5.37</v>
       </c>
       <c r="Z27" s="2" t="n">
         <v>21.47</v>
       </c>
       <c r="AA27" t="n">
-        <v>-7.15</v>
+        <v>-7.23</v>
       </c>
       <c r="AB27" s="2" t="n">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28">
@@ -2817,7 +2811,7 @@
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="n">
-        <v>-11</v>
+        <v>-5.15</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>4.29</v>
@@ -2825,8 +2819,8 @@
       <c r="F28" t="n">
         <v>-3.47</v>
       </c>
-      <c r="G28" t="n">
-        <v>-45</v>
+      <c r="G28" s="2" t="n">
+        <v>6.5</v>
       </c>
       <c r="H28" s="2" t="n">
         <v>1.33</v>
@@ -2854,7 +2848,7 @@
         <v>22.39</v>
       </c>
       <c r="Q28" t="n">
-        <v>-23.48</v>
+        <v>-15.62</v>
       </c>
       <c r="R28" t="n">
         <v>-2.21</v>
@@ -2870,10 +2864,10 @@
       </c>
       <c r="V28" t="inlineStr"/>
       <c r="W28" t="n">
-        <v>-28.06</v>
+        <v>-21.5</v>
       </c>
       <c r="X28" t="n">
-        <v>-8.08</v>
+        <v>-11.38</v>
       </c>
       <c r="Y28" s="2" t="n">
         <v>156.5</v>
@@ -2894,82 +2888,82 @@
           <t>Scotland</t>
         </is>
       </c>
-      <c r="B29" s="2" t="n">
-        <v>12.74</v>
+      <c r="B29" t="n">
+        <v>-8.41</v>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="n">
-        <v>-10.82</v>
+        <v>-16</v>
       </c>
       <c r="E29" t="n">
-        <v>-7.78</v>
-      </c>
-      <c r="F29" t="n">
-        <v>-11.53</v>
+        <v>-21.61</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>0.09</v>
       </c>
       <c r="G29" t="n">
-        <v>-15.36</v>
-      </c>
-      <c r="H29" t="n">
-        <v>-4.33</v>
+        <v>-12.71</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>1.1</v>
       </c>
       <c r="I29" t="n">
         <v>-100</v>
       </c>
       <c r="J29" s="2" t="n">
-        <v>2.23</v>
+        <v>12.74</v>
       </c>
       <c r="K29" t="n">
-        <v>-9.109999999999999</v>
+        <v>-28.78</v>
       </c>
       <c r="L29" t="n">
-        <v>-26.43</v>
+        <v>-24.86</v>
       </c>
       <c r="M29" t="n">
-        <v>-11.93</v>
+        <v>-26.26</v>
       </c>
       <c r="N29" s="2" t="n">
         <v>138</v>
       </c>
       <c r="O29" t="n">
-        <v>-9.140000000000001</v>
-      </c>
-      <c r="P29" t="n">
-        <v>-0.38</v>
+        <v>-12.84</v>
+      </c>
+      <c r="P29" s="2" t="n">
+        <v>11.76</v>
       </c>
       <c r="Q29" t="n">
-        <v>-13.98</v>
+        <v>-22.7</v>
       </c>
       <c r="R29" t="n">
-        <v>-10.67</v>
+        <v>-7.67</v>
       </c>
       <c r="S29" t="n">
-        <v>-21.71</v>
+        <v>-21.92</v>
       </c>
       <c r="T29" t="n">
-        <v>-6.67</v>
+        <v>-3.42</v>
       </c>
       <c r="U29" t="n">
-        <v>-15.49</v>
+        <v>-24.39</v>
       </c>
       <c r="V29" t="inlineStr"/>
       <c r="W29" t="n">
-        <v>-20.59</v>
-      </c>
-      <c r="X29" t="n">
-        <v>-0.28</v>
+        <v>-19.22</v>
+      </c>
+      <c r="X29" s="2" t="n">
+        <v>13.71</v>
       </c>
       <c r="Y29" s="2" t="n">
-        <v>3.12</v>
-      </c>
-      <c r="Z29" s="2" t="n">
-        <v>0.88</v>
+        <v>36</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>-15.25</v>
       </c>
       <c r="AA29" t="n">
-        <v>-10.87</v>
+        <v>-25.49</v>
       </c>
       <c r="AB29" s="2" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30">
@@ -2981,55 +2975,55 @@
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
-        <v>-36.84</v>
+        <v>-5.79</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
-      <c r="G30" t="n">
-        <v>-1.63</v>
+      <c r="G30" s="2" t="n">
+        <v>27.16</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>12.64</v>
-      </c>
-      <c r="I30" t="n">
-        <v>-100</v>
+        <v>3.43</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>55</v>
       </c>
       <c r="J30" s="2" t="n">
-        <v>26.43</v>
-      </c>
-      <c r="K30" t="n">
-        <v>-60.4</v>
+        <v>28.71</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>21.8</v>
       </c>
       <c r="L30" s="2" t="n">
-        <v>25</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="n">
-        <v>-42.11</v>
+        <v>-34.21</v>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" s="2" t="n">
         <v>3.86</v>
       </c>
       <c r="Q30" t="n">
-        <v>-41.58</v>
+        <v>-19.92</v>
       </c>
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr"/>
       <c r="T30" s="2" t="n">
-        <v>29.37</v>
+        <v>79.11</v>
       </c>
       <c r="U30" t="inlineStr"/>
       <c r="V30" t="inlineStr"/>
-      <c r="W30" t="n">
-        <v>-7.74</v>
+      <c r="W30" s="2" t="n">
+        <v>12.42</v>
       </c>
       <c r="X30" t="inlineStr"/>
       <c r="Y30" t="n">
-        <v>-24.32</v>
+        <v>-18.42</v>
       </c>
       <c r="Z30" s="2" t="n">
-        <v>32.95</v>
+        <v>6.63</v>
       </c>
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" s="2" t="n">
@@ -3044,56 +3038,56 @@
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
-      <c r="D31" s="2" t="n">
-        <v>5</v>
+      <c r="D31" t="n">
+        <v>-42.17</v>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="n">
-        <v>-3.22</v>
+        <v>-26.52</v>
       </c>
       <c r="H31" s="2" t="n">
         <v>15.44</v>
       </c>
       <c r="I31" t="n">
-        <v>-25</v>
+        <v>-100</v>
       </c>
       <c r="J31" s="2" t="n">
-        <v>31.44</v>
+        <v>32</v>
       </c>
       <c r="K31" t="n">
-        <v>-10</v>
+        <v>-56</v>
       </c>
       <c r="L31" t="n">
-        <v>-17.91</v>
+        <v>-7.04</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="n">
-        <v>-23.91</v>
+        <v>-43.48</v>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" s="2" t="n">
         <v>74.83</v>
       </c>
       <c r="Q31" t="n">
-        <v>-12.53</v>
+        <v>-13.12</v>
       </c>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="n">
-        <v>-25</v>
+        <v>-23.91</v>
       </c>
       <c r="U31" t="inlineStr"/>
       <c r="V31" t="inlineStr"/>
       <c r="W31" t="n">
-        <v>-21.22</v>
+        <v>-34.43</v>
       </c>
       <c r="X31" t="inlineStr"/>
       <c r="Y31" t="n">
-        <v>-22.83</v>
+        <v>-49.43</v>
       </c>
       <c r="Z31" s="2" t="n">
-        <v>13.17</v>
+        <v>27.43</v>
       </c>
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" s="2" t="n">
@@ -3109,55 +3103,55 @@
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="n">
-        <v>-58.46</v>
+        <v>-38.23</v>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="n">
-        <v>-35.23</v>
+        <v>-38.85</v>
       </c>
       <c r="H32" s="2" t="n">
         <v>6.09</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>275</v>
-      </c>
-      <c r="J32" s="2" t="n">
-        <v>27.82</v>
+        <v>100</v>
+      </c>
+      <c r="J32" t="n">
+        <v>-30.18</v>
       </c>
       <c r="K32" s="2" t="n">
         <v>94</v>
       </c>
-      <c r="L32" s="2" t="n">
-        <v>40.38</v>
+      <c r="L32" t="n">
+        <v>-46.15</v>
       </c>
       <c r="M32" t="inlineStr"/>
-      <c r="N32" s="2" t="n">
-        <v>103.85</v>
+      <c r="N32" t="n">
+        <v>-57.69</v>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="n">
         <v>-6.75</v>
       </c>
-      <c r="Q32" t="n">
-        <v>-14</v>
+      <c r="Q32" s="2" t="n">
+        <v>47.56</v>
       </c>
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="n">
-        <v>-50.77</v>
+        <v>-25.77</v>
       </c>
       <c r="U32" t="inlineStr"/>
       <c r="V32" t="inlineStr"/>
       <c r="W32" t="n">
-        <v>-45</v>
+        <v>-36.08</v>
       </c>
       <c r="X32" t="inlineStr"/>
       <c r="Y32" t="n">
-        <v>-34.62</v>
-      </c>
-      <c r="Z32" s="2" t="n">
-        <v>44.62</v>
+        <v>-35.54</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>-30.77</v>
       </c>
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" s="2" t="n">
@@ -3171,85 +3165,85 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-13.61</v>
+        <v>-14.03</v>
       </c>
       <c r="C33" t="n">
-        <v>-48.7</v>
+        <v>-50.83</v>
       </c>
       <c r="D33" t="n">
-        <v>-11.41</v>
+        <v>-5.46</v>
       </c>
       <c r="E33" t="n">
-        <v>-5.05</v>
+        <v>-5.53</v>
       </c>
       <c r="F33" t="n">
         <v>-19.78</v>
       </c>
       <c r="G33" t="n">
-        <v>-19.65</v>
+        <v>-17.44</v>
       </c>
       <c r="H33" t="n">
-        <v>-1.34</v>
+        <v>-3.12</v>
       </c>
       <c r="I33" t="n">
-        <v>-22.78</v>
+        <v>-30.5</v>
       </c>
       <c r="J33" s="2" t="n">
-        <v>4.31</v>
+        <v>2.18</v>
       </c>
       <c r="K33" t="n">
-        <v>-3.49</v>
+        <v>-5.05</v>
       </c>
       <c r="L33" t="n">
         <v>-22.85</v>
       </c>
       <c r="M33" s="2" t="n">
-        <v>3.21</v>
+        <v>2.92</v>
       </c>
       <c r="N33" t="n">
         <v>-100</v>
       </c>
       <c r="O33" t="n">
-        <v>-1.57</v>
+        <v>-1.28</v>
       </c>
       <c r="P33" s="2" t="n">
-        <v>5.37</v>
+        <v>3.26</v>
       </c>
       <c r="Q33" t="n">
-        <v>-24.6</v>
+        <v>-25.17</v>
       </c>
       <c r="R33" s="2" t="n">
-        <v>17.76</v>
+        <v>14.4</v>
       </c>
       <c r="S33" t="n">
-        <v>-16.07</v>
+        <v>-16.69</v>
       </c>
       <c r="T33" t="n">
         <v>-56.42</v>
       </c>
       <c r="U33" t="n">
-        <v>-2.32</v>
+        <v>-3.09</v>
       </c>
       <c r="V33" s="2" t="n">
         <v>57</v>
       </c>
       <c r="W33" t="n">
-        <v>-8.880000000000001</v>
+        <v>-7.98</v>
       </c>
       <c r="X33" t="n">
-        <v>-4.93</v>
+        <v>-6.98</v>
       </c>
       <c r="Y33" t="n">
-        <v>-28.94</v>
+        <v>-32.68</v>
       </c>
       <c r="Z33" t="n">
-        <v>-56.17</v>
+        <v>-59.54</v>
       </c>
       <c r="AA33" t="n">
-        <v>-2.1</v>
+        <v>-1.42</v>
       </c>
       <c r="AB33" s="2" t="n">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34">
@@ -3258,41 +3252,41 @@
           <t>Spain2</t>
         </is>
       </c>
-      <c r="B34" t="n">
-        <v>-1.82</v>
+      <c r="B34" s="2" t="n">
+        <v>1.26</v>
       </c>
       <c r="C34" t="n">
         <v>-52.86</v>
       </c>
       <c r="D34" t="n">
-        <v>-2.22</v>
+        <v>-7.73</v>
       </c>
       <c r="E34" t="n">
-        <v>-1</v>
+        <v>-2.42</v>
       </c>
       <c r="F34" t="n">
-        <v>-8.51</v>
+        <v>-8.02</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.87</v>
+        <v>-8.289999999999999</v>
       </c>
       <c r="H34" t="n">
-        <v>-5.05</v>
+        <v>-2.94</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>45.88</v>
+        <v>40.27</v>
       </c>
       <c r="J34" s="2" t="n">
-        <v>17.53</v>
+        <v>17.9</v>
       </c>
       <c r="K34" t="n">
-        <v>-5.29</v>
+        <v>-8.1</v>
       </c>
       <c r="L34" t="n">
         <v>-6.82</v>
       </c>
       <c r="M34" t="n">
-        <v>-7.89</v>
+        <v>-7.4</v>
       </c>
       <c r="N34" s="2" t="n">
         <v>50</v>
@@ -3301,31 +3295,31 @@
         <v>-3.01</v>
       </c>
       <c r="P34" s="2" t="n">
-        <v>1.11</v>
+        <v>2.25</v>
       </c>
       <c r="Q34" t="n">
-        <v>-4.85</v>
+        <v>-7.57</v>
       </c>
       <c r="R34" s="2" t="n">
-        <v>12.78</v>
+        <v>10.94</v>
       </c>
       <c r="S34" t="n">
-        <v>-18.61</v>
+        <v>-19.81</v>
       </c>
       <c r="T34" t="n">
         <v>-52.5</v>
       </c>
       <c r="U34" t="n">
-        <v>-0.87</v>
+        <v>-2.49</v>
       </c>
       <c r="V34" s="2" t="n">
         <v>0.7</v>
       </c>
       <c r="W34" t="n">
-        <v>-21.12</v>
+        <v>-21.5</v>
       </c>
       <c r="X34" t="n">
-        <v>-5.68</v>
+        <v>-6.2</v>
       </c>
       <c r="Y34" t="n">
         <v>-51.38</v>
@@ -3334,10 +3328,10 @@
         <v>26.25</v>
       </c>
       <c r="AA34" t="n">
-        <v>-3.62</v>
+        <v>-2.92</v>
       </c>
       <c r="AB34" s="2" t="n">
-        <v>178</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35">
@@ -3426,82 +3420,82 @@
           <t>Switzerland</t>
         </is>
       </c>
-      <c r="B36" t="n">
-        <v>-8.84</v>
+      <c r="B36" s="2" t="n">
+        <v>2.52</v>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
-        <v>-15.54</v>
+        <v>-43.25</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>4.75</v>
+        <v>0.57</v>
       </c>
       <c r="F36" t="n">
-        <v>-9.949999999999999</v>
+        <v>-8.9</v>
       </c>
       <c r="G36" t="n">
-        <v>-11.62</v>
+        <v>-11.77</v>
       </c>
       <c r="H36" s="2" t="n">
-        <v>4.37</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="I36" t="inlineStr"/>
       <c r="J36" s="2" t="n">
-        <v>7.67</v>
-      </c>
-      <c r="K36" t="n">
-        <v>-0.67</v>
+        <v>5.78</v>
+      </c>
+      <c r="K36" s="2" t="n">
+        <v>10.76</v>
       </c>
       <c r="L36" s="2" t="n">
-        <v>33.11</v>
+        <v>29.78</v>
       </c>
       <c r="M36" t="n">
-        <v>-5.24</v>
-      </c>
-      <c r="N36" t="n">
-        <v>-100</v>
+        <v>-0.97</v>
+      </c>
+      <c r="N36" s="2" t="n">
+        <v>333</v>
       </c>
       <c r="O36" t="n">
-        <v>-5.39</v>
+        <v>-6.88</v>
       </c>
       <c r="P36" s="2" t="n">
-        <v>3.71</v>
+        <v>2.39</v>
       </c>
       <c r="Q36" t="n">
-        <v>-38.25</v>
-      </c>
-      <c r="R36" t="n">
-        <v>-20.9</v>
+        <v>-19.94</v>
+      </c>
+      <c r="R36" s="2" t="n">
+        <v>24</v>
       </c>
       <c r="S36" t="n">
-        <v>-22.89</v>
+        <v>-16.37</v>
       </c>
       <c r="T36" s="2" t="n">
-        <v>27.54</v>
+        <v>49.46</v>
       </c>
       <c r="U36" t="n">
-        <v>-6.04</v>
+        <v>-5.51</v>
       </c>
       <c r="V36" t="n">
         <v>-100</v>
       </c>
       <c r="W36" t="n">
-        <v>-14.6</v>
+        <v>-13.87</v>
       </c>
       <c r="X36" s="2" t="n">
-        <v>5.97</v>
+        <v>3.19</v>
       </c>
       <c r="Y36" t="n">
         <v>-100</v>
       </c>
       <c r="Z36" t="n">
-        <v>-49.11</v>
+        <v>-19.89</v>
       </c>
       <c r="AA36" t="n">
-        <v>-18.04</v>
+        <v>-15.27</v>
       </c>
       <c r="AB36" s="2" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37">
@@ -3511,71 +3505,71 @@
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>9.27</v>
+        <v>11.37</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>33.89</v>
       </c>
       <c r="D37" t="n">
-        <v>-33.13</v>
+        <v>-31.88</v>
       </c>
       <c r="E37" t="n">
-        <v>-4.55</v>
+        <v>-4.06</v>
       </c>
       <c r="F37" t="n">
-        <v>-10.5</v>
+        <v>-8.6</v>
       </c>
       <c r="G37" t="n">
-        <v>-24.63</v>
+        <v>-24.05</v>
       </c>
       <c r="H37" t="n">
-        <v>-5.48</v>
+        <v>-5.64</v>
       </c>
       <c r="I37" s="2" t="n">
         <v>28.25</v>
       </c>
       <c r="J37" t="n">
-        <v>-6.31</v>
+        <v>-7.56</v>
       </c>
       <c r="K37" t="n">
-        <v>-24.66</v>
+        <v>-26.23</v>
       </c>
       <c r="L37" t="n">
         <v>-3.12</v>
       </c>
       <c r="M37" t="n">
-        <v>-7.48</v>
+        <v>-8.23</v>
       </c>
       <c r="N37" t="n">
         <v>-100</v>
       </c>
       <c r="O37" t="n">
-        <v>-7.66</v>
+        <v>-8.9</v>
       </c>
       <c r="P37" t="n">
-        <v>-12.74</v>
+        <v>-12.64</v>
       </c>
       <c r="Q37" t="n">
-        <v>-24.13</v>
-      </c>
-      <c r="R37" s="2" t="n">
-        <v>1.31</v>
+        <v>-25.2</v>
+      </c>
+      <c r="R37" t="n">
+        <v>-6.68</v>
       </c>
       <c r="S37" t="n">
-        <v>-15.78</v>
+        <v>-14.79</v>
       </c>
       <c r="T37" t="n">
         <v>-4.44</v>
       </c>
-      <c r="U37" t="n">
-        <v>-0.38</v>
+      <c r="U37" s="2" t="n">
+        <v>0.33</v>
       </c>
       <c r="V37" t="inlineStr"/>
       <c r="W37" t="n">
-        <v>-11.97</v>
+        <v>-11.32</v>
       </c>
       <c r="X37" t="n">
-        <v>-0.89</v>
+        <v>-1.84</v>
       </c>
       <c r="Y37" t="n">
         <v>-28.57</v>
@@ -3584,10 +3578,10 @@
         <v>-26.65</v>
       </c>
       <c r="AA37" t="n">
-        <v>-4.98</v>
+        <v>-6.73</v>
       </c>
       <c r="AB37" s="2" t="n">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38">
@@ -4021,734 +4015,660 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>brazil</t>
+          <t>england2</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" s="2" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="E43" t="n">
-        <v>-15.67</v>
-      </c>
-      <c r="F43" t="n">
-        <v>-2</v>
+        <v>43.8</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-100</v>
+      </c>
+      <c r="D43" t="n">
+        <v>-59.5</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>29</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>30.67</v>
+        <v>12</v>
       </c>
       <c r="H43" t="n">
-        <v>-30.1</v>
-      </c>
-      <c r="I43" t="inlineStr"/>
+        <v>-37.25</v>
+      </c>
+      <c r="I43" t="n">
+        <v>-100</v>
+      </c>
       <c r="J43" t="n">
-        <v>-25</v>
+        <v>-10.5</v>
       </c>
       <c r="K43" t="n">
-        <v>-29</v>
-      </c>
-      <c r="L43" t="inlineStr"/>
+        <v>-18.43</v>
+      </c>
+      <c r="L43" t="n">
+        <v>-100</v>
+      </c>
       <c r="M43" t="n">
-        <v>-13.3</v>
-      </c>
-      <c r="N43" t="inlineStr"/>
-      <c r="O43" t="n">
-        <v>-14.2</v>
+        <v>-1.71</v>
+      </c>
+      <c r="N43" t="n">
+        <v>-100</v>
+      </c>
+      <c r="O43" s="2" t="n">
+        <v>3.2</v>
       </c>
       <c r="P43" t="n">
-        <v>-50</v>
-      </c>
-      <c r="Q43" s="2" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="R43" t="inlineStr"/>
+        <v>-13.5</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>-14</v>
+      </c>
+      <c r="R43" s="2" t="n">
+        <v>8.33</v>
+      </c>
       <c r="S43" t="n">
-        <v>-1.9</v>
-      </c>
-      <c r="T43" t="inlineStr"/>
-      <c r="U43" s="2" t="n">
-        <v>24.14</v>
+        <v>-36.43</v>
+      </c>
+      <c r="T43" t="n">
+        <v>-100</v>
+      </c>
+      <c r="U43" t="n">
+        <v>-18.56</v>
       </c>
       <c r="V43" t="inlineStr"/>
       <c r="W43" s="2" t="n">
-        <v>30.67</v>
+        <v>21</v>
       </c>
       <c r="X43" t="n">
-        <v>-0.67</v>
+        <v>-23.14</v>
       </c>
       <c r="Y43" t="n">
-        <v>-100</v>
+        <v>-31.25</v>
       </c>
       <c r="Z43" t="n">
         <v>-100</v>
       </c>
-      <c r="AA43" t="n">
-        <v>-12.11</v>
+      <c r="AA43" s="2" t="n">
+        <v>4.5</v>
       </c>
       <c r="AB43" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>england2</t>
-        </is>
-      </c>
-      <c r="B44" s="2" t="n">
-        <v>43.8</v>
-      </c>
-      <c r="C44" t="n">
-        <v>-100</v>
-      </c>
+          <t>england3</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>-29.78</v>
+      </c>
+      <c r="C44" t="inlineStr"/>
       <c r="D44" t="n">
-        <v>-59.5</v>
-      </c>
-      <c r="E44" s="2" t="n">
-        <v>2</v>
+        <v>-30</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-26.75</v>
       </c>
       <c r="F44" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="G44" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="H44" t="n">
-        <v>-37.25</v>
+      <c r="G44" t="n">
+        <v>-54.67</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>10.45</v>
       </c>
       <c r="I44" t="n">
         <v>-100</v>
       </c>
-      <c r="J44" t="n">
-        <v>-10.5</v>
+      <c r="J44" s="2" t="n">
+        <v>40.6</v>
       </c>
       <c r="K44" t="n">
-        <v>-18.43</v>
+        <v>-44.57</v>
       </c>
       <c r="L44" t="n">
         <v>-100</v>
       </c>
       <c r="M44" t="n">
-        <v>-1.71</v>
+        <v>-18.3</v>
       </c>
       <c r="N44" t="n">
         <v>-100</v>
       </c>
-      <c r="O44" s="2" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="P44" t="n">
-        <v>-13.5</v>
+      <c r="O44" t="n">
+        <v>-20.4</v>
+      </c>
+      <c r="P44" s="2" t="n">
+        <v>26</v>
       </c>
       <c r="Q44" t="n">
-        <v>-14</v>
-      </c>
-      <c r="R44" s="2" t="n">
-        <v>8.33</v>
+        <v>-48.12</v>
+      </c>
+      <c r="R44" t="n">
+        <v>0</v>
       </c>
       <c r="S44" t="n">
-        <v>-36.43</v>
-      </c>
-      <c r="T44" t="n">
-        <v>-100</v>
+        <v>-70</v>
+      </c>
+      <c r="T44" s="2" t="n">
+        <v>138</v>
       </c>
       <c r="U44" t="n">
-        <v>-18.56</v>
+        <v>-26.5</v>
       </c>
       <c r="V44" t="inlineStr"/>
       <c r="W44" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="X44" t="n">
-        <v>-23.14</v>
+        <v>1.5</v>
+      </c>
+      <c r="X44" s="2" t="n">
+        <v>16</v>
       </c>
       <c r="Y44" t="n">
-        <v>-31.25</v>
-      </c>
-      <c r="Z44" t="n">
-        <v>-100</v>
-      </c>
-      <c r="AA44" s="2" t="n">
-        <v>4.5</v>
+        <v>-100</v>
+      </c>
+      <c r="Z44" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA44" t="n">
+        <v>-48</v>
       </c>
       <c r="AB44" s="2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>england3</t>
+          <t>england4</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-29.78</v>
+        <v>-29.6</v>
       </c>
       <c r="C45" t="inlineStr"/>
-      <c r="D45" t="n">
-        <v>-30</v>
-      </c>
-      <c r="E45" t="n">
-        <v>-26.75</v>
-      </c>
-      <c r="F45" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="G45" t="n">
-        <v>-54.67</v>
-      </c>
-      <c r="H45" s="2" t="n">
-        <v>10.45</v>
-      </c>
-      <c r="I45" t="n">
-        <v>-100</v>
-      </c>
-      <c r="J45" s="2" t="n">
-        <v>40.6</v>
-      </c>
-      <c r="K45" t="n">
-        <v>-44.57</v>
+      <c r="D45" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="n">
+        <v>-9.4</v>
+      </c>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="n">
+        <v>-18</v>
+      </c>
+      <c r="I45" s="2" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="J45" t="n">
+        <v>-63</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <v>14</v>
       </c>
       <c r="L45" t="n">
         <v>-100</v>
       </c>
-      <c r="M45" t="n">
-        <v>-18.3</v>
-      </c>
-      <c r="N45" t="n">
-        <v>-100</v>
-      </c>
-      <c r="O45" t="n">
-        <v>-20.4</v>
-      </c>
-      <c r="P45" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="Q45" t="n">
-        <v>-48.12</v>
+      <c r="M45" s="2" t="n">
+        <v>18.12</v>
+      </c>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" s="2" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="P45" t="n">
+        <v>-42.33</v>
+      </c>
+      <c r="Q45" s="2" t="n">
+        <v>68</v>
       </c>
       <c r="R45" t="n">
-        <v>0</v>
-      </c>
-      <c r="S45" t="n">
-        <v>-70</v>
-      </c>
-      <c r="T45" s="2" t="n">
-        <v>138</v>
+        <v>-20.8</v>
+      </c>
+      <c r="S45" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="T45" t="n">
+        <v>-100</v>
       </c>
       <c r="U45" t="n">
-        <v>-26.5</v>
-      </c>
-      <c r="V45" t="inlineStr"/>
-      <c r="W45" s="2" t="n">
-        <v>1.5</v>
+        <v>-2.4</v>
+      </c>
+      <c r="V45" t="n">
+        <v>-21.5</v>
+      </c>
+      <c r="W45" t="n">
+        <v>-100</v>
       </c>
       <c r="X45" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="Y45" t="n">
-        <v>-100</v>
-      </c>
-      <c r="Z45" s="2" t="n">
-        <v>22</v>
+        <v>5.33</v>
+      </c>
+      <c r="Y45" s="2" t="n">
+        <v>175</v>
+      </c>
+      <c r="Z45" t="n">
+        <v>-100</v>
       </c>
       <c r="AA45" t="n">
-        <v>-48</v>
+        <v>-17.14</v>
       </c>
       <c r="AB45" s="2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>england4</t>
+          <t>england5</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>-29.6</v>
-      </c>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="E46" t="inlineStr"/>
+        <v>-30.4</v>
+      </c>
+      <c r="C46" t="n">
+        <v>-100</v>
+      </c>
+      <c r="D46" t="n">
+        <v>-11.6</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-25.2</v>
+      </c>
       <c r="F46" t="n">
-        <v>-9.4</v>
-      </c>
-      <c r="G46" t="inlineStr"/>
+        <v>-35.5</v>
+      </c>
+      <c r="G46" t="n">
+        <v>-38.25</v>
+      </c>
       <c r="H46" t="n">
-        <v>-18</v>
+        <v>-1.7</v>
       </c>
       <c r="I46" s="2" t="n">
-        <v>8.25</v>
+        <v>225</v>
       </c>
       <c r="J46" t="n">
-        <v>-63</v>
-      </c>
-      <c r="K46" s="2" t="n">
-        <v>14</v>
-      </c>
-      <c r="L46" t="n">
-        <v>-100</v>
-      </c>
-      <c r="M46" s="2" t="n">
-        <v>18.12</v>
+        <v>-40.83</v>
+      </c>
+      <c r="K46" t="n">
+        <v>-65.40000000000001</v>
+      </c>
+      <c r="L46" s="2" t="n">
+        <v>175</v>
+      </c>
+      <c r="M46" t="n">
+        <v>-3.6</v>
       </c>
       <c r="N46" t="inlineStr"/>
-      <c r="O46" s="2" t="n">
-        <v>13.2</v>
+      <c r="O46" t="n">
+        <v>-17</v>
       </c>
       <c r="P46" t="n">
-        <v>-42.33</v>
-      </c>
-      <c r="Q46" s="2" t="n">
-        <v>68</v>
-      </c>
-      <c r="R46" t="n">
-        <v>-20.8</v>
+        <v>-32.6</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>-31.5</v>
+      </c>
+      <c r="R46" s="2" t="n">
+        <v>25</v>
       </c>
       <c r="S46" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="T46" t="n">
-        <v>-100</v>
-      </c>
-      <c r="U46" t="n">
-        <v>-2.4</v>
+        <v>116.67</v>
+      </c>
+      <c r="T46" s="2" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="U46" s="2" t="n">
+        <v>1.5</v>
       </c>
       <c r="V46" t="n">
-        <v>-21.5</v>
+        <v>-19</v>
       </c>
       <c r="W46" t="n">
-        <v>-100</v>
-      </c>
-      <c r="X46" s="2" t="n">
-        <v>5.33</v>
-      </c>
-      <c r="Y46" s="2" t="n">
-        <v>175</v>
-      </c>
+        <v>-12.67</v>
+      </c>
+      <c r="X46" t="n">
+        <v>-38.36</v>
+      </c>
+      <c r="Y46" t="inlineStr"/>
       <c r="Z46" t="n">
         <v>-100</v>
       </c>
-      <c r="AA46" t="n">
-        <v>-17.14</v>
+      <c r="AA46" s="2" t="n">
+        <v>14.8</v>
       </c>
       <c r="AB46" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>england5</t>
+          <t>italy2</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>-30.4</v>
+        <v>-24.4</v>
       </c>
       <c r="C47" t="n">
         <v>-100</v>
       </c>
-      <c r="D47" t="n">
-        <v>-11.6</v>
-      </c>
-      <c r="E47" t="n">
-        <v>-25.2</v>
-      </c>
-      <c r="F47" t="n">
-        <v>-35.5</v>
-      </c>
+      <c r="D47" s="2" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="F47" t="inlineStr"/>
       <c r="G47" t="n">
-        <v>-38.25</v>
+        <v>-41.2</v>
       </c>
       <c r="H47" t="n">
-        <v>-1.7</v>
+        <v>-31.37</v>
       </c>
       <c r="I47" s="2" t="n">
-        <v>225</v>
+        <v>50</v>
       </c>
       <c r="J47" t="n">
-        <v>-40.83</v>
+        <v>-57</v>
       </c>
       <c r="K47" t="n">
-        <v>-65.40000000000001</v>
-      </c>
-      <c r="L47" s="2" t="n">
-        <v>175</v>
-      </c>
-      <c r="M47" t="n">
-        <v>-3.6</v>
+        <v>-66.59999999999999</v>
+      </c>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" s="2" t="n">
+        <v>12.9</v>
       </c>
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="n">
-        <v>-17</v>
+        <v>-2.5</v>
       </c>
       <c r="P47" t="n">
-        <v>-32.6</v>
-      </c>
-      <c r="Q47" t="n">
-        <v>-31.5</v>
-      </c>
-      <c r="R47" s="2" t="n">
-        <v>25</v>
+        <v>-61</v>
+      </c>
+      <c r="Q47" s="2" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="R47" t="n">
+        <v>-100</v>
       </c>
       <c r="S47" s="2" t="n">
-        <v>116.67</v>
-      </c>
-      <c r="T47" s="2" t="n">
-        <v>13.33</v>
-      </c>
-      <c r="U47" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="V47" t="n">
-        <v>-19</v>
+        <v>56.25</v>
+      </c>
+      <c r="T47" t="n">
+        <v>-100</v>
+      </c>
+      <c r="U47" t="n">
+        <v>-7.75</v>
+      </c>
+      <c r="V47" s="2" t="n">
+        <v>15.33</v>
       </c>
       <c r="W47" t="n">
-        <v>-12.67</v>
+        <v>-10.33</v>
       </c>
       <c r="X47" t="n">
-        <v>-38.36</v>
-      </c>
-      <c r="Y47" t="inlineStr"/>
+        <v>-8.630000000000001</v>
+      </c>
+      <c r="Y47" s="2" t="n">
+        <v>31.5</v>
+      </c>
       <c r="Z47" t="n">
         <v>-100</v>
       </c>
-      <c r="AA47" s="2" t="n">
-        <v>14.8</v>
+      <c r="AA47" t="n">
+        <v>-10.67</v>
       </c>
       <c r="AB47" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>italy2</t>
+          <t>mexico</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>-24.4</v>
-      </c>
-      <c r="C48" t="n">
-        <v>-100</v>
-      </c>
-      <c r="D48" s="2" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="E48" s="2" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="F48" t="inlineStr"/>
+        <v>-13.11</v>
+      </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="n">
+        <v>-100</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-18.71</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-17.67</v>
+      </c>
       <c r="G48" t="n">
-        <v>-41.2</v>
+        <v>-100</v>
       </c>
       <c r="H48" t="n">
-        <v>-31.37</v>
-      </c>
-      <c r="I48" s="2" t="n">
-        <v>50</v>
-      </c>
+        <v>-59.92</v>
+      </c>
+      <c r="I48" t="inlineStr"/>
       <c r="J48" t="n">
-        <v>-57</v>
-      </c>
-      <c r="K48" t="n">
-        <v>-66.59999999999999</v>
-      </c>
-      <c r="L48" t="inlineStr"/>
+        <v>-53.86</v>
+      </c>
+      <c r="K48" s="2" t="n">
+        <v>61.2</v>
+      </c>
+      <c r="L48" s="2" t="n">
+        <v>125</v>
+      </c>
       <c r="M48" s="2" t="n">
-        <v>12.9</v>
+        <v>14.64</v>
       </c>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="n">
-        <v>-2.5</v>
+        <v>-4.33</v>
       </c>
       <c r="P48" t="n">
-        <v>-61</v>
+        <v>-44.33</v>
       </c>
       <c r="Q48" s="2" t="n">
-        <v>11.6</v>
-      </c>
-      <c r="R48" t="n">
-        <v>-100</v>
+        <v>50.11</v>
+      </c>
+      <c r="R48" s="2" t="n">
+        <v>37</v>
       </c>
       <c r="S48" s="2" t="n">
-        <v>56.25</v>
+        <v>31.14</v>
       </c>
       <c r="T48" t="n">
         <v>-100</v>
       </c>
       <c r="U48" t="n">
-        <v>-7.75</v>
-      </c>
-      <c r="V48" s="2" t="n">
-        <v>15.33</v>
-      </c>
-      <c r="W48" t="n">
-        <v>-10.33</v>
+        <v>-9.5</v>
+      </c>
+      <c r="V48" t="inlineStr"/>
+      <c r="W48" s="2" t="n">
+        <v>15.75</v>
       </c>
       <c r="X48" t="n">
-        <v>-8.630000000000001</v>
+        <v>-33.2</v>
       </c>
       <c r="Y48" s="2" t="n">
-        <v>31.5</v>
+        <v>50</v>
       </c>
       <c r="Z48" t="n">
-        <v>-100</v>
-      </c>
-      <c r="AA48" t="n">
-        <v>-10.67</v>
+        <v>-50</v>
+      </c>
+      <c r="AA48" s="2" t="n">
+        <v>21.29</v>
       </c>
       <c r="AB48" s="2" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>mexico</t>
+          <t>turkey</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>-13.11</v>
-      </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="n">
-        <v>-100</v>
+        <v>-12.67</v>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>61</v>
       </c>
       <c r="E49" t="n">
-        <v>-18.71</v>
+        <v>-23.5</v>
       </c>
       <c r="F49" t="n">
-        <v>-17.67</v>
-      </c>
-      <c r="G49" t="n">
-        <v>-100</v>
+        <v>-100</v>
+      </c>
+      <c r="G49" s="2" t="n">
+        <v>57</v>
       </c>
       <c r="H49" t="n">
-        <v>-59.92</v>
-      </c>
-      <c r="I49" t="inlineStr"/>
-      <c r="J49" t="n">
-        <v>-53.86</v>
+        <v>-32.33</v>
+      </c>
+      <c r="I49" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <v>15.25</v>
       </c>
       <c r="K49" s="2" t="n">
-        <v>61.2</v>
-      </c>
-      <c r="L49" s="2" t="n">
-        <v>125</v>
-      </c>
-      <c r="M49" s="2" t="n">
-        <v>14.64</v>
-      </c>
-      <c r="N49" t="inlineStr"/>
-      <c r="O49" t="n">
-        <v>-4.33</v>
-      </c>
-      <c r="P49" t="n">
-        <v>-44.33</v>
+        <v>43.83</v>
+      </c>
+      <c r="L49" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="M49" t="n">
+        <v>-0.63</v>
+      </c>
+      <c r="N49" t="n">
+        <v>-100</v>
+      </c>
+      <c r="O49" s="2" t="n">
+        <v>13.67</v>
+      </c>
+      <c r="P49" s="2" t="n">
+        <v>1.4</v>
       </c>
       <c r="Q49" s="2" t="n">
-        <v>50.11</v>
-      </c>
-      <c r="R49" s="2" t="n">
-        <v>37</v>
+        <v>41.2</v>
+      </c>
+      <c r="R49" t="n">
+        <v>-100</v>
       </c>
       <c r="S49" s="2" t="n">
-        <v>31.14</v>
-      </c>
-      <c r="T49" t="n">
-        <v>-100</v>
+        <v>7.5</v>
+      </c>
+      <c r="T49" s="2" t="n">
+        <v>175</v>
       </c>
       <c r="U49" t="n">
-        <v>-9.5</v>
+        <v>-24.5</v>
       </c>
       <c r="V49" t="inlineStr"/>
       <c r="W49" s="2" t="n">
-        <v>15.75</v>
-      </c>
-      <c r="X49" t="n">
-        <v>-33.2</v>
+        <v>37</v>
+      </c>
+      <c r="X49" s="2" t="n">
+        <v>33</v>
       </c>
       <c r="Y49" s="2" t="n">
-        <v>50</v>
+        <v>40.75</v>
       </c>
       <c r="Z49" t="n">
-        <v>-50</v>
-      </c>
-      <c r="AA49" s="2" t="n">
-        <v>21.29</v>
+        <v>-48.75</v>
+      </c>
+      <c r="AA49" t="n">
+        <v>-2.67</v>
       </c>
       <c r="AB49" s="2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>turkey</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>-12.67</v>
-      </c>
-      <c r="C50" s="2" t="n">
-        <v>80</v>
-      </c>
-      <c r="D50" s="2" t="n">
-        <v>61</v>
-      </c>
-      <c r="E50" t="n">
-        <v>-23.5</v>
+          <t>usa</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="n">
+        <v>-20</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>19.2</v>
       </c>
       <c r="F50" t="n">
-        <v>-100</v>
+        <v>-25.3</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>57</v>
-      </c>
-      <c r="H50" t="n">
-        <v>-32.33</v>
-      </c>
-      <c r="I50" t="n">
-        <v>-100</v>
-      </c>
+        <v>37.33</v>
+      </c>
+      <c r="H50" s="2" t="n">
+        <v>5.61</v>
+      </c>
+      <c r="I50" t="inlineStr"/>
       <c r="J50" s="2" t="n">
-        <v>15.25</v>
+        <v>1.44</v>
       </c>
       <c r="K50" s="2" t="n">
-        <v>43.83</v>
-      </c>
-      <c r="L50" t="n">
-        <v>-4.5</v>
+        <v>20</v>
+      </c>
+      <c r="L50" s="2" t="n">
+        <v>45.75</v>
       </c>
       <c r="M50" t="n">
-        <v>-0.63</v>
-      </c>
-      <c r="N50" t="n">
-        <v>-100</v>
-      </c>
-      <c r="O50" s="2" t="n">
-        <v>13.67</v>
+        <v>-29.74</v>
+      </c>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="n">
+        <v>-11.04</v>
       </c>
       <c r="P50" s="2" t="n">
-        <v>1.4</v>
+        <v>10.75</v>
       </c>
       <c r="Q50" s="2" t="n">
-        <v>41.2</v>
-      </c>
-      <c r="R50" t="n">
-        <v>-100</v>
+        <v>22.14</v>
+      </c>
+      <c r="R50" s="2" t="n">
+        <v>47.15</v>
       </c>
       <c r="S50" s="2" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="T50" s="2" t="n">
-        <v>175</v>
-      </c>
-      <c r="U50" t="n">
-        <v>-24.5</v>
+        <v>3.89</v>
+      </c>
+      <c r="T50" t="n">
+        <v>-100</v>
+      </c>
+      <c r="U50" s="2" t="n">
+        <v>3.47</v>
       </c>
       <c r="V50" t="inlineStr"/>
       <c r="W50" s="2" t="n">
-        <v>37</v>
-      </c>
-      <c r="X50" s="2" t="n">
-        <v>33</v>
-      </c>
-      <c r="Y50" s="2" t="n">
-        <v>40.75</v>
-      </c>
-      <c r="Z50" t="n">
-        <v>-48.75</v>
-      </c>
-      <c r="AA50" t="n">
-        <v>-2.67</v>
+        <v>4</v>
+      </c>
+      <c r="X50" t="n">
+        <v>-0.35</v>
+      </c>
+      <c r="Y50" t="inlineStr"/>
+      <c r="Z50" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="AA50" s="2" t="n">
+        <v>12.78</v>
       </c>
       <c r="AB50" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="inlineStr">
-        <is>
-          <t>usa</t>
-        </is>
-      </c>
-      <c r="B51" s="2" t="n">
-        <v>4.88</v>
-      </c>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="n">
-        <v>-20</v>
-      </c>
-      <c r="E51" s="2" t="n">
-        <v>19.2</v>
-      </c>
-      <c r="F51" t="n">
-        <v>-25.3</v>
-      </c>
-      <c r="G51" s="2" t="n">
-        <v>37.33</v>
-      </c>
-      <c r="H51" s="2" t="n">
-        <v>5.61</v>
-      </c>
-      <c r="I51" t="inlineStr"/>
-      <c r="J51" s="2" t="n">
-        <v>1.44</v>
-      </c>
-      <c r="K51" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="L51" s="2" t="n">
-        <v>45.75</v>
-      </c>
-      <c r="M51" t="n">
-        <v>-29.74</v>
-      </c>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="n">
-        <v>-11.04</v>
-      </c>
-      <c r="P51" s="2" t="n">
-        <v>10.75</v>
-      </c>
-      <c r="Q51" s="2" t="n">
-        <v>22.14</v>
-      </c>
-      <c r="R51" s="2" t="n">
-        <v>47.15</v>
-      </c>
-      <c r="S51" s="2" t="n">
-        <v>3.89</v>
-      </c>
-      <c r="T51" t="n">
-        <v>-100</v>
-      </c>
-      <c r="U51" s="2" t="n">
-        <v>3.47</v>
-      </c>
-      <c r="V51" t="inlineStr"/>
-      <c r="W51" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="X51" t="n">
-        <v>-0.35</v>
-      </c>
-      <c r="Y51" t="inlineStr"/>
-      <c r="Z51" s="2" t="n">
-        <v>67</v>
-      </c>
-      <c r="AA51" s="2" t="n">
-        <v>12.78</v>
-      </c>
-      <c r="AB51" s="2" t="n">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
model updated for 2026
</commit_message>
<xml_diff>
--- a/ROI_leagues.xlsx
+++ b/ROI_leagues.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB48"/>
+  <dimension ref="A1:AB50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2221,2222 +2221,2222 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Mexico2</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>15.5</v>
-      </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="n">
-        <v>-33.73</v>
+          <t>Mexico</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-17.28</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>10.81</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>11.67</v>
-      </c>
-      <c r="F21" s="2" t="n">
-        <v>6.17</v>
+        <v>9.08</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-12.95</v>
       </c>
       <c r="G21" t="n">
-        <v>-48.36</v>
-      </c>
-      <c r="H21" s="2" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="I21" t="n">
-        <v>-100</v>
-      </c>
-      <c r="J21" s="2" t="n">
-        <v>30.34</v>
+        <v>-14.83</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-12.58</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>28.83</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-16.46</v>
       </c>
       <c r="K21" t="n">
-        <v>-20.93</v>
+        <v>-2.61</v>
       </c>
       <c r="L21" t="n">
-        <v>-6.7</v>
+        <v>-4.2</v>
       </c>
       <c r="M21" t="n">
-        <v>-7.7</v>
-      </c>
-      <c r="N21" s="2" t="n">
-        <v>87.5</v>
+        <v>-6.53</v>
+      </c>
+      <c r="N21" t="n">
+        <v>-100</v>
       </c>
       <c r="O21" t="n">
-        <v>-5.44</v>
-      </c>
-      <c r="P21" s="2" t="n">
-        <v>13.15</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>-34.34</v>
+        <v>-6.36</v>
+      </c>
+      <c r="P21" t="n">
+        <v>-13.76</v>
+      </c>
+      <c r="Q21" s="2" t="n">
+        <v>10</v>
       </c>
       <c r="R21" t="n">
-        <v>-33.25</v>
+        <v>-29.63</v>
       </c>
       <c r="S21" t="n">
-        <v>-20.67</v>
+        <v>-14.68</v>
       </c>
       <c r="T21" t="n">
-        <v>-100</v>
+        <v>-46.11</v>
       </c>
       <c r="U21" t="n">
-        <v>-0.97</v>
+        <v>-7.58</v>
       </c>
       <c r="V21" t="inlineStr"/>
       <c r="W21" t="n">
-        <v>-33</v>
-      </c>
-      <c r="X21" s="2" t="n">
-        <v>4.51</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>-100</v>
+        <v>-1.05</v>
+      </c>
+      <c r="X21" t="n">
+        <v>-7.16</v>
+      </c>
+      <c r="Y21" s="2" t="n">
+        <v>108.33</v>
       </c>
       <c r="Z21" s="2" t="n">
-        <v>14.83</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="AA21" t="n">
-        <v>-23.61</v>
+        <v>-2.87</v>
       </c>
       <c r="AB21" s="2" t="n">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>-15.63</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>14.23</v>
-      </c>
-      <c r="E22" t="n">
-        <v>-0.35</v>
-      </c>
-      <c r="F22" t="n">
-        <v>-6.5</v>
+          <t>Mexico2</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="n">
+        <v>-33.73</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>6.17</v>
       </c>
       <c r="G22" t="n">
-        <v>-19.48</v>
-      </c>
-      <c r="H22" t="n">
-        <v>-12.02</v>
-      </c>
-      <c r="I22" s="2" t="n">
-        <v>75</v>
-      </c>
-      <c r="J22" t="n">
-        <v>-21.3</v>
+        <v>-48.36</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>30.34</v>
       </c>
       <c r="K22" t="n">
-        <v>-3.69</v>
+        <v>-20.93</v>
       </c>
       <c r="L22" t="n">
-        <v>-22.73</v>
+        <v>-6.7</v>
       </c>
       <c r="M22" t="n">
-        <v>-1.92</v>
-      </c>
-      <c r="N22" t="n">
-        <v>-100</v>
+        <v>-7.7</v>
+      </c>
+      <c r="N22" s="2" t="n">
+        <v>87.5</v>
       </c>
       <c r="O22" t="n">
-        <v>-5.85</v>
-      </c>
-      <c r="P22" t="n">
-        <v>-4.67</v>
+        <v>-5.44</v>
+      </c>
+      <c r="P22" s="2" t="n">
+        <v>13.15</v>
       </c>
       <c r="Q22" t="n">
-        <v>-4.98</v>
+        <v>-34.34</v>
       </c>
       <c r="R22" t="n">
-        <v>-29</v>
+        <v>-33.25</v>
       </c>
       <c r="S22" t="n">
-        <v>-25.11</v>
+        <v>-20.67</v>
       </c>
       <c r="T22" t="n">
-        <v>-15.58</v>
+        <v>-100</v>
       </c>
       <c r="U22" t="n">
-        <v>-12.1</v>
-      </c>
-      <c r="V22" t="n">
-        <v>-100</v>
-      </c>
+        <v>-0.97</v>
+      </c>
+      <c r="V22" t="inlineStr"/>
       <c r="W22" t="n">
-        <v>-23.37</v>
-      </c>
-      <c r="X22" t="n">
-        <v>-5.65</v>
+        <v>-33</v>
+      </c>
+      <c r="X22" s="2" t="n">
+        <v>4.51</v>
       </c>
       <c r="Y22" t="n">
-        <v>-8.33</v>
-      </c>
-      <c r="Z22" t="n">
-        <v>-35.71</v>
+        <v>-100</v>
+      </c>
+      <c r="Z22" s="2" t="n">
+        <v>14.83</v>
       </c>
       <c r="AA22" t="n">
-        <v>-2.01</v>
+        <v>-23.61</v>
       </c>
       <c r="AB22" s="2" t="n">
-        <v>89</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-4.66</v>
+        <v>-15.63</v>
       </c>
       <c r="C23" t="n">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>15.33</v>
+        <v>14.23</v>
       </c>
       <c r="E23" t="n">
-        <v>-17.33</v>
+        <v>-0.35</v>
       </c>
       <c r="F23" t="n">
-        <v>-4.55</v>
-      </c>
-      <c r="G23" s="2" t="n">
-        <v>17.29</v>
+        <v>-6.5</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-19.48</v>
       </c>
       <c r="H23" t="n">
-        <v>-14.48</v>
-      </c>
-      <c r="I23" t="n">
-        <v>-100</v>
+        <v>-12.02</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>75</v>
       </c>
       <c r="J23" t="n">
-        <v>-2.37</v>
-      </c>
-      <c r="K23" s="2" t="n">
-        <v>22.38</v>
-      </c>
-      <c r="L23" s="2" t="n">
-        <v>18.11</v>
-      </c>
-      <c r="M23" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" s="2" t="n">
-        <v>1.56</v>
+        <v>-21.3</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-3.69</v>
+      </c>
+      <c r="L23" t="n">
+        <v>-22.73</v>
+      </c>
+      <c r="M23" t="n">
+        <v>-1.92</v>
+      </c>
+      <c r="N23" t="n">
+        <v>-100</v>
+      </c>
+      <c r="O23" t="n">
+        <v>-5.85</v>
       </c>
       <c r="P23" t="n">
-        <v>-16.76</v>
-      </c>
-      <c r="Q23" s="2" t="n">
-        <v>11.36</v>
+        <v>-4.67</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>-4.98</v>
       </c>
       <c r="R23" t="n">
-        <v>-8.56</v>
+        <v>-29</v>
       </c>
       <c r="S23" t="n">
-        <v>-19.02</v>
+        <v>-25.11</v>
       </c>
       <c r="T23" t="n">
-        <v>-67.14</v>
+        <v>-15.58</v>
       </c>
       <c r="U23" t="n">
-        <v>-12.71</v>
-      </c>
-      <c r="V23" t="inlineStr"/>
+        <v>-12.1</v>
+      </c>
+      <c r="V23" t="n">
+        <v>-100</v>
+      </c>
       <c r="W23" t="n">
-        <v>-2.21</v>
+        <v>-23.37</v>
       </c>
       <c r="X23" t="n">
-        <v>-10.59</v>
+        <v>-5.65</v>
       </c>
       <c r="Y23" t="n">
-        <v>-100</v>
-      </c>
-      <c r="Z23" s="2" t="n">
-        <v>17.17</v>
-      </c>
-      <c r="AA23" s="2" t="n">
-        <v>5.18</v>
+        <v>-8.33</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>-35.71</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>-2.01</v>
       </c>
       <c r="AB23" s="2" t="n">
-        <v>66</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-13.97</v>
-      </c>
-      <c r="C24" t="inlineStr"/>
+        <v>-4.66</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-100</v>
+      </c>
       <c r="D24" s="2" t="n">
-        <v>17.11</v>
+        <v>15.33</v>
       </c>
       <c r="E24" t="n">
-        <v>-8.710000000000001</v>
-      </c>
-      <c r="F24" s="2" t="n">
-        <v>3.56</v>
+        <v>-17.33</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-4.55</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>6.1</v>
+        <v>17.29</v>
       </c>
       <c r="H24" t="n">
-        <v>-8.51</v>
+        <v>-14.48</v>
       </c>
       <c r="I24" t="n">
-        <v>-34.79</v>
+        <v>-100</v>
       </c>
       <c r="J24" t="n">
-        <v>-8.869999999999999</v>
-      </c>
-      <c r="K24" t="n">
-        <v>-1.61</v>
-      </c>
-      <c r="L24" t="n">
-        <v>-17.86</v>
-      </c>
-      <c r="M24" t="n">
-        <v>-0.85</v>
-      </c>
-      <c r="N24" t="n">
-        <v>-100</v>
-      </c>
-      <c r="O24" t="n">
-        <v>-2.47</v>
+        <v>-2.37</v>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>22.38</v>
+      </c>
+      <c r="L24" s="2" t="n">
+        <v>18.11</v>
+      </c>
+      <c r="M24" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" s="2" t="n">
+        <v>1.56</v>
       </c>
       <c r="P24" t="n">
-        <v>-18.43</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>-11.74</v>
+        <v>-16.76</v>
+      </c>
+      <c r="Q24" s="2" t="n">
+        <v>11.36</v>
       </c>
       <c r="R24" t="n">
-        <v>-10.25</v>
+        <v>-8.56</v>
       </c>
       <c r="S24" t="n">
-        <v>-34.18</v>
+        <v>-19.02</v>
       </c>
       <c r="T24" t="n">
-        <v>-2.67</v>
+        <v>-67.14</v>
       </c>
       <c r="U24" t="n">
-        <v>-10.56</v>
+        <v>-12.71</v>
       </c>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="n">
-        <v>-10.95</v>
-      </c>
-      <c r="X24" s="2" t="n">
-        <v>6.73</v>
+        <v>-2.21</v>
+      </c>
+      <c r="X24" t="n">
+        <v>-10.59</v>
       </c>
       <c r="Y24" t="n">
-        <v>-26.26</v>
+        <v>-100</v>
       </c>
       <c r="Z24" s="2" t="n">
-        <v>3.67</v>
-      </c>
-      <c r="AA24" t="n">
-        <v>-7.77</v>
+        <v>17.17</v>
+      </c>
+      <c r="AA24" s="2" t="n">
+        <v>5.18</v>
       </c>
       <c r="AB24" s="2" t="n">
-        <v>132</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-3.41</v>
-      </c>
-      <c r="C25" s="2" t="n">
-        <v>8.33</v>
-      </c>
-      <c r="D25" t="n">
-        <v>-21.24</v>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>3.41</v>
-      </c>
-      <c r="F25" t="n">
-        <v>-8.41</v>
-      </c>
-      <c r="G25" t="n">
-        <v>-9.359999999999999</v>
+        <v>-13.97</v>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" s="2" t="n">
+        <v>17.11</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-8.710000000000001</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>6.1</v>
       </c>
       <c r="H25" t="n">
-        <v>-4.63</v>
+        <v>-8.51</v>
       </c>
       <c r="I25" t="n">
-        <v>-18.71</v>
-      </c>
-      <c r="J25" s="2" t="n">
-        <v>7.79</v>
-      </c>
-      <c r="K25" s="2" t="n">
-        <v>2.28</v>
-      </c>
-      <c r="L25" s="2" t="n">
-        <v>22.37</v>
+        <v>-34.79</v>
+      </c>
+      <c r="J25" t="n">
+        <v>-8.869999999999999</v>
+      </c>
+      <c r="K25" t="n">
+        <v>-1.61</v>
+      </c>
+      <c r="L25" t="n">
+        <v>-17.86</v>
       </c>
       <c r="M25" t="n">
-        <v>-2.95</v>
-      </c>
-      <c r="N25" t="inlineStr"/>
+        <v>-0.85</v>
+      </c>
+      <c r="N25" t="n">
+        <v>-100</v>
+      </c>
       <c r="O25" t="n">
-        <v>-2.88</v>
-      </c>
-      <c r="P25" s="2" t="n">
-        <v>38.2</v>
+        <v>-2.47</v>
+      </c>
+      <c r="P25" t="n">
+        <v>-18.43</v>
       </c>
       <c r="Q25" t="n">
-        <v>-6.13</v>
-      </c>
-      <c r="R25" s="2" t="n">
-        <v>7.12</v>
-      </c>
-      <c r="S25" s="2" t="n">
-        <v>8.1</v>
+        <v>-11.74</v>
+      </c>
+      <c r="R25" t="n">
+        <v>-10.25</v>
+      </c>
+      <c r="S25" t="n">
+        <v>-34.18</v>
       </c>
       <c r="T25" t="n">
-        <v>-11.36</v>
+        <v>-2.67</v>
       </c>
       <c r="U25" t="n">
-        <v>-2.64</v>
+        <v>-10.56</v>
       </c>
       <c r="V25" t="inlineStr"/>
       <c r="W25" t="n">
-        <v>-14.33</v>
-      </c>
-      <c r="X25" t="n">
-        <v>-5.71</v>
-      </c>
-      <c r="Y25" s="2" t="n">
-        <v>24.21</v>
+        <v>-10.95</v>
+      </c>
+      <c r="X25" s="2" t="n">
+        <v>6.73</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>-26.26</v>
       </c>
       <c r="Z25" s="2" t="n">
-        <v>39</v>
-      </c>
-      <c r="AA25" s="2" t="n">
-        <v>1.93</v>
+        <v>3.67</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>-7.77</v>
       </c>
       <c r="AB25" s="2" t="n">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Portugal2</t>
-        </is>
-      </c>
-      <c r="B26" s="2" t="n">
-        <v>5.27</v>
-      </c>
-      <c r="C26" t="n">
-        <v>-82.78</v>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>-3.41</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>8.33</v>
       </c>
       <c r="D26" t="n">
-        <v>-14.67</v>
-      </c>
-      <c r="E26" t="n">
-        <v>-0.87</v>
+        <v>-21.24</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>3.41</v>
       </c>
       <c r="F26" t="n">
-        <v>-13.35</v>
-      </c>
-      <c r="G26" s="2" t="n">
-        <v>0.48</v>
+        <v>-8.41</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-9.359999999999999</v>
       </c>
       <c r="H26" t="n">
-        <v>-3.28</v>
-      </c>
-      <c r="I26" s="2" t="n">
-        <v>20.63</v>
-      </c>
-      <c r="J26" t="n">
-        <v>-25.74</v>
-      </c>
-      <c r="K26" t="n">
-        <v>-19.14</v>
-      </c>
-      <c r="L26" t="n">
-        <v>-53.12</v>
+        <v>-4.63</v>
+      </c>
+      <c r="I26" t="n">
+        <v>-18.71</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>7.79</v>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <v>22.37</v>
       </c>
       <c r="M26" t="n">
-        <v>-1.15</v>
+        <v>-2.95</v>
       </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>-2.33</v>
-      </c>
-      <c r="P26" t="n">
-        <v>-16.34</v>
+        <v>-2.88</v>
+      </c>
+      <c r="P26" s="2" t="n">
+        <v>38.2</v>
       </c>
       <c r="Q26" t="n">
-        <v>-25.45</v>
+        <v>-6.13</v>
       </c>
       <c r="R26" s="2" t="n">
-        <v>22.6</v>
-      </c>
-      <c r="S26" t="n">
-        <v>-12.27</v>
+        <v>7.12</v>
+      </c>
+      <c r="S26" s="2" t="n">
+        <v>8.1</v>
       </c>
       <c r="T26" t="n">
-        <v>-39.32</v>
+        <v>-11.36</v>
       </c>
       <c r="U26" t="n">
-        <v>-0.64</v>
-      </c>
-      <c r="V26" t="n">
-        <v>-10</v>
-      </c>
-      <c r="W26" s="2" t="n">
-        <v>5.76</v>
-      </c>
-      <c r="X26" s="2" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="Y26" t="n">
-        <v>-5.37</v>
+        <v>-2.64</v>
+      </c>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="n">
+        <v>-14.33</v>
+      </c>
+      <c r="X26" t="n">
+        <v>-5.71</v>
+      </c>
+      <c r="Y26" s="2" t="n">
+        <v>24.21</v>
       </c>
       <c r="Z26" s="2" t="n">
-        <v>21.47</v>
-      </c>
-      <c r="AA26" t="n">
-        <v>-7.23</v>
+        <v>39</v>
+      </c>
+      <c r="AA26" s="2" t="n">
+        <v>1.93</v>
       </c>
       <c r="AB26" s="2" t="n">
-        <v>138</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Saudiarabia</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>-10.11</v>
-      </c>
-      <c r="C27" t="inlineStr"/>
+          <t>Portugal2</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>5.27</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-82.78</v>
+      </c>
       <c r="D27" t="n">
-        <v>-5.15</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>4.29</v>
+        <v>-14.67</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-0.87</v>
       </c>
       <c r="F27" t="n">
-        <v>-3.47</v>
+        <v>-13.35</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="H27" s="2" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" s="2" t="n">
-        <v>6.54</v>
-      </c>
-      <c r="K27" s="2" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="L27" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="M27" s="2" t="n">
-        <v>1.97</v>
-      </c>
-      <c r="N27" s="2" t="n">
-        <v>195</v>
-      </c>
+        <v>0.48</v>
+      </c>
+      <c r="H27" t="n">
+        <v>-3.28</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>20.63</v>
+      </c>
+      <c r="J27" t="n">
+        <v>-25.74</v>
+      </c>
+      <c r="K27" t="n">
+        <v>-19.14</v>
+      </c>
+      <c r="L27" t="n">
+        <v>-53.12</v>
+      </c>
+      <c r="M27" t="n">
+        <v>-1.15</v>
+      </c>
+      <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>-5.05</v>
-      </c>
-      <c r="P27" s="2" t="n">
-        <v>22.39</v>
+        <v>-2.33</v>
+      </c>
+      <c r="P27" t="n">
+        <v>-16.34</v>
       </c>
       <c r="Q27" t="n">
-        <v>-15.62</v>
-      </c>
-      <c r="R27" t="n">
-        <v>-2.21</v>
-      </c>
-      <c r="S27" s="2" t="n">
-        <v>9.17</v>
+        <v>-25.45</v>
+      </c>
+      <c r="R27" s="2" t="n">
+        <v>22.6</v>
+      </c>
+      <c r="S27" t="n">
+        <v>-12.27</v>
       </c>
       <c r="T27" t="n">
-        <v>-51.43</v>
+        <v>-39.32</v>
       </c>
       <c r="U27" t="n">
-        <v>-2.35</v>
-      </c>
-      <c r="V27" t="inlineStr"/>
-      <c r="W27" t="n">
-        <v>-21.5</v>
-      </c>
-      <c r="X27" t="n">
-        <v>-11.38</v>
-      </c>
-      <c r="Y27" s="2" t="n">
-        <v>156.5</v>
+        <v>-0.64</v>
+      </c>
+      <c r="V27" t="n">
+        <v>-10</v>
+      </c>
+      <c r="W27" s="2" t="n">
+        <v>5.76</v>
+      </c>
+      <c r="X27" s="2" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>-5.37</v>
       </c>
       <c r="Z27" s="2" t="n">
-        <v>53.25</v>
-      </c>
-      <c r="AA27" s="2" t="n">
-        <v>9.26</v>
+        <v>21.47</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>-7.23</v>
       </c>
       <c r="AB27" s="2" t="n">
-        <v>39</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Scotland</t>
+          <t>Saudiarabia</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-8.41</v>
+        <v>-10.11</v>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="n">
-        <v>-16</v>
-      </c>
-      <c r="E28" t="n">
-        <v>-21.61</v>
-      </c>
-      <c r="F28" s="2" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="G28" t="n">
-        <v>-12.71</v>
+        <v>-5.15</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-3.47</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>6.5</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="I28" t="n">
-        <v>-100</v>
-      </c>
+        <v>1.33</v>
+      </c>
+      <c r="I28" t="inlineStr"/>
       <c r="J28" s="2" t="n">
-        <v>12.74</v>
-      </c>
-      <c r="K28" t="n">
-        <v>-28.78</v>
-      </c>
-      <c r="L28" t="n">
-        <v>-24.86</v>
-      </c>
-      <c r="M28" t="n">
-        <v>-26.26</v>
+        <v>6.54</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="L28" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="M28" s="2" t="n">
+        <v>1.97</v>
       </c>
       <c r="N28" s="2" t="n">
-        <v>138</v>
+        <v>195</v>
       </c>
       <c r="O28" t="n">
-        <v>-12.84</v>
+        <v>-5.05</v>
       </c>
       <c r="P28" s="2" t="n">
-        <v>11.76</v>
+        <v>22.39</v>
       </c>
       <c r="Q28" t="n">
-        <v>-22.7</v>
+        <v>-15.62</v>
       </c>
       <c r="R28" t="n">
-        <v>-7.67</v>
-      </c>
-      <c r="S28" t="n">
-        <v>-21.92</v>
+        <v>-2.21</v>
+      </c>
+      <c r="S28" s="2" t="n">
+        <v>9.17</v>
       </c>
       <c r="T28" t="n">
-        <v>-3.42</v>
+        <v>-51.43</v>
       </c>
       <c r="U28" t="n">
-        <v>-24.39</v>
+        <v>-2.35</v>
       </c>
       <c r="V28" t="inlineStr"/>
       <c r="W28" t="n">
-        <v>-19.22</v>
-      </c>
-      <c r="X28" s="2" t="n">
-        <v>13.71</v>
+        <v>-21.5</v>
+      </c>
+      <c r="X28" t="n">
+        <v>-11.38</v>
       </c>
       <c r="Y28" s="2" t="n">
-        <v>36</v>
-      </c>
-      <c r="Z28" t="n">
-        <v>-15.25</v>
-      </c>
-      <c r="AA28" t="n">
-        <v>-25.49</v>
+        <v>156.5</v>
+      </c>
+      <c r="Z28" s="2" t="n">
+        <v>53.25</v>
+      </c>
+      <c r="AA28" s="2" t="n">
+        <v>9.26</v>
       </c>
       <c r="AB28" s="2" t="n">
-        <v>81</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Scotland2</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr"/>
+          <t>Scotland</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>-8.41</v>
+      </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="n">
-        <v>-5.79</v>
-      </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" s="2" t="n">
-        <v>27.16</v>
+        <v>-16</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-21.61</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="G29" t="n">
+        <v>-12.71</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>3.43</v>
-      </c>
-      <c r="I29" s="2" t="n">
-        <v>55</v>
+        <v>1.1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>-100</v>
       </c>
       <c r="J29" s="2" t="n">
-        <v>28.71</v>
-      </c>
-      <c r="K29" s="2" t="n">
-        <v>21.8</v>
-      </c>
-      <c r="L29" s="2" t="n">
-        <v>9.630000000000001</v>
-      </c>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="n">
-        <v>-34.21</v>
-      </c>
-      <c r="O29" t="inlineStr"/>
+        <v>12.74</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-28.78</v>
+      </c>
+      <c r="L29" t="n">
+        <v>-24.86</v>
+      </c>
+      <c r="M29" t="n">
+        <v>-26.26</v>
+      </c>
+      <c r="N29" s="2" t="n">
+        <v>138</v>
+      </c>
+      <c r="O29" t="n">
+        <v>-12.84</v>
+      </c>
       <c r="P29" s="2" t="n">
-        <v>3.86</v>
+        <v>11.76</v>
       </c>
       <c r="Q29" t="n">
-        <v>-19.92</v>
-      </c>
-      <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr"/>
-      <c r="T29" s="2" t="n">
-        <v>79.11</v>
-      </c>
-      <c r="U29" t="inlineStr"/>
+        <v>-22.7</v>
+      </c>
+      <c r="R29" t="n">
+        <v>-7.67</v>
+      </c>
+      <c r="S29" t="n">
+        <v>-21.92</v>
+      </c>
+      <c r="T29" t="n">
+        <v>-3.42</v>
+      </c>
+      <c r="U29" t="n">
+        <v>-24.39</v>
+      </c>
       <c r="V29" t="inlineStr"/>
-      <c r="W29" s="2" t="n">
-        <v>12.42</v>
-      </c>
-      <c r="X29" t="inlineStr"/>
-      <c r="Y29" t="n">
-        <v>-18.42</v>
-      </c>
-      <c r="Z29" s="2" t="n">
-        <v>6.63</v>
-      </c>
-      <c r="AA29" t="inlineStr"/>
+      <c r="W29" t="n">
+        <v>-19.22</v>
+      </c>
+      <c r="X29" s="2" t="n">
+        <v>13.71</v>
+      </c>
+      <c r="Y29" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>-15.25</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>-25.49</v>
+      </c>
       <c r="AB29" s="2" t="n">
-        <v>19</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Scotland3</t>
+          <t>Scotland2</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
-        <v>-42.17</v>
+        <v>-5.79</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
-      <c r="G30" t="n">
-        <v>-26.52</v>
+      <c r="G30" s="2" t="n">
+        <v>27.16</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>15.44</v>
-      </c>
-      <c r="I30" t="n">
-        <v>-100</v>
+        <v>3.43</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>55</v>
       </c>
       <c r="J30" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="K30" t="n">
-        <v>-56</v>
-      </c>
-      <c r="L30" t="n">
-        <v>-7.04</v>
+        <v>28.71</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>21.8</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>9.630000000000001</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="n">
-        <v>-43.48</v>
+        <v>-34.21</v>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" s="2" t="n">
-        <v>74.83</v>
+        <v>3.86</v>
       </c>
       <c r="Q30" t="n">
-        <v>-13.12</v>
+        <v>-19.92</v>
       </c>
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr"/>
-      <c r="T30" t="n">
-        <v>-23.91</v>
+      <c r="T30" s="2" t="n">
+        <v>79.11</v>
       </c>
       <c r="U30" t="inlineStr"/>
       <c r="V30" t="inlineStr"/>
-      <c r="W30" t="n">
-        <v>-34.43</v>
+      <c r="W30" s="2" t="n">
+        <v>12.42</v>
       </c>
       <c r="X30" t="inlineStr"/>
       <c r="Y30" t="n">
-        <v>-49.43</v>
+        <v>-18.42</v>
       </c>
       <c r="Z30" s="2" t="n">
-        <v>27.43</v>
+        <v>6.63</v>
       </c>
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" s="2" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Scotland4</t>
+          <t>Scotland3</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="n">
-        <v>-38.23</v>
+        <v>-42.17</v>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="n">
-        <v>-38.85</v>
+        <v>-26.52</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>6.09</v>
-      </c>
-      <c r="I31" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="J31" t="n">
-        <v>-30.18</v>
-      </c>
-      <c r="K31" s="2" t="n">
-        <v>94</v>
+        <v>15.44</v>
+      </c>
+      <c r="I31" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="K31" t="n">
+        <v>-56</v>
       </c>
       <c r="L31" t="n">
-        <v>-46.15</v>
+        <v>-7.04</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="n">
-        <v>-57.69</v>
+        <v>-43.48</v>
       </c>
       <c r="O31" t="inlineStr"/>
-      <c r="P31" t="n">
-        <v>-6.75</v>
-      </c>
-      <c r="Q31" s="2" t="n">
-        <v>47.56</v>
+      <c r="P31" s="2" t="n">
+        <v>74.83</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>-13.12</v>
       </c>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="n">
-        <v>-25.77</v>
+        <v>-23.91</v>
       </c>
       <c r="U31" t="inlineStr"/>
       <c r="V31" t="inlineStr"/>
       <c r="W31" t="n">
-        <v>-36.08</v>
+        <v>-34.43</v>
       </c>
       <c r="X31" t="inlineStr"/>
       <c r="Y31" t="n">
-        <v>-35.54</v>
-      </c>
-      <c r="Z31" t="n">
-        <v>-30.77</v>
+        <v>-49.43</v>
+      </c>
+      <c r="Z31" s="2" t="n">
+        <v>27.43</v>
       </c>
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" s="2" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>-14.03</v>
-      </c>
-      <c r="C32" t="n">
-        <v>-50.83</v>
-      </c>
+          <t>Scotland4</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
       <c r="D32" t="n">
-        <v>-5.46</v>
-      </c>
-      <c r="E32" t="n">
-        <v>-5.53</v>
-      </c>
-      <c r="F32" t="n">
-        <v>-19.78</v>
-      </c>
+        <v>-38.23</v>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
       <c r="G32" t="n">
-        <v>-17.44</v>
-      </c>
-      <c r="H32" t="n">
-        <v>-3.12</v>
-      </c>
-      <c r="I32" t="n">
-        <v>-30.5</v>
-      </c>
-      <c r="J32" s="2" t="n">
-        <v>2.18</v>
-      </c>
-      <c r="K32" t="n">
-        <v>-5.05</v>
+        <v>-38.85</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J32" t="n">
+        <v>-30.18</v>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>94</v>
       </c>
       <c r="L32" t="n">
-        <v>-22.85</v>
-      </c>
-      <c r="M32" s="2" t="n">
-        <v>2.92</v>
-      </c>
+        <v>-46.15</v>
+      </c>
+      <c r="M32" t="inlineStr"/>
       <c r="N32" t="n">
-        <v>-100</v>
-      </c>
-      <c r="O32" t="n">
-        <v>-1.28</v>
-      </c>
-      <c r="P32" s="2" t="n">
-        <v>3.26</v>
-      </c>
-      <c r="Q32" t="n">
-        <v>-25.17</v>
-      </c>
-      <c r="R32" s="2" t="n">
-        <v>14.4</v>
-      </c>
-      <c r="S32" t="n">
-        <v>-16.69</v>
-      </c>
+        <v>-57.69</v>
+      </c>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="n">
+        <v>-6.75</v>
+      </c>
+      <c r="Q32" s="2" t="n">
+        <v>47.56</v>
+      </c>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr"/>
       <c r="T32" t="n">
-        <v>-56.42</v>
-      </c>
-      <c r="U32" t="n">
-        <v>-3.09</v>
-      </c>
-      <c r="V32" s="2" t="n">
-        <v>57</v>
-      </c>
+        <v>-25.77</v>
+      </c>
+      <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr"/>
       <c r="W32" t="n">
-        <v>-7.98</v>
-      </c>
-      <c r="X32" t="n">
-        <v>-6.98</v>
-      </c>
+        <v>-36.08</v>
+      </c>
+      <c r="X32" t="inlineStr"/>
       <c r="Y32" t="n">
-        <v>-32.68</v>
+        <v>-35.54</v>
       </c>
       <c r="Z32" t="n">
-        <v>-59.54</v>
-      </c>
-      <c r="AA32" t="n">
-        <v>-1.42</v>
-      </c>
+        <v>-30.77</v>
+      </c>
+      <c r="AA32" t="inlineStr"/>
       <c r="AB32" s="2" t="n">
-        <v>131</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Spain2</t>
-        </is>
-      </c>
-      <c r="B33" s="2" t="n">
-        <v>3.31</v>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-14.03</v>
       </c>
       <c r="C33" t="n">
-        <v>-52.86</v>
+        <v>-50.83</v>
       </c>
       <c r="D33" t="n">
-        <v>-7.28</v>
+        <v>-5.46</v>
       </c>
       <c r="E33" t="n">
-        <v>-1.53</v>
+        <v>-5.53</v>
       </c>
       <c r="F33" t="n">
-        <v>-8.6</v>
+        <v>-19.78</v>
       </c>
       <c r="G33" t="n">
-        <v>-7.89</v>
+        <v>-17.44</v>
       </c>
       <c r="H33" t="n">
-        <v>-2.85</v>
-      </c>
-      <c r="I33" s="2" t="n">
-        <v>40.27</v>
+        <v>-3.12</v>
+      </c>
+      <c r="I33" t="n">
+        <v>-30.5</v>
       </c>
       <c r="J33" s="2" t="n">
-        <v>15.19</v>
+        <v>2.18</v>
       </c>
       <c r="K33" t="n">
-        <v>-8.609999999999999</v>
+        <v>-5.05</v>
       </c>
       <c r="L33" t="n">
-        <v>-6.82</v>
-      </c>
-      <c r="M33" t="n">
-        <v>-7.19</v>
-      </c>
-      <c r="N33" s="2" t="n">
-        <v>50</v>
+        <v>-22.85</v>
+      </c>
+      <c r="M33" s="2" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="N33" t="n">
+        <v>-100</v>
       </c>
       <c r="O33" t="n">
-        <v>-2.95</v>
+        <v>-1.28</v>
       </c>
       <c r="P33" s="2" t="n">
-        <v>3.97</v>
+        <v>3.26</v>
       </c>
       <c r="Q33" t="n">
-        <v>-7.47</v>
+        <v>-25.17</v>
       </c>
       <c r="R33" s="2" t="n">
-        <v>10.94</v>
+        <v>14.4</v>
       </c>
       <c r="S33" t="n">
-        <v>-19.98</v>
+        <v>-16.69</v>
       </c>
       <c r="T33" t="n">
-        <v>-52.5</v>
+        <v>-56.42</v>
       </c>
       <c r="U33" t="n">
-        <v>-3.72</v>
+        <v>-3.09</v>
       </c>
       <c r="V33" s="2" t="n">
-        <v>0.7</v>
+        <v>57</v>
       </c>
       <c r="W33" t="n">
-        <v>-21.18</v>
+        <v>-7.98</v>
       </c>
       <c r="X33" t="n">
-        <v>-5.65</v>
+        <v>-6.98</v>
       </c>
       <c r="Y33" t="n">
-        <v>-51.38</v>
-      </c>
-      <c r="Z33" s="2" t="n">
-        <v>26.25</v>
+        <v>-32.68</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>-59.54</v>
       </c>
       <c r="AA33" t="n">
-        <v>-3.49</v>
+        <v>-1.42</v>
       </c>
       <c r="AB33" s="2" t="n">
-        <v>196</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Sweden</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>-7.95</v>
-      </c>
-      <c r="C34" t="inlineStr"/>
+          <t>Spain2</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="C34" t="n">
+        <v>-52.86</v>
+      </c>
       <c r="D34" t="n">
-        <v>-24</v>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>11.33</v>
+        <v>-7.28</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-1.53</v>
       </c>
       <c r="F34" t="n">
-        <v>-7.17</v>
+        <v>-8.6</v>
       </c>
       <c r="G34" t="n">
-        <v>-36.5</v>
+        <v>-7.89</v>
       </c>
       <c r="H34" t="n">
-        <v>-7.29</v>
-      </c>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="n">
-        <v>-30.71</v>
-      </c>
-      <c r="K34" s="2" t="n">
-        <v>13.62</v>
+        <v>-2.85</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <v>40.27</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <v>15.19</v>
+      </c>
+      <c r="K34" t="n">
+        <v>-8.609999999999999</v>
       </c>
       <c r="L34" t="n">
+        <v>-6.82</v>
+      </c>
+      <c r="M34" t="n">
+        <v>-7.19</v>
+      </c>
+      <c r="N34" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="O34" t="n">
+        <v>-2.95</v>
+      </c>
+      <c r="P34" s="2" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>-7.47</v>
+      </c>
+      <c r="R34" s="2" t="n">
+        <v>10.94</v>
+      </c>
+      <c r="S34" t="n">
+        <v>-19.98</v>
+      </c>
+      <c r="T34" t="n">
         <v>-52.5</v>
       </c>
-      <c r="M34" s="2" t="n">
-        <v>19.96</v>
-      </c>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" s="2" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="P34" t="n">
-        <v>-5.97</v>
-      </c>
-      <c r="Q34" t="n">
-        <v>-1.3</v>
-      </c>
-      <c r="R34" t="n">
-        <v>-49.6</v>
-      </c>
-      <c r="S34" t="n">
-        <v>-18.82</v>
-      </c>
-      <c r="T34" t="n">
-        <v>-24</v>
-      </c>
       <c r="U34" t="n">
-        <v>-12.67</v>
-      </c>
-      <c r="V34" t="inlineStr"/>
-      <c r="W34" s="2" t="n">
-        <v>3.52</v>
+        <v>-3.72</v>
+      </c>
+      <c r="V34" s="2" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="W34" t="n">
+        <v>-21.18</v>
       </c>
       <c r="X34" t="n">
-        <v>-11.24</v>
+        <v>-5.65</v>
       </c>
       <c r="Y34" t="n">
-        <v>-100</v>
+        <v>-51.38</v>
       </c>
       <c r="Z34" s="2" t="n">
-        <v>18.44</v>
-      </c>
-      <c r="AA34" s="2" t="n">
-        <v>10.98</v>
+        <v>26.25</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>-3.49</v>
       </c>
       <c r="AB34" s="2" t="n">
-        <v>58</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Switzerland</t>
-        </is>
-      </c>
-      <c r="B35" s="2" t="n">
-        <v>2.52</v>
+          <t>Sweden</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-7.95</v>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="n">
-        <v>-43.25</v>
+        <v>-24</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>0.57</v>
+        <v>11.33</v>
       </c>
       <c r="F35" t="n">
-        <v>-8.9</v>
+        <v>-7.17</v>
       </c>
       <c r="G35" t="n">
-        <v>-11.77</v>
-      </c>
-      <c r="H35" s="2" t="n">
-        <v>9.300000000000001</v>
+        <v>-36.5</v>
+      </c>
+      <c r="H35" t="n">
+        <v>-7.29</v>
       </c>
       <c r="I35" t="inlineStr"/>
-      <c r="J35" s="2" t="n">
-        <v>5.78</v>
+      <c r="J35" t="n">
+        <v>-30.71</v>
       </c>
       <c r="K35" s="2" t="n">
-        <v>10.76</v>
-      </c>
-      <c r="L35" s="2" t="n">
-        <v>29.78</v>
-      </c>
-      <c r="M35" t="n">
-        <v>-0.97</v>
-      </c>
-      <c r="N35" s="2" t="n">
-        <v>333</v>
-      </c>
-      <c r="O35" t="n">
-        <v>-6.88</v>
-      </c>
-      <c r="P35" s="2" t="n">
-        <v>2.39</v>
+        <v>13.62</v>
+      </c>
+      <c r="L35" t="n">
+        <v>-52.5</v>
+      </c>
+      <c r="M35" s="2" t="n">
+        <v>19.96</v>
+      </c>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" s="2" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P35" t="n">
+        <v>-5.97</v>
       </c>
       <c r="Q35" t="n">
-        <v>-19.94</v>
-      </c>
-      <c r="R35" s="2" t="n">
-        <v>24</v>
+        <v>-1.3</v>
+      </c>
+      <c r="R35" t="n">
+        <v>-49.6</v>
       </c>
       <c r="S35" t="n">
-        <v>-16.37</v>
-      </c>
-      <c r="T35" s="2" t="n">
-        <v>49.46</v>
+        <v>-18.82</v>
+      </c>
+      <c r="T35" t="n">
+        <v>-24</v>
       </c>
       <c r="U35" t="n">
-        <v>-5.51</v>
-      </c>
-      <c r="V35" t="n">
-        <v>-100</v>
-      </c>
-      <c r="W35" t="n">
-        <v>-13.87</v>
-      </c>
-      <c r="X35" s="2" t="n">
-        <v>3.19</v>
+        <v>-12.67</v>
+      </c>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" s="2" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="X35" t="n">
+        <v>-11.24</v>
       </c>
       <c r="Y35" t="n">
         <v>-100</v>
       </c>
-      <c r="Z35" t="n">
-        <v>-19.89</v>
-      </c>
-      <c r="AA35" t="n">
-        <v>-15.27</v>
+      <c r="Z35" s="2" t="n">
+        <v>18.44</v>
+      </c>
+      <c r="AA35" s="2" t="n">
+        <v>10.98</v>
       </c>
       <c r="AB35" s="2" t="n">
-        <v>82</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>11.89</v>
-      </c>
-      <c r="C36" s="2" t="n">
-        <v>33.89</v>
-      </c>
+        <v>2.52</v>
+      </c>
+      <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
-        <v>-30.26</v>
-      </c>
-      <c r="E36" t="n">
-        <v>-3.88</v>
+        <v>-43.25</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>0.57</v>
       </c>
       <c r="F36" t="n">
-        <v>-8.6</v>
+        <v>-8.9</v>
       </c>
       <c r="G36" t="n">
-        <v>-23.34</v>
-      </c>
-      <c r="H36" t="n">
-        <v>-5.5</v>
-      </c>
-      <c r="I36" s="2" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="J36" t="n">
-        <v>-7.56</v>
-      </c>
-      <c r="K36" t="n">
-        <v>-28.31</v>
-      </c>
-      <c r="L36" t="n">
-        <v>-3.12</v>
+        <v>-11.77</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" s="2" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="K36" s="2" t="n">
+        <v>10.76</v>
+      </c>
+      <c r="L36" s="2" t="n">
+        <v>29.78</v>
       </c>
       <c r="M36" t="n">
-        <v>-8.41</v>
-      </c>
-      <c r="N36" t="n">
-        <v>-100</v>
+        <v>-0.97</v>
+      </c>
+      <c r="N36" s="2" t="n">
+        <v>333</v>
       </c>
       <c r="O36" t="n">
-        <v>-8.529999999999999</v>
-      </c>
-      <c r="P36" t="n">
-        <v>-12.64</v>
+        <v>-6.88</v>
+      </c>
+      <c r="P36" s="2" t="n">
+        <v>2.39</v>
       </c>
       <c r="Q36" t="n">
-        <v>-24.23</v>
-      </c>
-      <c r="R36" t="n">
-        <v>-9.08</v>
+        <v>-19.94</v>
+      </c>
+      <c r="R36" s="2" t="n">
+        <v>24</v>
       </c>
       <c r="S36" t="n">
-        <v>-15.68</v>
-      </c>
-      <c r="T36" t="n">
-        <v>-4.44</v>
-      </c>
-      <c r="U36" s="2" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="V36" t="inlineStr"/>
+        <v>-16.37</v>
+      </c>
+      <c r="T36" s="2" t="n">
+        <v>49.46</v>
+      </c>
+      <c r="U36" t="n">
+        <v>-5.51</v>
+      </c>
+      <c r="V36" t="n">
+        <v>-100</v>
+      </c>
       <c r="W36" t="n">
-        <v>-10.9</v>
-      </c>
-      <c r="X36" t="n">
-        <v>-2.27</v>
+        <v>-13.87</v>
+      </c>
+      <c r="X36" s="2" t="n">
+        <v>3.19</v>
       </c>
       <c r="Y36" t="n">
-        <v>-28.57</v>
+        <v>-100</v>
       </c>
       <c r="Z36" t="n">
-        <v>-26.65</v>
+        <v>-19.89</v>
       </c>
       <c r="AA36" t="n">
-        <v>-6.94</v>
+        <v>-15.27</v>
       </c>
       <c r="AB36" s="2" t="n">
-        <v>168</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>UCL</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>6.62</v>
-      </c>
-      <c r="C37" t="n">
-        <v>-100</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <v>8.27</v>
+        <v>11.89</v>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>33.89</v>
+      </c>
+      <c r="D37" t="n">
+        <v>-30.26</v>
       </c>
       <c r="E37" t="n">
-        <v>-10</v>
-      </c>
-      <c r="F37" s="2" t="n">
-        <v>5.78</v>
+        <v>-3.88</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-8.6</v>
       </c>
       <c r="G37" t="n">
-        <v>-34.25</v>
+        <v>-23.34</v>
       </c>
       <c r="H37" t="n">
-        <v>-8.279999999999999</v>
+        <v>-5.5</v>
       </c>
       <c r="I37" s="2" t="n">
-        <v>45.75</v>
-      </c>
-      <c r="J37" s="2" t="n">
-        <v>5.79</v>
+        <v>2.6</v>
+      </c>
+      <c r="J37" t="n">
+        <v>-7.56</v>
       </c>
       <c r="K37" t="n">
-        <v>-24.36</v>
+        <v>-28.31</v>
       </c>
       <c r="L37" t="n">
-        <v>-15</v>
+        <v>-3.12</v>
       </c>
       <c r="M37" t="n">
-        <v>-6.53</v>
-      </c>
-      <c r="N37" s="2" t="n">
-        <v>21.25</v>
+        <v>-8.41</v>
+      </c>
+      <c r="N37" t="n">
+        <v>-100</v>
       </c>
       <c r="O37" t="n">
-        <v>-5.58</v>
-      </c>
-      <c r="P37" s="2" t="n">
-        <v>12.15</v>
-      </c>
-      <c r="Q37" s="2" t="n">
-        <v>9.27</v>
-      </c>
-      <c r="R37" s="2" t="n">
-        <v>4.71</v>
+        <v>-8.529999999999999</v>
+      </c>
+      <c r="P37" t="n">
+        <v>-12.64</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>-24.23</v>
+      </c>
+      <c r="R37" t="n">
+        <v>-9.08</v>
       </c>
       <c r="S37" t="n">
-        <v>-13.19</v>
-      </c>
-      <c r="T37" s="2" t="n">
-        <v>20.31</v>
-      </c>
-      <c r="U37" t="n">
-        <v>-6.73</v>
-      </c>
-      <c r="V37" t="n">
-        <v>-48.83</v>
-      </c>
+        <v>-15.68</v>
+      </c>
+      <c r="T37" t="n">
+        <v>-4.44</v>
+      </c>
+      <c r="U37" s="2" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="V37" t="inlineStr"/>
       <c r="W37" t="n">
-        <v>-8.48</v>
-      </c>
-      <c r="X37" s="2" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="Y37" s="2" t="n">
-        <v>25.3</v>
+        <v>-10.9</v>
+      </c>
+      <c r="X37" t="n">
+        <v>-2.27</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>-28.57</v>
       </c>
       <c r="Z37" t="n">
-        <v>-5.69</v>
+        <v>-26.65</v>
       </c>
       <c r="AA37" t="n">
-        <v>-7.5</v>
+        <v>-6.94</v>
       </c>
       <c r="AB37" s="2" t="n">
-        <v>61</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>UEL</t>
+          <t>UCL</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>26.82</v>
-      </c>
-      <c r="C38" s="2" t="n">
-        <v>65</v>
+        <v>6.62</v>
+      </c>
+      <c r="C38" t="n">
+        <v>-100</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>5.29</v>
-      </c>
-      <c r="E38" s="2" t="n">
-        <v>1.88</v>
-      </c>
-      <c r="F38" t="n">
-        <v>-1.22</v>
+        <v>8.27</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-10</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>5.78</v>
       </c>
       <c r="G38" t="n">
-        <v>-10.27</v>
+        <v>-34.25</v>
       </c>
       <c r="H38" t="n">
-        <v>-2.02</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0</v>
-      </c>
-      <c r="J38" t="n">
-        <v>-15.19</v>
+        <v>-8.279999999999999</v>
+      </c>
+      <c r="I38" s="2" t="n">
+        <v>45.75</v>
+      </c>
+      <c r="J38" s="2" t="n">
+        <v>5.79</v>
       </c>
       <c r="K38" t="n">
-        <v>-35.14</v>
+        <v>-24.36</v>
       </c>
       <c r="L38" t="n">
-        <v>-47.5</v>
+        <v>-15</v>
       </c>
       <c r="M38" t="n">
-        <v>-15.27</v>
+        <v>-6.53</v>
       </c>
       <c r="N38" s="2" t="n">
-        <v>25</v>
+        <v>21.25</v>
       </c>
       <c r="O38" t="n">
-        <v>-3.34</v>
-      </c>
-      <c r="P38" t="n">
-        <v>-19.73</v>
-      </c>
-      <c r="Q38" t="n">
-        <v>-10.85</v>
-      </c>
-      <c r="R38" t="n">
-        <v>-2.2</v>
+        <v>-5.58</v>
+      </c>
+      <c r="P38" s="2" t="n">
+        <v>12.15</v>
+      </c>
+      <c r="Q38" s="2" t="n">
+        <v>9.27</v>
+      </c>
+      <c r="R38" s="2" t="n">
+        <v>4.71</v>
       </c>
       <c r="S38" t="n">
-        <v>-16.09</v>
-      </c>
-      <c r="T38" t="n">
-        <v>-16.67</v>
-      </c>
-      <c r="U38" s="2" t="n">
-        <v>4.59</v>
-      </c>
-      <c r="V38" s="2" t="n">
-        <v>57</v>
+        <v>-13.19</v>
+      </c>
+      <c r="T38" s="2" t="n">
+        <v>20.31</v>
+      </c>
+      <c r="U38" t="n">
+        <v>-6.73</v>
+      </c>
+      <c r="V38" t="n">
+        <v>-48.83</v>
       </c>
       <c r="W38" t="n">
-        <v>-24.04</v>
-      </c>
-      <c r="X38" t="n">
-        <v>-2.27</v>
-      </c>
-      <c r="Y38" t="n">
-        <v>-25</v>
-      </c>
-      <c r="Z38" s="2" t="n">
-        <v>18.33</v>
+        <v>-8.48</v>
+      </c>
+      <c r="X38" s="2" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="Y38" s="2" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>-5.69</v>
       </c>
       <c r="AA38" t="n">
-        <v>-12.63</v>
+        <v>-7.5</v>
       </c>
       <c r="AB38" s="2" t="n">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>UFCL</t>
+          <t>UEL</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>25.45</v>
-      </c>
-      <c r="C39" t="n">
-        <v>-100</v>
+        <v>26.82</v>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>65</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>6.82</v>
-      </c>
-      <c r="E39" t="n">
-        <v>-31.88</v>
-      </c>
-      <c r="F39" s="2" t="n">
-        <v>13.11</v>
-      </c>
-      <c r="G39" s="2" t="n">
-        <v>4.79</v>
+        <v>5.29</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-1.22</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-10.27</v>
       </c>
       <c r="H39" t="n">
-        <v>-2</v>
-      </c>
-      <c r="I39" s="2" t="n">
-        <v>58.33</v>
-      </c>
-      <c r="J39" s="2" t="n">
-        <v>3.14</v>
+        <v>-2.02</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>-15.19</v>
       </c>
       <c r="K39" t="n">
-        <v>-13.63</v>
+        <v>-35.14</v>
       </c>
       <c r="L39" t="n">
-        <v>-31.67</v>
+        <v>-47.5</v>
       </c>
       <c r="M39" t="n">
-        <v>-9.859999999999999</v>
-      </c>
-      <c r="N39" t="n">
-        <v>-100</v>
-      </c>
-      <c r="O39" s="2" t="n">
-        <v>0.47</v>
+        <v>-15.27</v>
+      </c>
+      <c r="N39" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="O39" t="n">
+        <v>-3.34</v>
       </c>
       <c r="P39" t="n">
-        <v>-24.19</v>
+        <v>-19.73</v>
       </c>
       <c r="Q39" t="n">
-        <v>-9.92</v>
-      </c>
-      <c r="R39" s="2" t="n">
-        <v>15.71</v>
-      </c>
-      <c r="S39" s="2" t="n">
-        <v>20.38</v>
+        <v>-10.85</v>
+      </c>
+      <c r="R39" t="n">
+        <v>-2.2</v>
+      </c>
+      <c r="S39" t="n">
+        <v>-16.09</v>
       </c>
       <c r="T39" t="n">
-        <v>-28</v>
-      </c>
-      <c r="U39" t="n">
-        <v>-0.41</v>
+        <v>-16.67</v>
+      </c>
+      <c r="U39" s="2" t="n">
+        <v>4.59</v>
       </c>
       <c r="V39" s="2" t="n">
         <v>57</v>
       </c>
-      <c r="W39" s="2" t="n">
-        <v>10.53</v>
+      <c r="W39" t="n">
+        <v>-24.04</v>
       </c>
       <c r="X39" t="n">
-        <v>-4.29</v>
-      </c>
-      <c r="Y39" s="2" t="n">
-        <v>40.81</v>
-      </c>
-      <c r="Z39" t="n">
-        <v>-39.31</v>
+        <v>-2.27</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>-25</v>
+      </c>
+      <c r="Z39" s="2" t="n">
+        <v>18.33</v>
       </c>
       <c r="AA39" t="n">
-        <v>-11.07</v>
+        <v>-12.63</v>
       </c>
       <c r="AB39" s="2" t="n">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>UNL</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>-21.18</v>
-      </c>
-      <c r="C40" s="2" t="n">
-        <v>64.17</v>
+          <t>UFCL</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="n">
+        <v>25.45</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-100</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>5.71</v>
+        <v>6.82</v>
       </c>
       <c r="E40" t="n">
-        <v>-11.52</v>
-      </c>
-      <c r="F40" t="n">
-        <v>-2.62</v>
+        <v>-31.88</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>13.11</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>12.91</v>
+        <v>4.79</v>
       </c>
       <c r="H40" t="n">
-        <v>-11.86</v>
+        <v>-2</v>
       </c>
       <c r="I40" s="2" t="n">
-        <v>5.92</v>
+        <v>58.33</v>
       </c>
       <c r="J40" s="2" t="n">
-        <v>2.67</v>
-      </c>
-      <c r="K40" s="2" t="n">
-        <v>23.74</v>
-      </c>
-      <c r="L40" s="2" t="n">
-        <v>31.58</v>
-      </c>
-      <c r="M40" s="2" t="n">
-        <v>2.75</v>
-      </c>
-      <c r="N40" s="2" t="n">
-        <v>208.33</v>
-      </c>
-      <c r="O40" t="n">
-        <v>-7.44</v>
-      </c>
-      <c r="P40" s="2" t="n">
-        <v>21.23</v>
+        <v>3.14</v>
+      </c>
+      <c r="K40" t="n">
+        <v>-13.63</v>
+      </c>
+      <c r="L40" t="n">
+        <v>-31.67</v>
+      </c>
+      <c r="M40" t="n">
+        <v>-9.859999999999999</v>
+      </c>
+      <c r="N40" t="n">
+        <v>-100</v>
+      </c>
+      <c r="O40" s="2" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="P40" t="n">
+        <v>-24.19</v>
       </c>
       <c r="Q40" t="n">
-        <v>-2.06</v>
+        <v>-9.92</v>
       </c>
       <c r="R40" s="2" t="n">
-        <v>1.92</v>
-      </c>
-      <c r="S40" t="n">
-        <v>-3</v>
-      </c>
-      <c r="T40" s="2" t="n">
-        <v>37.43</v>
+        <v>15.71</v>
+      </c>
+      <c r="S40" s="2" t="n">
+        <v>20.38</v>
+      </c>
+      <c r="T40" t="n">
+        <v>-28</v>
       </c>
       <c r="U40" t="n">
-        <v>-9.869999999999999</v>
-      </c>
-      <c r="V40" t="inlineStr"/>
+        <v>-0.41</v>
+      </c>
+      <c r="V40" s="2" t="n">
+        <v>57</v>
+      </c>
       <c r="W40" s="2" t="n">
-        <v>5.11</v>
+        <v>10.53</v>
       </c>
       <c r="X40" t="n">
-        <v>-18.68</v>
-      </c>
-      <c r="Y40" t="n">
-        <v>-4.21</v>
+        <v>-4.29</v>
+      </c>
+      <c r="Y40" s="2" t="n">
+        <v>40.81</v>
       </c>
       <c r="Z40" t="n">
-        <v>-15.11</v>
-      </c>
-      <c r="AA40" s="2" t="n">
-        <v>8.31</v>
+        <v>-39.31</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>-11.07</v>
       </c>
       <c r="AB40" s="2" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Usa</t>
+          <t>UNL</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-29.68</v>
-      </c>
-      <c r="C41" t="inlineStr"/>
+        <v>-21.18</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>64.17</v>
+      </c>
       <c r="D41" s="2" t="n">
-        <v>47.36</v>
+        <v>5.71</v>
       </c>
       <c r="E41" t="n">
-        <v>-15</v>
-      </c>
-      <c r="F41" s="2" t="n">
-        <v>10.56</v>
+        <v>-11.52</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-2.62</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>23.25</v>
+        <v>12.91</v>
       </c>
       <c r="H41" t="n">
-        <v>-5.82</v>
-      </c>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="n">
-        <v>-3.44</v>
-      </c>
-      <c r="K41" t="n">
-        <v>-59.4</v>
+        <v>-11.86</v>
+      </c>
+      <c r="I41" s="2" t="n">
+        <v>5.92</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="K41" s="2" t="n">
+        <v>23.74</v>
       </c>
       <c r="L41" s="2" t="n">
-        <v>5.2</v>
+        <v>31.58</v>
       </c>
       <c r="M41" s="2" t="n">
-        <v>9.67</v>
-      </c>
-      <c r="N41" t="inlineStr"/>
+        <v>2.75</v>
+      </c>
+      <c r="N41" s="2" t="n">
+        <v>208.33</v>
+      </c>
       <c r="O41" t="n">
-        <v>-0.59</v>
-      </c>
-      <c r="P41" t="n">
-        <v>-0.46</v>
+        <v>-7.44</v>
+      </c>
+      <c r="P41" s="2" t="n">
+        <v>21.23</v>
       </c>
       <c r="Q41" t="n">
-        <v>-19</v>
-      </c>
-      <c r="R41" t="n">
-        <v>-6.04</v>
-      </c>
-      <c r="S41" s="2" t="n">
-        <v>2.26</v>
-      </c>
-      <c r="T41" t="n">
-        <v>-34.25</v>
+        <v>-2.06</v>
+      </c>
+      <c r="R41" s="2" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="S41" t="n">
+        <v>-3</v>
+      </c>
+      <c r="T41" s="2" t="n">
+        <v>37.43</v>
       </c>
       <c r="U41" t="n">
-        <v>-5.8</v>
+        <v>-9.869999999999999</v>
       </c>
       <c r="V41" t="inlineStr"/>
-      <c r="W41" t="n">
-        <v>-8.550000000000001</v>
+      <c r="W41" s="2" t="n">
+        <v>5.11</v>
       </c>
       <c r="X41" t="n">
-        <v>-8.84</v>
-      </c>
-      <c r="Y41" t="inlineStr"/>
-      <c r="Z41" s="2" t="n">
-        <v>24</v>
+        <v>-18.68</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>-4.21</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>-15.11</v>
       </c>
       <c r="AA41" s="2" t="n">
-        <v>14.32</v>
+        <v>8.31</v>
       </c>
       <c r="AB41" s="2" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>england2</t>
-        </is>
-      </c>
-      <c r="B42" s="2" t="n">
-        <v>43.8</v>
-      </c>
-      <c r="C42" t="n">
-        <v>-100</v>
-      </c>
-      <c r="D42" t="n">
-        <v>-59.5</v>
-      </c>
-      <c r="E42" s="2" t="n">
-        <v>2</v>
+          <t>Usa</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>-29.68</v>
+      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" s="2" t="n">
+        <v>47.36</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-15</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>29</v>
+        <v>10.56</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>12</v>
+        <v>23.25</v>
       </c>
       <c r="H42" t="n">
-        <v>-37.25</v>
-      </c>
-      <c r="I42" t="n">
-        <v>-100</v>
-      </c>
+        <v>-5.82</v>
+      </c>
+      <c r="I42" t="inlineStr"/>
       <c r="J42" t="n">
-        <v>-10.5</v>
+        <v>-1.14</v>
       </c>
       <c r="K42" t="n">
-        <v>-18.43</v>
-      </c>
-      <c r="L42" t="n">
-        <v>-100</v>
-      </c>
-      <c r="M42" t="n">
-        <v>-1.71</v>
-      </c>
-      <c r="N42" t="n">
-        <v>-100</v>
-      </c>
-      <c r="O42" s="2" t="n">
-        <v>3.2</v>
+        <v>-54.89</v>
+      </c>
+      <c r="L42" s="2" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="M42" s="2" t="n">
+        <v>9.74</v>
+      </c>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="n">
+        <v>-0.59</v>
       </c>
       <c r="P42" t="n">
-        <v>-13.5</v>
+        <v>-2.57</v>
       </c>
       <c r="Q42" t="n">
-        <v>-14</v>
-      </c>
-      <c r="R42" s="2" t="n">
-        <v>8.33</v>
-      </c>
-      <c r="S42" t="n">
-        <v>-36.43</v>
+        <v>-50</v>
+      </c>
+      <c r="R42" t="n">
+        <v>-9.279999999999999</v>
+      </c>
+      <c r="S42" s="2" t="n">
+        <v>7.94</v>
       </c>
       <c r="T42" t="n">
-        <v>-100</v>
+        <v>-34.25</v>
       </c>
       <c r="U42" t="n">
-        <v>-18.56</v>
+        <v>-5.8</v>
       </c>
       <c r="V42" t="inlineStr"/>
-      <c r="W42" s="2" t="n">
-        <v>21</v>
+      <c r="W42" t="n">
+        <v>-8.550000000000001</v>
       </c>
       <c r="X42" t="n">
-        <v>-23.14</v>
-      </c>
-      <c r="Y42" t="n">
-        <v>-31.25</v>
-      </c>
-      <c r="Z42" t="n">
-        <v>-100</v>
+        <v>-8.92</v>
+      </c>
+      <c r="Y42" t="inlineStr"/>
+      <c r="Z42" s="2" t="n">
+        <v>24</v>
       </c>
       <c r="AA42" s="2" t="n">
-        <v>4.5</v>
+        <v>14.32</v>
       </c>
       <c r="AB42" s="2" t="n">
-        <v>11</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>england3</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>-29.78</v>
-      </c>
-      <c r="C43" t="inlineStr"/>
+          <t>england2</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>43.8</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-100</v>
+      </c>
       <c r="D43" t="n">
-        <v>-30</v>
-      </c>
-      <c r="E43" t="n">
-        <v>-26.75</v>
+        <v>-59.5</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="F43" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="G43" t="n">
-        <v>-54.67</v>
-      </c>
-      <c r="H43" s="2" t="n">
-        <v>10.45</v>
+      <c r="G43" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="H43" t="n">
+        <v>-37.25</v>
       </c>
       <c r="I43" t="n">
         <v>-100</v>
       </c>
-      <c r="J43" s="2" t="n">
-        <v>40.6</v>
+      <c r="J43" t="n">
+        <v>-10.5</v>
       </c>
       <c r="K43" t="n">
-        <v>-44.57</v>
+        <v>-18.43</v>
       </c>
       <c r="L43" t="n">
         <v>-100</v>
       </c>
       <c r="M43" t="n">
-        <v>-18.3</v>
+        <v>-1.71</v>
       </c>
       <c r="N43" t="n">
         <v>-100</v>
       </c>
-      <c r="O43" t="n">
-        <v>-20.4</v>
-      </c>
-      <c r="P43" s="2" t="n">
-        <v>26</v>
+      <c r="O43" s="2" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="P43" t="n">
+        <v>-13.5</v>
       </c>
       <c r="Q43" t="n">
-        <v>-48.12</v>
-      </c>
-      <c r="R43" t="n">
-        <v>0</v>
+        <v>-14</v>
+      </c>
+      <c r="R43" s="2" t="n">
+        <v>8.33</v>
       </c>
       <c r="S43" t="n">
-        <v>-70</v>
-      </c>
-      <c r="T43" s="2" t="n">
-        <v>138</v>
+        <v>-36.43</v>
+      </c>
+      <c r="T43" t="n">
+        <v>-100</v>
       </c>
       <c r="U43" t="n">
-        <v>-26.5</v>
+        <v>-18.56</v>
       </c>
       <c r="V43" t="inlineStr"/>
       <c r="W43" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="X43" s="2" t="n">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="X43" t="n">
+        <v>-23.14</v>
       </c>
       <c r="Y43" t="n">
-        <v>-100</v>
-      </c>
-      <c r="Z43" s="2" t="n">
-        <v>22</v>
-      </c>
-      <c r="AA43" t="n">
-        <v>-48</v>
+        <v>-31.25</v>
+      </c>
+      <c r="Z43" t="n">
+        <v>-100</v>
+      </c>
+      <c r="AA43" s="2" t="n">
+        <v>4.5</v>
       </c>
       <c r="AB43" s="2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>england4</t>
+          <t>england3</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>-29.6</v>
+        <v>-29.78</v>
       </c>
       <c r="C44" t="inlineStr"/>
-      <c r="D44" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="n">
-        <v>-9.4</v>
-      </c>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="n">
-        <v>-18</v>
-      </c>
-      <c r="I44" s="2" t="n">
-        <v>8.25</v>
-      </c>
-      <c r="J44" t="n">
-        <v>-63</v>
-      </c>
-      <c r="K44" s="2" t="n">
-        <v>14</v>
+      <c r="D44" t="n">
+        <v>-30</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-26.75</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="G44" t="n">
+        <v>-54.67</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>10.45</v>
+      </c>
+      <c r="I44" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J44" s="2" t="n">
+        <v>40.6</v>
+      </c>
+      <c r="K44" t="n">
+        <v>-44.57</v>
       </c>
       <c r="L44" t="n">
         <v>-100</v>
       </c>
-      <c r="M44" s="2" t="n">
-        <v>18.12</v>
-      </c>
-      <c r="N44" t="inlineStr"/>
-      <c r="O44" s="2" t="n">
-        <v>13.2</v>
-      </c>
-      <c r="P44" t="n">
-        <v>-42.33</v>
-      </c>
-      <c r="Q44" s="2" t="n">
-        <v>68</v>
+      <c r="M44" t="n">
+        <v>-18.3</v>
+      </c>
+      <c r="N44" t="n">
+        <v>-100</v>
+      </c>
+      <c r="O44" t="n">
+        <v>-20.4</v>
+      </c>
+      <c r="P44" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>-48.12</v>
       </c>
       <c r="R44" t="n">
-        <v>-20.8</v>
-      </c>
-      <c r="S44" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="T44" t="n">
-        <v>-100</v>
+        <v>0</v>
+      </c>
+      <c r="S44" t="n">
+        <v>-70</v>
+      </c>
+      <c r="T44" s="2" t="n">
+        <v>138</v>
       </c>
       <c r="U44" t="n">
-        <v>-2.4</v>
-      </c>
-      <c r="V44" t="n">
-        <v>-21.5</v>
-      </c>
-      <c r="W44" t="n">
-        <v>-100</v>
+        <v>-26.5</v>
+      </c>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" s="2" t="n">
+        <v>1.5</v>
       </c>
       <c r="X44" s="2" t="n">
-        <v>5.33</v>
-      </c>
-      <c r="Y44" s="2" t="n">
-        <v>175</v>
-      </c>
-      <c r="Z44" t="n">
-        <v>-100</v>
+        <v>16</v>
+      </c>
+      <c r="Y44" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Z44" s="2" t="n">
+        <v>22</v>
       </c>
       <c r="AA44" t="n">
-        <v>-17.14</v>
+        <v>-48</v>
       </c>
       <c r="AB44" s="2" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>england5</t>
+          <t>england4</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-30.4</v>
-      </c>
-      <c r="C45" t="n">
-        <v>-100</v>
-      </c>
-      <c r="D45" t="n">
-        <v>-11.6</v>
-      </c>
-      <c r="E45" t="n">
-        <v>-25.2</v>
-      </c>
+        <v>-29.6</v>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E45" t="inlineStr"/>
       <c r="F45" t="n">
-        <v>-35.5</v>
-      </c>
-      <c r="G45" t="n">
-        <v>-38.25</v>
-      </c>
+        <v>-9.4</v>
+      </c>
+      <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
-        <v>-1.7</v>
+        <v>-18</v>
       </c>
       <c r="I45" s="2" t="n">
-        <v>225</v>
+        <v>8.25</v>
       </c>
       <c r="J45" t="n">
-        <v>-40.83</v>
-      </c>
-      <c r="K45" t="n">
-        <v>-65.40000000000001</v>
-      </c>
-      <c r="L45" s="2" t="n">
+        <v>-63</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="L45" t="n">
+        <v>-100</v>
+      </c>
+      <c r="M45" s="2" t="n">
+        <v>18.12</v>
+      </c>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" s="2" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="P45" t="n">
+        <v>-42.33</v>
+      </c>
+      <c r="Q45" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="R45" t="n">
+        <v>-20.8</v>
+      </c>
+      <c r="S45" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="T45" t="n">
+        <v>-100</v>
+      </c>
+      <c r="U45" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="V45" t="n">
+        <v>-21.5</v>
+      </c>
+      <c r="W45" t="n">
+        <v>-100</v>
+      </c>
+      <c r="X45" s="2" t="n">
+        <v>5.33</v>
+      </c>
+      <c r="Y45" s="2" t="n">
         <v>175</v>
       </c>
-      <c r="M45" t="n">
-        <v>-3.6</v>
-      </c>
-      <c r="N45" t="inlineStr"/>
-      <c r="O45" t="n">
-        <v>-17</v>
-      </c>
-      <c r="P45" t="n">
-        <v>-32.6</v>
-      </c>
-      <c r="Q45" t="n">
-        <v>-31.5</v>
-      </c>
-      <c r="R45" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="S45" s="2" t="n">
-        <v>116.67</v>
-      </c>
-      <c r="T45" s="2" t="n">
-        <v>13.33</v>
-      </c>
-      <c r="U45" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="V45" t="n">
-        <v>-19</v>
-      </c>
-      <c r="W45" t="n">
-        <v>-12.67</v>
-      </c>
-      <c r="X45" t="n">
-        <v>-38.36</v>
-      </c>
-      <c r="Y45" t="inlineStr"/>
       <c r="Z45" t="n">
         <v>-100</v>
       </c>
-      <c r="AA45" s="2" t="n">
-        <v>14.8</v>
+      <c r="AA45" t="n">
+        <v>-17.14</v>
       </c>
       <c r="AB45" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>italy2</t>
+          <t>england5</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>-24.4</v>
+        <v>-30.4</v>
       </c>
       <c r="C46" t="n">
         <v>-100</v>
       </c>
-      <c r="D46" s="2" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="E46" s="2" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="F46" t="inlineStr"/>
+      <c r="D46" t="n">
+        <v>-11.6</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-25.2</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-35.5</v>
+      </c>
       <c r="G46" t="n">
-        <v>-41.2</v>
+        <v>-38.25</v>
       </c>
       <c r="H46" t="n">
-        <v>-31.37</v>
+        <v>-1.7</v>
       </c>
       <c r="I46" s="2" t="n">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="J46" t="n">
-        <v>-57</v>
+        <v>-40.83</v>
       </c>
       <c r="K46" t="n">
-        <v>-66.59999999999999</v>
-      </c>
-      <c r="L46" t="inlineStr"/>
-      <c r="M46" s="2" t="n">
-        <v>12.9</v>
+        <v>-65.40000000000001</v>
+      </c>
+      <c r="L46" s="2" t="n">
+        <v>175</v>
+      </c>
+      <c r="M46" t="n">
+        <v>-3.6</v>
       </c>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="n">
-        <v>-2.5</v>
+        <v>-17</v>
       </c>
       <c r="P46" t="n">
-        <v>-61</v>
-      </c>
-      <c r="Q46" s="2" t="n">
-        <v>11.6</v>
-      </c>
-      <c r="R46" t="n">
-        <v>-100</v>
+        <v>-32.6</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>-31.5</v>
+      </c>
+      <c r="R46" s="2" t="n">
+        <v>25</v>
       </c>
       <c r="S46" s="2" t="n">
-        <v>56.25</v>
-      </c>
-      <c r="T46" t="n">
-        <v>-100</v>
-      </c>
-      <c r="U46" t="n">
-        <v>-7.75</v>
-      </c>
-      <c r="V46" s="2" t="n">
-        <v>15.33</v>
+        <v>116.67</v>
+      </c>
+      <c r="T46" s="2" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="U46" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="V46" t="n">
+        <v>-19</v>
       </c>
       <c r="W46" t="n">
-        <v>-10.33</v>
+        <v>-12.67</v>
       </c>
       <c r="X46" t="n">
-        <v>-8.630000000000001</v>
-      </c>
-      <c r="Y46" s="2" t="n">
-        <v>31.5</v>
-      </c>
+        <v>-38.36</v>
+      </c>
+      <c r="Y46" t="inlineStr"/>
       <c r="Z46" t="n">
         <v>-100</v>
       </c>
-      <c r="AA46" t="n">
-        <v>-10.67</v>
+      <c r="AA46" s="2" t="n">
+        <v>14.8</v>
       </c>
       <c r="AB46" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>turkey</t>
+          <t>italy2</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>-12.67</v>
-      </c>
-      <c r="C47" s="2" t="n">
-        <v>80</v>
+        <v>-24.4</v>
+      </c>
+      <c r="C47" t="n">
+        <v>-100</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>61</v>
-      </c>
-      <c r="E47" t="n">
-        <v>-23.5</v>
-      </c>
-      <c r="F47" t="n">
-        <v>-100</v>
-      </c>
-      <c r="G47" s="2" t="n">
-        <v>57</v>
+        <v>37.5</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="n">
+        <v>-41.2</v>
       </c>
       <c r="H47" t="n">
-        <v>-32.33</v>
-      </c>
-      <c r="I47" t="n">
-        <v>-100</v>
-      </c>
-      <c r="J47" s="2" t="n">
-        <v>15.25</v>
-      </c>
-      <c r="K47" s="2" t="n">
-        <v>43.83</v>
-      </c>
-      <c r="L47" t="n">
-        <v>-4.5</v>
-      </c>
-      <c r="M47" t="n">
-        <v>-0.63</v>
-      </c>
-      <c r="N47" t="n">
-        <v>-100</v>
-      </c>
-      <c r="O47" s="2" t="n">
-        <v>13.67</v>
-      </c>
-      <c r="P47" s="2" t="n">
-        <v>1.4</v>
+        <v>-31.37</v>
+      </c>
+      <c r="I47" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="J47" t="n">
+        <v>-57</v>
+      </c>
+      <c r="K47" t="n">
+        <v>-66.59999999999999</v>
+      </c>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" s="2" t="n">
+        <v>12.9</v>
+      </c>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="P47" t="n">
+        <v>-61</v>
       </c>
       <c r="Q47" s="2" t="n">
-        <v>41.2</v>
+        <v>11.6</v>
       </c>
       <c r="R47" t="n">
         <v>-100</v>
       </c>
       <c r="S47" s="2" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="T47" s="2" t="n">
-        <v>175</v>
+        <v>56.25</v>
+      </c>
+      <c r="T47" t="n">
+        <v>-100</v>
       </c>
       <c r="U47" t="n">
-        <v>-24.5</v>
-      </c>
-      <c r="V47" t="inlineStr"/>
-      <c r="W47" s="2" t="n">
-        <v>37</v>
-      </c>
-      <c r="X47" s="2" t="n">
-        <v>33</v>
+        <v>-7.75</v>
+      </c>
+      <c r="V47" s="2" t="n">
+        <v>15.33</v>
+      </c>
+      <c r="W47" t="n">
+        <v>-10.33</v>
+      </c>
+      <c r="X47" t="n">
+        <v>-8.630000000000001</v>
       </c>
       <c r="Y47" s="2" t="n">
-        <v>40.75</v>
+        <v>31.5</v>
       </c>
       <c r="Z47" t="n">
-        <v>-48.75</v>
+        <v>-100</v>
       </c>
       <c r="AA47" t="n">
-        <v>-2.67</v>
+        <v>-10.67</v>
       </c>
       <c r="AB47" s="2" t="n">
         <v>10</v>
@@ -4445,78 +4445,244 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>usa</t>
-        </is>
-      </c>
-      <c r="B48" s="2" t="n">
-        <v>4.88</v>
+          <t>mexico</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>-13.11</v>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="n">
-        <v>-20</v>
-      </c>
-      <c r="E48" s="2" t="n">
-        <v>19.2</v>
+        <v>-100</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-18.71</v>
       </c>
       <c r="F48" t="n">
-        <v>-25.3</v>
-      </c>
-      <c r="G48" s="2" t="n">
-        <v>37.33</v>
-      </c>
-      <c r="H48" s="2" t="n">
-        <v>5.61</v>
+        <v>-17.67</v>
+      </c>
+      <c r="G48" t="n">
+        <v>-100</v>
+      </c>
+      <c r="H48" t="n">
+        <v>-59.92</v>
       </c>
       <c r="I48" t="inlineStr"/>
-      <c r="J48" s="2" t="n">
-        <v>1.44</v>
+      <c r="J48" t="n">
+        <v>-53.86</v>
       </c>
       <c r="K48" s="2" t="n">
-        <v>20</v>
+        <v>61.2</v>
       </c>
       <c r="L48" s="2" t="n">
-        <v>45.75</v>
-      </c>
-      <c r="M48" t="n">
-        <v>-29.74</v>
+        <v>125</v>
+      </c>
+      <c r="M48" s="2" t="n">
+        <v>14.64</v>
       </c>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="n">
-        <v>-11.04</v>
-      </c>
-      <c r="P48" s="2" t="n">
-        <v>10.75</v>
+        <v>-4.33</v>
+      </c>
+      <c r="P48" t="n">
+        <v>-44.33</v>
       </c>
       <c r="Q48" s="2" t="n">
-        <v>22.14</v>
+        <v>50.11</v>
       </c>
       <c r="R48" s="2" t="n">
-        <v>47.15</v>
+        <v>37</v>
       </c>
       <c r="S48" s="2" t="n">
-        <v>3.89</v>
+        <v>31.14</v>
       </c>
       <c r="T48" t="n">
         <v>-100</v>
       </c>
-      <c r="U48" s="2" t="n">
-        <v>3.47</v>
+      <c r="U48" t="n">
+        <v>-9.5</v>
       </c>
       <c r="V48" t="inlineStr"/>
       <c r="W48" s="2" t="n">
+        <v>15.75</v>
+      </c>
+      <c r="X48" t="n">
+        <v>-33.2</v>
+      </c>
+      <c r="Y48" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>-50</v>
+      </c>
+      <c r="AA48" s="2" t="n">
+        <v>21.29</v>
+      </c>
+      <c r="AB48" s="2" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>turkey</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>-12.67</v>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-23.5</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-100</v>
+      </c>
+      <c r="G49" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="H49" t="n">
+        <v>-32.33</v>
+      </c>
+      <c r="I49" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <v>15.25</v>
+      </c>
+      <c r="K49" s="2" t="n">
+        <v>43.83</v>
+      </c>
+      <c r="L49" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="M49" t="n">
+        <v>-0.63</v>
+      </c>
+      <c r="N49" t="n">
+        <v>-100</v>
+      </c>
+      <c r="O49" s="2" t="n">
+        <v>13.67</v>
+      </c>
+      <c r="P49" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="Q49" s="2" t="n">
+        <v>41.2</v>
+      </c>
+      <c r="R49" t="n">
+        <v>-100</v>
+      </c>
+      <c r="S49" s="2" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="T49" s="2" t="n">
+        <v>175</v>
+      </c>
+      <c r="U49" t="n">
+        <v>-24.5</v>
+      </c>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="X49" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y49" s="2" t="n">
+        <v>40.75</v>
+      </c>
+      <c r="Z49" t="n">
+        <v>-48.75</v>
+      </c>
+      <c r="AA49" t="n">
+        <v>-2.67</v>
+      </c>
+      <c r="AB49" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>usa</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="n">
+        <v>-20</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-25.3</v>
+      </c>
+      <c r="G50" s="2" t="n">
+        <v>37.33</v>
+      </c>
+      <c r="H50" s="2" t="n">
+        <v>5.61</v>
+      </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" s="2" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="K50" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="L50" s="2" t="n">
+        <v>45.75</v>
+      </c>
+      <c r="M50" t="n">
+        <v>-29.74</v>
+      </c>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="n">
+        <v>-11.04</v>
+      </c>
+      <c r="P50" s="2" t="n">
+        <v>10.75</v>
+      </c>
+      <c r="Q50" s="2" t="n">
+        <v>22.14</v>
+      </c>
+      <c r="R50" s="2" t="n">
+        <v>47.15</v>
+      </c>
+      <c r="S50" s="2" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="T50" t="n">
+        <v>-100</v>
+      </c>
+      <c r="U50" s="2" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="V50" t="inlineStr"/>
+      <c r="W50" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="X48" t="n">
+      <c r="X50" t="n">
         <v>-0.35</v>
       </c>
-      <c r="Y48" t="inlineStr"/>
-      <c r="Z48" s="2" t="n">
+      <c r="Y50" t="inlineStr"/>
+      <c r="Z50" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="AA48" s="2" t="n">
+      <c r="AA50" s="2" t="n">
         <v>12.78</v>
       </c>
-      <c r="AB48" s="2" t="n">
+      <c r="AB50" s="2" t="n">
         <v>23</v>
       </c>
     </row>

</xml_diff>